<commit_message>
updating metabolism rate laws
</commit_message>
<xml_diff>
--- a/data/Model.xlsx
+++ b/data/Model.xlsx
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2340" uniqueCount="1286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2365" uniqueCount="1305">
   <si>
     <t>ID</t>
   </si>
@@ -3909,6 +3909,63 @@
   </si>
   <si>
     <t>10.1038/msb4100155</t>
+  </si>
+  <si>
+    <t>Vmax * Adk-Protein[c]</t>
+  </si>
+  <si>
+    <t>Vmax * Cmk-Protein[c]</t>
+  </si>
+  <si>
+    <t>Vmax * Eno-Protein[c]</t>
+  </si>
+  <si>
+    <t>Vmax * Fba-Protein[c]</t>
+  </si>
+  <si>
+    <t>Vmax * Gap-Protein[c]</t>
+  </si>
+  <si>
+    <t>Vmax * Pgm-Protein[c]</t>
+  </si>
+  <si>
+    <t>Vmax * Gk-Protein[c]</t>
+  </si>
+  <si>
+    <t>Vmax * Hpt-Protein[c]</t>
+  </si>
+  <si>
+    <t>Vmax * Ldh-Protein[c]</t>
+  </si>
+  <si>
+    <t>Vmax * Nox-Protein[c]</t>
+  </si>
+  <si>
+    <t>Vmax * Pfk-Protein[c]</t>
+  </si>
+  <si>
+    <t>Vmax * PgiB-Protein[c]</t>
+  </si>
+  <si>
+    <t>Vmax * Pgk-Protein[c]</t>
+  </si>
+  <si>
+    <t>Vmax * Ppa-Protein[c]</t>
+  </si>
+  <si>
+    <t>Vmax * Pyk-Protein[c]</t>
+  </si>
+  <si>
+    <t>Vmax * Rpe-Protein[c]</t>
+  </si>
+  <si>
+    <t>Vmax * LacA-Protein[c]</t>
+  </si>
+  <si>
+    <t>Vmax * Udk-Protein[c]</t>
+  </si>
+  <si>
+    <t>Vmax * PyrH-Protein[c]</t>
   </si>
 </sst>
 </file>
@@ -4374,7 +4431,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" sqref="A1:XFD1"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4455,7 +4512,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4524,10 +4581,10 @@
   <dimension ref="A1:O167"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B163" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B172" sqref="A1:XFD1048576"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9668,10 +9725,10 @@
   <dimension ref="A1:J177"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A170" sqref="A170"/>
-      <selection pane="bottomRight" activeCell="D22" sqref="A1:XFD1048576"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9735,9 +9792,8 @@
       <c r="E2" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="F2" s="4" t="str">
-        <f>CONCATENATE("Vmax * ",E2,"[c]")</f>
-        <v>Vmax * Adk-Protein[c]</v>
+      <c r="F2" s="4" t="s">
+        <v>1286</v>
       </c>
       <c r="G2" s="5">
         <v>1247</v>
@@ -9811,9 +9867,8 @@
       <c r="E5" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="F5" s="4" t="str">
-        <f>CONCATENATE("Vmax * ",E5,"[c]")</f>
-        <v>Vmax * Cmk-Protein[c]</v>
+      <c r="F5" s="4" t="s">
+        <v>1287</v>
       </c>
       <c r="G5" s="5">
         <v>250</v>
@@ -10241,9 +10296,8 @@
       <c r="E26" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F26" s="4" t="str">
-        <f t="shared" ref="F26:F40" si="0">CONCATENATE("Vmax * ",E26,"[c]")</f>
-        <v>Vmax * Eno-Protein[c]</v>
+      <c r="F26" s="4" t="s">
+        <v>1288</v>
       </c>
       <c r="G26" s="5">
         <v>180</v>
@@ -10271,9 +10325,8 @@
       <c r="E27" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="F27" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>Vmax * Fba-Protein[c]</v>
+      <c r="F27" s="4" t="s">
+        <v>1289</v>
       </c>
       <c r="G27" s="5">
         <v>1005.6</v>
@@ -10301,9 +10354,8 @@
       <c r="E28" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="F28" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>Vmax * Gap-Protein[c]</v>
+      <c r="F28" s="4" t="s">
+        <v>1290</v>
       </c>
       <c r="G28" s="5">
         <v>4200</v>
@@ -10331,9 +10383,8 @@
       <c r="E29" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="F29" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>Vmax * Pgm-Protein[c]</v>
+      <c r="F29" s="4" t="s">
+        <v>1291</v>
       </c>
       <c r="G29" s="5">
         <v>13200</v>
@@ -10361,9 +10412,8 @@
       <c r="E30" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="F30" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>Vmax * Gk-Protein[c]</v>
+      <c r="F30" s="4" t="s">
+        <v>1292</v>
       </c>
       <c r="G30" s="5">
         <v>0.105</v>
@@ -10391,9 +10441,8 @@
       <c r="E31" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="F31" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>Vmax * Hpt-Protein[c]</v>
+      <c r="F31" s="4" t="s">
+        <v>1293</v>
       </c>
       <c r="G31" s="5">
         <v>628.79999999999995</v>
@@ -10421,9 +10470,8 @@
       <c r="E32" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="F32" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>Vmax * Ldh-Protein[c]</v>
+      <c r="F32" s="4" t="s">
+        <v>1294</v>
       </c>
       <c r="G32" s="5">
         <v>220</v>
@@ -10451,9 +10499,8 @@
       <c r="E33" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="F33" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>Vmax * Nox-Protein[c]</v>
+      <c r="F33" s="4" t="s">
+        <v>1295</v>
       </c>
       <c r="G33" s="5">
         <v>21667.02</v>
@@ -10481,9 +10528,8 @@
       <c r="E34" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="F34" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>Vmax * Pfk-Protein[c]</v>
+      <c r="F34" s="4" t="s">
+        <v>1296</v>
       </c>
       <c r="G34" s="5">
         <v>10020</v>
@@ -10511,9 +10557,8 @@
       <c r="E35" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="F35" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>Vmax * Pfk-Protein[c]</v>
+      <c r="F35" s="4" t="s">
+        <v>1296</v>
       </c>
       <c r="G35" s="5">
         <v>30.6</v>
@@ -10541,9 +10586,8 @@
       <c r="E36" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="F36" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>Vmax * Pfk-Protein[c]</v>
+      <c r="F36" s="4" t="s">
+        <v>1296</v>
       </c>
       <c r="G36" s="5">
         <v>12</v>
@@ -10571,9 +10615,8 @@
       <c r="E37" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="F37" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>Vmax * PgiB-Protein[c]</v>
+      <c r="F37" s="4" t="s">
+        <v>1297</v>
       </c>
       <c r="G37" s="5">
         <v>1511</v>
@@ -10601,9 +10644,8 @@
       <c r="E38" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="F38" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>Vmax * Pgk-Protein[c]</v>
+      <c r="F38" s="4" t="s">
+        <v>1298</v>
       </c>
       <c r="G38" s="5">
         <v>88800</v>
@@ -10631,9 +10673,8 @@
       <c r="E39" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="F39" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>Vmax * Pgk-Protein[c]</v>
+      <c r="F39" s="4" t="s">
+        <v>1298</v>
       </c>
       <c r="G39" s="5">
         <v>340</v>
@@ -10661,9 +10702,8 @@
       <c r="E40" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="F40" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>Vmax * Ppa-Protein[c]</v>
+      <c r="F40" s="4" t="s">
+        <v>1299</v>
       </c>
       <c r="G40" s="5">
         <v>213000</v>
@@ -10714,9 +10754,8 @@
       <c r="E42" s="4" t="s">
         <v>297</v>
       </c>
-      <c r="F42" s="4" t="str">
-        <f>CONCATENATE("Vmax * ",E42,"[c]")</f>
-        <v>Vmax * Pyk-Protein[c]</v>
+      <c r="F42" s="4" t="s">
+        <v>1300</v>
       </c>
       <c r="G42" s="5">
         <v>9600</v>
@@ -10744,9 +10783,8 @@
       <c r="E43" s="4" t="s">
         <v>297</v>
       </c>
-      <c r="F43" s="4" t="str">
-        <f>CONCATENATE("Vmax * ",E43,"[c]")</f>
-        <v>Vmax * Pyk-Protein[c]</v>
+      <c r="F43" s="4" t="s">
+        <v>1300</v>
       </c>
       <c r="G43" s="5">
         <v>47</v>
@@ -10774,9 +10812,8 @@
       <c r="E44" s="4" t="s">
         <v>297</v>
       </c>
-      <c r="F44" s="4" t="str">
-        <f>CONCATENATE("Vmax * ",E44,"[c]")</f>
-        <v>Vmax * Pyk-Protein[c]</v>
+      <c r="F44" s="4" t="s">
+        <v>1300</v>
       </c>
       <c r="G44" s="5">
         <v>200</v>
@@ -10827,9 +10864,8 @@
       <c r="E46" s="4" t="s">
         <v>301</v>
       </c>
-      <c r="F46" s="4" t="str">
-        <f>CONCATENATE("Vmax * ",E46,"[c]")</f>
-        <v>Vmax * Rpe-Protein[c]</v>
+      <c r="F46" s="4" t="s">
+        <v>1301</v>
       </c>
       <c r="G46" s="5">
         <v>120</v>
@@ -10857,9 +10893,8 @@
       <c r="E47" s="4" t="s">
         <v>305</v>
       </c>
-      <c r="F47" s="4" t="str">
-        <f>CONCATENATE("Vmax * ",E47,"[c]")</f>
-        <v>Vmax * LacA-Protein[c]</v>
+      <c r="F47" s="4" t="s">
+        <v>1302</v>
       </c>
       <c r="G47" s="5">
         <v>4140</v>
@@ -10976,9 +11011,8 @@
       <c r="E52" s="4" t="s">
         <v>317</v>
       </c>
-      <c r="F52" s="4" t="str">
-        <f>CONCATENATE("Vmax * ",E52,"[c]")</f>
-        <v>Vmax * Udk-Protein[c]</v>
+      <c r="F52" s="4" t="s">
+        <v>1303</v>
       </c>
       <c r="G52" s="5">
         <v>6.5</v>
@@ -11006,9 +11040,8 @@
       <c r="E53" s="4" t="s">
         <v>317</v>
       </c>
-      <c r="F53" s="4" t="str">
-        <f>CONCATENATE("Vmax * ",E53,"[c]")</f>
-        <v>Vmax * Udk-Protein[c]</v>
+      <c r="F53" s="4" t="s">
+        <v>1303</v>
       </c>
       <c r="G53" s="5">
         <v>1.58</v>
@@ -11036,9 +11069,8 @@
       <c r="E54" s="4" t="s">
         <v>321</v>
       </c>
-      <c r="F54" s="4" t="str">
-        <f>CONCATENATE("Vmax * ",E54,"[c]")</f>
-        <v>Vmax * PyrH-Protein[c]</v>
+      <c r="F54" s="4" t="s">
+        <v>1304</v>
       </c>
       <c r="G54" s="5">
         <v>52</v>
@@ -14614,7 +14646,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" sqref="A1:XFD1"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -14733,7 +14765,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
adding dry weight fraction parameter
</commit_message>
<xml_diff>
--- a/data/Model.xlsx
+++ b/data/Model.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="989"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="989" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Submodels" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2365" uniqueCount="1305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2372" uniqueCount="1312">
   <si>
     <t>ID</t>
   </si>
@@ -3611,24 +3611,15 @@
     <t>Units</t>
   </si>
   <si>
-    <t>CellCycleLength</t>
-  </si>
-  <si>
     <t>Cell cycle length</t>
   </si>
   <si>
     <t>s</t>
   </si>
   <si>
-    <t>RnaHalfLife</t>
-  </si>
-  <si>
     <t>RNA half life</t>
   </si>
   <si>
-    <t>CarbonExchangeRate</t>
-  </si>
-  <si>
     <t>Carbon-containing metabolite exchange rate</t>
   </si>
   <si>
@@ -3638,9 +3629,6 @@
     <t>Exchange rate upper bound for carbon-containing metabolites (mmol/gDCW/h). Maranas et al. used 5 mmol/gDCW/h for all carbon-containing metabolites [Ref-0004]. Feist et al. used 11.2 mmol/gDCW/h for glucose [Ref-0005].</t>
   </si>
   <si>
-    <t>NonCarbonExchangeRate</t>
-  </si>
-  <si>
     <t>Non-carbon-containing metabolite exchange rate</t>
   </si>
   <si>
@@ -3966,6 +3954,39 @@
   </si>
   <si>
     <t>Vmax * PyrH-Protein[c]</t>
+  </si>
+  <si>
+    <t>cellCycleLength</t>
+  </si>
+  <si>
+    <t>rnaHalfLife</t>
+  </si>
+  <si>
+    <t>carbonExchangeRate</t>
+  </si>
+  <si>
+    <t>nonCarbonExchangeRate</t>
+  </si>
+  <si>
+    <t>fractionDryWeight</t>
+  </si>
+  <si>
+    <t>Fraction of cell mass which is non water</t>
+  </si>
+  <si>
+    <t>dimensionless</t>
+  </si>
+  <si>
+    <t>[Ref-0006]</t>
+  </si>
+  <si>
+    <t>Ref-0006</t>
+  </si>
+  <si>
+    <t>Bray, Dennis. Cell movements: from molecules to motility. Garland Science, 2001.</t>
+  </si>
+  <si>
+    <t>ISBN</t>
   </si>
 </sst>
 </file>
@@ -4427,7 +4448,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -4655,7 +4676,7 @@
         <v>31</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>1211</v>
+        <v>1207</v>
       </c>
       <c r="E2" s="4">
         <v>503.149</v>
@@ -4693,7 +4714,7 @@
         <v>36</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>1212</v>
+        <v>1208</v>
       </c>
       <c r="E3" s="4">
         <v>479.12400000000002</v>
@@ -4731,7 +4752,7 @@
         <v>38</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>1213</v>
+        <v>1209</v>
       </c>
       <c r="E4" s="4">
         <v>519.14800000000002</v>
@@ -4769,7 +4790,7 @@
         <v>40</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>1214</v>
+        <v>1210</v>
       </c>
       <c r="E5" s="4">
         <v>480.10899999999998</v>
@@ -4807,7 +4828,7 @@
         <v>42</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>1215</v>
+        <v>1211</v>
       </c>
       <c r="E6" s="4">
         <v>440.17599999999999</v>
@@ -4845,7 +4866,7 @@
         <v>45</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>1216</v>
+        <v>1212</v>
       </c>
       <c r="E7" s="4">
         <v>345.20499999999998</v>
@@ -4887,7 +4908,7 @@
         <v>48</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>1217</v>
+        <v>1213</v>
       </c>
       <c r="E8" s="4">
         <v>321.18</v>
@@ -4929,7 +4950,7 @@
         <v>50</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>1218</v>
+        <v>1214</v>
       </c>
       <c r="E9" s="4">
         <v>361.20400000000001</v>
@@ -4971,7 +4992,7 @@
         <v>52</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>1219</v>
+        <v>1215</v>
       </c>
       <c r="E10" s="4">
         <v>322.16500000000002</v>
@@ -5048,7 +5069,7 @@
         <v>57</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>1220</v>
+        <v>1216</v>
       </c>
       <c r="E12" s="4">
         <v>174.95099999999999</v>
@@ -5083,7 +5104,7 @@
         <v>59</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>1221</v>
+        <v>1217</v>
       </c>
       <c r="E13" s="4">
         <v>95.979299999999995</v>
@@ -5153,7 +5174,7 @@
         <v>64</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>1222</v>
+        <v>1218</v>
       </c>
       <c r="E15" s="4">
         <v>89.0929</v>
@@ -5195,7 +5216,7 @@
         <v>68</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>1223</v>
+        <v>1219</v>
       </c>
       <c r="E16" s="4">
         <v>175.208</v>
@@ -5237,7 +5258,7 @@
         <v>71</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>1224</v>
+        <v>1220</v>
       </c>
       <c r="E17" s="4">
         <v>132.09399999999999</v>
@@ -5279,7 +5300,7 @@
         <v>74</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>1225</v>
+        <v>1221</v>
       </c>
       <c r="E18" s="4">
         <v>132.11799999999999</v>
@@ -5321,7 +5342,7 @@
         <v>77</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>1226</v>
+        <v>1222</v>
       </c>
       <c r="E19" s="4">
         <v>121.158</v>
@@ -5363,7 +5384,7 @@
         <v>80</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>1227</v>
+        <v>1223</v>
       </c>
       <c r="E20" s="4">
         <v>146.14400000000001</v>
@@ -5405,7 +5426,7 @@
         <v>83</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>1228</v>
+        <v>1224</v>
       </c>
       <c r="E21" s="4">
         <v>146.12100000000001</v>
@@ -5447,7 +5468,7 @@
         <v>86</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>1229</v>
+        <v>1225</v>
       </c>
       <c r="E22" s="4">
         <v>75.066400000000002</v>
@@ -5489,7 +5510,7 @@
         <v>89</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>1230</v>
+        <v>1226</v>
       </c>
       <c r="E23" s="4">
         <v>155.154</v>
@@ -5531,7 +5552,7 @@
         <v>92</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>1231</v>
+        <v>1227</v>
       </c>
       <c r="E24" s="4">
         <v>131.172</v>
@@ -5573,7 +5594,7 @@
         <v>95</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>1231</v>
+        <v>1227</v>
       </c>
       <c r="E25" s="4">
         <v>131.172</v>
@@ -5615,7 +5636,7 @@
         <v>98</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>1232</v>
+        <v>1228</v>
       </c>
       <c r="E26" s="4">
         <v>147.19499999999999</v>
@@ -5657,7 +5678,7 @@
         <v>101</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>1233</v>
+        <v>1229</v>
       </c>
       <c r="E27" s="4">
         <v>149.21100000000001</v>
@@ -5699,7 +5720,7 @@
         <v>104</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>1234</v>
+        <v>1230</v>
       </c>
       <c r="E28" s="4">
         <v>165.18899999999999</v>
@@ -5741,7 +5762,7 @@
         <v>107</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>1235</v>
+        <v>1231</v>
       </c>
       <c r="E29" s="4">
         <v>115.13</v>
@@ -5783,7 +5804,7 @@
         <v>110</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>1236</v>
+        <v>1232</v>
       </c>
       <c r="E30" s="4">
         <v>105.092</v>
@@ -5825,7 +5846,7 @@
         <v>113</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>1237</v>
+        <v>1233</v>
       </c>
       <c r="E31" s="4">
         <v>119.119</v>
@@ -5867,7 +5888,7 @@
         <v>116</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>1238</v>
+        <v>1234</v>
       </c>
       <c r="E32" s="4">
         <v>204.22499999999999</v>
@@ -5909,7 +5930,7 @@
         <v>119</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>1239</v>
+        <v>1235</v>
       </c>
       <c r="E33" s="4">
         <v>181.18799999999999</v>
@@ -5951,7 +5972,7 @@
         <v>122</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>1240</v>
+        <v>1236</v>
       </c>
       <c r="E34" s="4">
         <v>117.146</v>
@@ -8063,7 +8084,7 @@
         <v>343</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>1241</v>
+        <v>1237</v>
       </c>
       <c r="E95" s="4">
         <v>135.126</v>
@@ -8086,7 +8107,7 @@
         <v>345</v>
       </c>
       <c r="D96" s="4" t="s">
-        <v>1242</v>
+        <v>1238</v>
       </c>
       <c r="E96" s="4">
         <v>424.17700000000002</v>
@@ -8109,7 +8130,7 @@
         <v>348</v>
       </c>
       <c r="D97" s="4" t="s">
-        <v>1222</v>
+        <v>1218</v>
       </c>
       <c r="E97" s="4">
         <v>89.0929</v>
@@ -8132,7 +8153,7 @@
         <v>351</v>
       </c>
       <c r="D98" s="4" t="s">
-        <v>1223</v>
+        <v>1219</v>
       </c>
       <c r="E98" s="4">
         <v>175.208</v>
@@ -8155,7 +8176,7 @@
         <v>354</v>
       </c>
       <c r="D99" s="4" t="s">
-        <v>1225</v>
+        <v>1221</v>
       </c>
       <c r="E99" s="4">
         <v>132.11799999999999</v>
@@ -8178,7 +8199,7 @@
         <v>357</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>1224</v>
+        <v>1220</v>
       </c>
       <c r="E100" s="4">
         <v>132.09399999999999</v>
@@ -8201,7 +8222,7 @@
         <v>360</v>
       </c>
       <c r="D101" s="4" t="s">
-        <v>1243</v>
+        <v>1239</v>
       </c>
       <c r="E101" s="4">
         <v>160.17099999999999</v>
@@ -8224,7 +8245,7 @@
         <v>363</v>
       </c>
       <c r="D102" s="4" t="s">
-        <v>1244</v>
+        <v>1240</v>
       </c>
       <c r="E102" s="4">
         <v>332.40100000000001</v>
@@ -8247,7 +8268,7 @@
         <v>366</v>
       </c>
       <c r="D103" s="4" t="s">
-        <v>1245</v>
+        <v>1241</v>
       </c>
       <c r="E103" s="4">
         <v>246.22</v>
@@ -8270,7 +8291,7 @@
         <v>369</v>
       </c>
       <c r="D104" s="4" t="s">
-        <v>1246</v>
+        <v>1242</v>
       </c>
       <c r="E104" s="4">
         <v>246.17400000000001</v>
@@ -8293,7 +8314,7 @@
         <v>371</v>
       </c>
       <c r="D105" s="4" t="s">
-        <v>1247</v>
+        <v>1243</v>
       </c>
       <c r="E105" s="4">
         <v>400.15199999999999</v>
@@ -8339,7 +8360,7 @@
         <v>377</v>
       </c>
       <c r="D107" s="4" t="s">
-        <v>1226</v>
+        <v>1222</v>
       </c>
       <c r="E107" s="4">
         <v>121.158</v>
@@ -8362,7 +8383,7 @@
         <v>380</v>
       </c>
       <c r="D108" s="4" t="s">
-        <v>1248</v>
+        <v>1244</v>
       </c>
       <c r="E108" s="4">
         <v>243.21600000000001</v>
@@ -8385,7 +8406,7 @@
         <v>383</v>
       </c>
       <c r="D109" s="4" t="s">
-        <v>1249</v>
+        <v>1245</v>
       </c>
       <c r="E109" s="4">
         <v>224.30099999999999</v>
@@ -8408,7 +8429,7 @@
         <v>386</v>
       </c>
       <c r="D110" s="4" t="s">
-        <v>1250</v>
+        <v>1246</v>
       </c>
       <c r="E110" s="4">
         <v>262.005</v>
@@ -8431,7 +8452,7 @@
         <v>389</v>
       </c>
       <c r="D111" s="4" t="s">
-        <v>1251</v>
+        <v>1247</v>
       </c>
       <c r="E111" s="4">
         <v>198.06800000000001</v>
@@ -8454,7 +8475,7 @@
         <v>392</v>
       </c>
       <c r="D112" s="4" t="s">
-        <v>1252</v>
+        <v>1248</v>
       </c>
       <c r="E112" s="4">
         <v>258.12</v>
@@ -8477,7 +8498,7 @@
         <v>395</v>
       </c>
       <c r="D113" s="4" t="s">
-        <v>1253</v>
+        <v>1249</v>
       </c>
       <c r="E113" s="4">
         <v>336.084</v>
@@ -8500,7 +8521,7 @@
         <v>398</v>
       </c>
       <c r="D114" s="4" t="s">
-        <v>1254</v>
+        <v>1250</v>
       </c>
       <c r="E114" s="4">
         <v>183.03299999999999</v>
@@ -8523,7 +8544,7 @@
         <v>401</v>
       </c>
       <c r="D115" s="4" t="s">
-        <v>1254</v>
+        <v>1250</v>
       </c>
       <c r="E115" s="4">
         <v>183.03299999999999</v>
@@ -8546,7 +8567,7 @@
         <v>404</v>
       </c>
       <c r="D116" s="4" t="s">
-        <v>1252</v>
+        <v>1248</v>
       </c>
       <c r="E116" s="4">
         <v>258.12</v>
@@ -8569,7 +8590,7 @@
         <v>407</v>
       </c>
       <c r="D117" s="4" t="s">
-        <v>1255</v>
+        <v>1251</v>
       </c>
       <c r="E117" s="4">
         <v>180.155</v>
@@ -8592,7 +8613,7 @@
         <v>410</v>
       </c>
       <c r="D118" s="4" t="s">
-        <v>1227</v>
+        <v>1223</v>
       </c>
       <c r="E118" s="4">
         <v>146.14400000000001</v>
@@ -8615,7 +8636,7 @@
         <v>413</v>
       </c>
       <c r="D119" s="4" t="s">
-        <v>1228</v>
+        <v>1224</v>
       </c>
       <c r="E119" s="4">
         <v>146.12100000000001</v>
@@ -8638,7 +8659,7 @@
         <v>416</v>
       </c>
       <c r="D120" s="4" t="s">
-        <v>1229</v>
+        <v>1225</v>
       </c>
       <c r="E120" s="4">
         <v>75.066400000000002</v>
@@ -8661,7 +8682,7 @@
         <v>419</v>
       </c>
       <c r="D121" s="4" t="s">
-        <v>1256</v>
+        <v>1252</v>
       </c>
       <c r="E121" s="4">
         <v>151.126</v>
@@ -8684,7 +8705,7 @@
         <v>422</v>
       </c>
       <c r="D122" s="4" t="s">
-        <v>1257</v>
+        <v>1253</v>
       </c>
       <c r="E122" s="4">
         <v>274.27300000000002</v>
@@ -8707,7 +8728,7 @@
         <v>425</v>
       </c>
       <c r="D123" s="4" t="s">
-        <v>1258</v>
+        <v>1254</v>
       </c>
       <c r="E123" s="4">
         <v>274.22699999999998</v>
@@ -8730,7 +8751,7 @@
         <v>428</v>
       </c>
       <c r="D124" s="4" t="s">
-        <v>1225</v>
+        <v>1221</v>
       </c>
       <c r="E124" s="4">
         <v>132.11799999999999</v>
@@ -8753,7 +8774,7 @@
         <v>431</v>
       </c>
       <c r="D125" s="4" t="s">
-        <v>1230</v>
+        <v>1226</v>
       </c>
       <c r="E125" s="4">
         <v>155.154</v>
@@ -8776,7 +8797,7 @@
         <v>434</v>
       </c>
       <c r="D126" s="4" t="s">
-        <v>1259</v>
+        <v>1255</v>
       </c>
       <c r="E126" s="4">
         <v>292.29300000000001</v>
@@ -8799,7 +8820,7 @@
         <v>437</v>
       </c>
       <c r="D127" s="4" t="s">
-        <v>1231</v>
+        <v>1227</v>
       </c>
       <c r="E127" s="4">
         <v>131.172</v>
@@ -8822,7 +8843,7 @@
         <v>440</v>
       </c>
       <c r="D128" s="4" t="s">
-        <v>1260</v>
+        <v>1256</v>
       </c>
       <c r="E128" s="4">
         <v>244.33</v>
@@ -8845,7 +8866,7 @@
         <v>443</v>
       </c>
       <c r="D129" s="4" t="s">
-        <v>1261</v>
+        <v>1257</v>
       </c>
       <c r="E129" s="4">
         <v>89.069800000000001</v>
@@ -8868,7 +8889,7 @@
         <v>446</v>
       </c>
       <c r="D130" s="4" t="s">
-        <v>1231</v>
+        <v>1227</v>
       </c>
       <c r="E130" s="4">
         <v>131.172</v>
@@ -8891,7 +8912,7 @@
         <v>449</v>
       </c>
       <c r="D131" s="4" t="s">
-        <v>1232</v>
+        <v>1228</v>
       </c>
       <c r="E131" s="4">
         <v>147.19499999999999</v>
@@ -8914,7 +8935,7 @@
         <v>452</v>
       </c>
       <c r="D132" s="4" t="s">
-        <v>1260</v>
+        <v>1256</v>
       </c>
       <c r="E132" s="4">
         <v>244.33</v>
@@ -8937,7 +8958,7 @@
         <v>455</v>
       </c>
       <c r="D133" s="4" t="s">
-        <v>1262</v>
+        <v>1258</v>
       </c>
       <c r="E133" s="4">
         <v>276.375</v>
@@ -8960,7 +8981,7 @@
         <v>458</v>
       </c>
       <c r="D134" s="4" t="s">
-        <v>1233</v>
+        <v>1229</v>
       </c>
       <c r="E134" s="4">
         <v>149.21100000000001</v>
@@ -8983,7 +9004,7 @@
         <v>461</v>
       </c>
       <c r="D135" s="4" t="s">
-        <v>1263</v>
+        <v>1259</v>
       </c>
       <c r="E135" s="4">
         <v>280.40699999999998</v>
@@ -9006,7 +9027,7 @@
         <v>464</v>
       </c>
       <c r="D136" s="4" t="s">
-        <v>1264</v>
+        <v>1260</v>
       </c>
       <c r="E136" s="4">
         <v>662.41600000000005</v>
@@ -9029,7 +9050,7 @@
         <v>467</v>
       </c>
       <c r="D137" s="4" t="s">
-        <v>1265</v>
+        <v>1261</v>
       </c>
       <c r="E137" s="4">
         <v>663.42399999999998</v>
@@ -9075,7 +9096,7 @@
         <v>473</v>
       </c>
       <c r="D139" s="4" t="s">
-        <v>1266</v>
+        <v>1262</v>
       </c>
       <c r="E139" s="4">
         <v>165.018</v>
@@ -9098,7 +9119,7 @@
         <v>476</v>
       </c>
       <c r="D140" s="4" t="s">
-        <v>1234</v>
+        <v>1230</v>
       </c>
       <c r="E140" s="4">
         <v>165.18899999999999</v>
@@ -9121,7 +9142,7 @@
         <v>479</v>
       </c>
       <c r="D141" s="4" t="s">
-        <v>1221</v>
+        <v>1217</v>
       </c>
       <c r="E141" s="4">
         <v>95.979299999999995</v>
@@ -9144,7 +9165,7 @@
         <v>482</v>
       </c>
       <c r="D142" s="4" t="s">
-        <v>1220</v>
+        <v>1216</v>
       </c>
       <c r="E142" s="4">
         <v>174.95099999999999</v>
@@ -9167,7 +9188,7 @@
         <v>485</v>
       </c>
       <c r="D143" s="4" t="s">
-        <v>1235</v>
+        <v>1231</v>
       </c>
       <c r="E143" s="4">
         <v>115.13</v>
@@ -9190,7 +9211,7 @@
         <v>488</v>
       </c>
       <c r="D144" s="4" t="s">
-        <v>1267</v>
+        <v>1263</v>
       </c>
       <c r="E144" s="4">
         <v>385.03</v>
@@ -9213,7 +9234,7 @@
         <v>491</v>
       </c>
       <c r="D145" s="4" t="s">
-        <v>1268</v>
+        <v>1264</v>
       </c>
       <c r="E145" s="4">
         <v>87.054000000000002</v>
@@ -9236,7 +9257,7 @@
         <v>494</v>
       </c>
       <c r="D146" s="4" t="s">
-        <v>1269</v>
+        <v>1265</v>
       </c>
       <c r="E146" s="4">
         <v>312.36200000000002</v>
@@ -9259,7 +9280,7 @@
         <v>497</v>
       </c>
       <c r="D147" s="4" t="s">
-        <v>1270</v>
+        <v>1266</v>
       </c>
       <c r="E147" s="4">
         <v>212.245</v>
@@ -9282,7 +9303,7 @@
         <v>500</v>
       </c>
       <c r="D148" s="4" t="s">
-        <v>1271</v>
+        <v>1267</v>
       </c>
       <c r="E148" s="4">
         <v>228.09399999999999</v>
@@ -9305,7 +9326,7 @@
         <v>503</v>
       </c>
       <c r="D149" s="4" t="s">
-        <v>1271</v>
+        <v>1267</v>
       </c>
       <c r="E149" s="4">
         <v>228.09399999999999</v>
@@ -9328,7 +9349,7 @@
         <v>506</v>
       </c>
       <c r="D150" s="4" t="s">
-        <v>1272</v>
+        <v>1268</v>
       </c>
       <c r="E150" s="4">
         <v>288.14499999999998</v>
@@ -9351,7 +9372,7 @@
         <v>509</v>
       </c>
       <c r="D151" s="4" t="s">
-        <v>1236</v>
+        <v>1232</v>
       </c>
       <c r="E151" s="4">
         <v>105.092</v>
@@ -9374,7 +9395,7 @@
         <v>512</v>
       </c>
       <c r="D152" s="4" t="s">
-        <v>1273</v>
+        <v>1269</v>
       </c>
       <c r="E152" s="4">
         <v>192.16900000000001</v>
@@ -9397,7 +9418,7 @@
         <v>515</v>
       </c>
       <c r="D153" s="4" t="s">
-        <v>1274</v>
+        <v>1270</v>
       </c>
       <c r="E153" s="4">
         <v>168.042</v>
@@ -9420,7 +9441,7 @@
         <v>518</v>
       </c>
       <c r="D154" s="4" t="s">
-        <v>1274</v>
+        <v>1270</v>
       </c>
       <c r="E154" s="4">
         <v>168.042</v>
@@ -9443,7 +9464,7 @@
         <v>521</v>
       </c>
       <c r="D155" s="4" t="s">
-        <v>1237</v>
+        <v>1233</v>
       </c>
       <c r="E155" s="4">
         <v>119.119</v>
@@ -9466,7 +9487,7 @@
         <v>524</v>
       </c>
       <c r="D156" s="4" t="s">
-        <v>1238</v>
+        <v>1234</v>
       </c>
       <c r="E156" s="4">
         <v>204.22499999999999</v>
@@ -9489,7 +9510,7 @@
         <v>527</v>
       </c>
       <c r="D157" s="4" t="s">
-        <v>1239</v>
+        <v>1235</v>
       </c>
       <c r="E157" s="4">
         <v>181.18799999999999</v>
@@ -9512,7 +9533,7 @@
         <v>530</v>
       </c>
       <c r="D158" s="4" t="s">
-        <v>1275</v>
+        <v>1271</v>
       </c>
       <c r="E158" s="4">
         <v>220.22200000000001</v>
@@ -9535,7 +9556,7 @@
         <v>533</v>
       </c>
       <c r="D159" s="4" t="s">
-        <v>1276</v>
+        <v>1272</v>
       </c>
       <c r="E159" s="4">
         <v>390.43400000000003</v>
@@ -9558,7 +9579,7 @@
         <v>536</v>
       </c>
       <c r="D160" s="4" t="s">
-        <v>1277</v>
+        <v>1273</v>
       </c>
       <c r="E160" s="4">
         <v>344.36099999999999</v>
@@ -9581,7 +9602,7 @@
         <v>538</v>
       </c>
       <c r="D161" s="4" t="s">
-        <v>1278</v>
+        <v>1274</v>
       </c>
       <c r="E161" s="4">
         <v>401.137</v>
@@ -9604,7 +9625,7 @@
         <v>541</v>
       </c>
       <c r="D162" s="4" t="s">
-        <v>1279</v>
+        <v>1275</v>
       </c>
       <c r="E162" s="4">
         <v>112.087</v>
@@ -9627,7 +9648,7 @@
         <v>544</v>
       </c>
       <c r="D163" s="4" t="s">
-        <v>1280</v>
+        <v>1276</v>
       </c>
       <c r="E163" s="4">
         <v>244.20099999999999</v>
@@ -9650,7 +9671,7 @@
         <v>547</v>
       </c>
       <c r="D164" s="4" t="s">
-        <v>1240</v>
+        <v>1236</v>
       </c>
       <c r="E164" s="4">
         <v>117.146</v>
@@ -9673,7 +9694,7 @@
         <v>550</v>
       </c>
       <c r="D165" s="4" t="s">
-        <v>1281</v>
+        <v>1277</v>
       </c>
       <c r="E165" s="4">
         <v>216.27699999999999</v>
@@ -9696,7 +9717,7 @@
         <v>503</v>
       </c>
       <c r="D166" s="4" t="s">
-        <v>1271</v>
+        <v>1267</v>
       </c>
       <c r="E166" s="4">
         <v>228.09399999999999</v>
@@ -9728,7 +9749,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A170" sqref="A170"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9793,7 +9814,7 @@
         <v>233</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>1286</v>
+        <v>1282</v>
       </c>
       <c r="G2" s="5">
         <v>1247</v>
@@ -9868,7 +9889,7 @@
         <v>241</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>1287</v>
+        <v>1283</v>
       </c>
       <c r="G5" s="5">
         <v>250</v>
@@ -10297,7 +10318,7 @@
         <v>245</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>1288</v>
+        <v>1284</v>
       </c>
       <c r="G26" s="5">
         <v>180</v>
@@ -10326,7 +10347,7 @@
         <v>249</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>1289</v>
+        <v>1285</v>
       </c>
       <c r="G27" s="5">
         <v>1005.6</v>
@@ -10355,7 +10376,7 @@
         <v>253</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>1290</v>
+        <v>1286</v>
       </c>
       <c r="G28" s="5">
         <v>4200</v>
@@ -10384,7 +10405,7 @@
         <v>257</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>1291</v>
+        <v>1287</v>
       </c>
       <c r="G29" s="5">
         <v>13200</v>
@@ -10413,7 +10434,7 @@
         <v>261</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>1292</v>
+        <v>1288</v>
       </c>
       <c r="G30" s="5">
         <v>0.105</v>
@@ -10442,7 +10463,7 @@
         <v>265</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>1293</v>
+        <v>1289</v>
       </c>
       <c r="G31" s="5">
         <v>628.79999999999995</v>
@@ -10471,7 +10492,7 @@
         <v>269</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>1294</v>
+        <v>1290</v>
       </c>
       <c r="G32" s="5">
         <v>220</v>
@@ -10500,7 +10521,7 @@
         <v>273</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>1295</v>
+        <v>1291</v>
       </c>
       <c r="G33" s="5">
         <v>21667.02</v>
@@ -10529,7 +10550,7 @@
         <v>277</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>1296</v>
+        <v>1292</v>
       </c>
       <c r="G34" s="5">
         <v>10020</v>
@@ -10558,7 +10579,7 @@
         <v>277</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>1296</v>
+        <v>1292</v>
       </c>
       <c r="G35" s="5">
         <v>30.6</v>
@@ -10587,7 +10608,7 @@
         <v>277</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>1296</v>
+        <v>1292</v>
       </c>
       <c r="G36" s="5">
         <v>12</v>
@@ -10616,7 +10637,7 @@
         <v>281</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>1297</v>
+        <v>1293</v>
       </c>
       <c r="G37" s="5">
         <v>1511</v>
@@ -10645,7 +10666,7 @@
         <v>285</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>1298</v>
+        <v>1294</v>
       </c>
       <c r="G38" s="5">
         <v>88800</v>
@@ -10674,7 +10695,7 @@
         <v>285</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>1298</v>
+        <v>1294</v>
       </c>
       <c r="G39" s="5">
         <v>340</v>
@@ -10703,7 +10724,7 @@
         <v>289</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>1299</v>
+        <v>1295</v>
       </c>
       <c r="G40" s="5">
         <v>213000</v>
@@ -10755,7 +10776,7 @@
         <v>297</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>1300</v>
+        <v>1296</v>
       </c>
       <c r="G42" s="5">
         <v>9600</v>
@@ -10784,7 +10805,7 @@
         <v>297</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>1300</v>
+        <v>1296</v>
       </c>
       <c r="G43" s="5">
         <v>47</v>
@@ -10813,7 +10834,7 @@
         <v>297</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>1300</v>
+        <v>1296</v>
       </c>
       <c r="G44" s="5">
         <v>200</v>
@@ -10865,7 +10886,7 @@
         <v>301</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>1301</v>
+        <v>1297</v>
       </c>
       <c r="G46" s="5">
         <v>120</v>
@@ -10894,7 +10915,7 @@
         <v>305</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>1302</v>
+        <v>1298</v>
       </c>
       <c r="G47" s="5">
         <v>4140</v>
@@ -11012,7 +11033,7 @@
         <v>317</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>1303</v>
+        <v>1299</v>
       </c>
       <c r="G52" s="5">
         <v>6.5</v>
@@ -11041,7 +11062,7 @@
         <v>317</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>1303</v>
+        <v>1299</v>
       </c>
       <c r="G53" s="5">
         <v>1.58</v>
@@ -11070,7 +11091,7 @@
         <v>321</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>1304</v>
+        <v>1300</v>
       </c>
       <c r="G54" s="5">
         <v>52</v>
@@ -14640,13 +14661,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -14684,38 +14705,38 @@
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>1301</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>1186</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>1187</v>
       </c>
       <c r="D2" s="4">
         <v>36000</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>1189</v>
+        <v>1302</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="D3" s="4">
         <v>300</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>1191</v>
+        <v>1303</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>1192</v>
+        <v>1189</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>3</v>
@@ -14724,18 +14745,18 @@
         <v>12</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>1193</v>
+        <v>1190</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>1194</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>1195</v>
+        <v>1304</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>1196</v>
+        <v>1192</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>3</v>
@@ -14744,10 +14765,27 @@
         <v>20</v>
       </c>
       <c r="E5" s="4" t="s">
+        <v>1190</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>1193</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>1197</v>
+    </row>
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>1306</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>1307</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>1308</v>
       </c>
     </row>
   </sheetData>
@@ -14759,13 +14797,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -14796,75 +14834,89 @@
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>1198</v>
+        <v>1194</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>1199</v>
+        <v>1195</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>1200</v>
+        <v>1196</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>1201</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>1202</v>
+        <v>1198</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>1203</v>
+        <v>1199</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>1196</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>1200</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>1204</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>1205</v>
+        <v>1201</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>1206</v>
+        <v>1202</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>1200</v>
+        <v>1196</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>1207</v>
+        <v>1203</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>1208</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>1209</v>
+        <v>1205</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>1282</v>
+        <v>1278</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>1200</v>
+        <v>1196</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>1283</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>1210</v>
+        <v>1206</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>1284</v>
+        <v>1280</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>1200</v>
+        <v>1196</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>1285</v>
+        <v>1281</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>1309</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>1310</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>1311</v>
+      </c>
+      <c r="D7" s="4">
+        <v>815332823</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding references for reaction kinetics
</commit_message>
<xml_diff>
--- a/data/Model.xlsx
+++ b/data/Model.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="989" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="989" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Submodels" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1">Compartments!$A$1:$C$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4">Parameters!$A$1:$F$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3">Reactions!$A$1:$J$177</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Reactions!$A$1:$K$177</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5">References!$A$1:$E$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Species!$A$1:$N$167</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">Submodels!$A$1:$C$5</definedName>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2372" uniqueCount="1312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2511" uniqueCount="1357">
   <si>
     <t>ID</t>
   </si>
@@ -3987,6 +3987,141 @@
   </si>
   <si>
     <t>ISBN</t>
+  </si>
+  <si>
+    <t>Kinetics constrained by cell theory (mass doubling).</t>
+  </si>
+  <si>
+    <t>Kinetics determined by RNA half liife.</t>
+  </si>
+  <si>
+    <t>Ref-0007</t>
+  </si>
+  <si>
+    <t>Vmax: 1247 U/mg [Ref-0007].</t>
+  </si>
+  <si>
+    <t>Vmax: 250 U/mg [Ref-0007].</t>
+  </si>
+  <si>
+    <t>Vmax: 180 U/mg [Ref-0007].</t>
+  </si>
+  <si>
+    <t>Vmax: 220 1/s [Ref-0007].</t>
+  </si>
+  <si>
+    <t>Vmax: 0.105 U/mg [Ref-0007].</t>
+  </si>
+  <si>
+    <t>Vmax: 10.48 1/s [Ref-0007].</t>
+  </si>
+  <si>
+    <t>Vmax: 220 U/mg [Ref-0007].</t>
+  </si>
+  <si>
+    <t>Vmax: 21667.0 1/min [Ref-0007].</t>
+  </si>
+  <si>
+    <t>Vmax: 167 1/s [Ref-0007].</t>
+  </si>
+  <si>
+    <t>Vmax: 30.6 U/mg [Ref-0007].</t>
+  </si>
+  <si>
+    <t>Vmax: 12 U/mg [Ref-0007].</t>
+  </si>
+  <si>
+    <t>Vmax: 1511 U/mg [Ref-0007].</t>
+  </si>
+  <si>
+    <t>Vmax: 1480 U/mg [Ref-0007].</t>
+  </si>
+  <si>
+    <t>Vmax: 340 U/mg [Ref-0007].</t>
+  </si>
+  <si>
+    <t>Vmax: 3550 1/s [Ref-0007].</t>
+  </si>
+  <si>
+    <t>Vmax: 160 1/s [Ref-0007].</t>
+  </si>
+  <si>
+    <t>Vmax: 47 U/mg [Ref-0007].</t>
+  </si>
+  <si>
+    <t>Vmax: 200 U/mg [Ref-0007].</t>
+  </si>
+  <si>
+    <t>Vmax: 2 1/s [Ref-0007].</t>
+  </si>
+  <si>
+    <t>Vmax: 69 1/s [Ref-0007].</t>
+  </si>
+  <si>
+    <t>Vmax: 6.5 U/mg [Ref-0007].</t>
+  </si>
+  <si>
+    <t>Vmax: 1.58 U/mg [Ref-0007].</t>
+  </si>
+  <si>
+    <t>Vmax: 52 U/mg [Ref-0007].</t>
+  </si>
+  <si>
+    <t>Ref-0008</t>
+  </si>
+  <si>
+    <t>Ref-0009</t>
+  </si>
+  <si>
+    <t>Vmax: 1820 1/min [Ref-0008], 16.76 1/s [Ref-0009].</t>
+  </si>
+  <si>
+    <t>Vmax: 0.12 1/s [Ref-0007], 112 1/s [Ref-0010], 70 1/s [Ref-0011], 305 U/mg [Ref-0012].</t>
+  </si>
+  <si>
+    <t>Ref-0010</t>
+  </si>
+  <si>
+    <t>Ref-0011</t>
+  </si>
+  <si>
+    <t>Ref-0012</t>
+  </si>
+  <si>
+    <t>Berry, Alan, and Karen E. Marshall. "Identification of zinc‐binding ligands in the Class II fructose‐1, 6‐bisphosphate aldolase of Escherichia coli." FEBS letters 318.1 (1993): 11-16.</t>
+  </si>
+  <si>
+    <t>Iturrate, Laura, et al. "Preparation and Characterization of a Bifunctional Aldolase/Kinase Enzyme: A More Efficient Biocatalyst for C C Bond Formation." Chemistry–A European Journal 16.13 (2010): 4018-4030.</t>
+  </si>
+  <si>
+    <t>Fillinger, Sabine, et al. "Two glyceraldehyde-3-phosphate dehydrogenases with opposite physiological roles in a nonphotosynthetic bacterium." Journal of Biological Chemistry 275.19 (2000): 14031-14037.</t>
+  </si>
+  <si>
+    <t>Even, S., et al. "Pyruvate metabolism in Lactococcus lactis is dependent upon glyceraldehyde-3-phosphate dehydrogenase activity." Metabolic engineering 1.3 (1999): 198-205.</t>
+  </si>
+  <si>
+    <t>Crow, Vaughan L., and C. L. Wittenberger. "Separation and properties of NAD+-and NADP+-dependent glyceraldehyde-3-phosphate dehydrogenases from Streptococcus mutans." Journal of Biological Chemistry 254.4 (1979): 1134-1142.</t>
+  </si>
+  <si>
+    <t>10.1016/0014-5793(93)81317-S</t>
+  </si>
+  <si>
+    <t>10.1006/mben.1999.0120</t>
+  </si>
+  <si>
+    <t>10.1074/jbc.275.19.14031</t>
+  </si>
+  <si>
+    <t>10.1002/chem.200903096</t>
+  </si>
+  <si>
+    <t>PMID</t>
+  </si>
+  <si>
+    <t>Wittig, Ulrike, et al. "SABIO-RK: integration and curation of reaction kinetics data." Data integration in the life sciences. Springer Berlin Heidelberg, 2006.</t>
+  </si>
+  <si>
+    <t>10.1007/11799511_9</t>
   </si>
 </sst>
 </file>
@@ -4601,11 +4736,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O167"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9743,13 +9878,14 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J177"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:K177"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A170" sqref="A170"/>
-      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomRight" activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9762,10 +9898,11 @@
     <col min="7" max="7" width="9.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="10" style="4"/>
-    <col min="11" max="16384" width="9.140625" style="4"/>
+    <col min="11" max="11" width="24.7109375" style="4" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="3" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="3" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9796,8 +9933,11 @@
       <c r="J1" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>560</v>
       </c>
@@ -9825,8 +9965,11 @@
       <c r="J2" s="4" t="s">
         <v>564</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K2" s="4" t="s">
+        <v>1315</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>565</v>
       </c>
@@ -9849,7 +9992,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>568</v>
       </c>
@@ -9872,7 +10015,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>572</v>
       </c>
@@ -9900,8 +10043,11 @@
       <c r="J5" s="4" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K5" s="4" t="s">
+        <v>1316</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>576</v>
       </c>
@@ -9921,7 +10067,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>580</v>
       </c>
@@ -9941,7 +10087,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>584</v>
       </c>
@@ -9961,7 +10107,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>587</v>
       </c>
@@ -9981,7 +10127,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>590</v>
       </c>
@@ -10001,7 +10147,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>593</v>
       </c>
@@ -10021,7 +10167,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>596</v>
       </c>
@@ -10041,7 +10187,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>600</v>
       </c>
@@ -10061,7 +10207,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>603</v>
       </c>
@@ -10081,7 +10227,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>606</v>
       </c>
@@ -10101,7 +10247,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>609</v>
       </c>
@@ -10121,7 +10267,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>612</v>
       </c>
@@ -10141,7 +10287,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>615</v>
       </c>
@@ -10161,7 +10307,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>618</v>
       </c>
@@ -10181,7 +10327,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>621</v>
       </c>
@@ -10201,7 +10347,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>624</v>
       </c>
@@ -10221,7 +10367,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>627</v>
       </c>
@@ -10241,7 +10387,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>630</v>
       </c>
@@ -10261,7 +10407,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>633</v>
       </c>
@@ -10281,7 +10427,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>636</v>
       </c>
@@ -10301,7 +10447,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>639</v>
       </c>
@@ -10329,8 +10475,11 @@
       <c r="J26" s="4" t="s">
         <v>642</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K26" s="4" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>643</v>
       </c>
@@ -10358,8 +10507,11 @@
       <c r="J27" s="4" t="s">
         <v>646</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K27" s="4" t="s">
+        <v>1340</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>647</v>
       </c>
@@ -10387,8 +10539,11 @@
       <c r="J28" s="4" t="s">
         <v>650</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K28" s="4" t="s">
+        <v>1341</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>651</v>
       </c>
@@ -10416,8 +10571,11 @@
       <c r="J29" s="4" t="s">
         <v>654</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K29" s="4" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>655</v>
       </c>
@@ -10445,8 +10603,11 @@
       <c r="J30" s="4" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K30" s="4" t="s">
+        <v>1319</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>659</v>
       </c>
@@ -10474,8 +10635,11 @@
       <c r="J31" s="4" t="s">
         <v>662</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K31" s="4" t="s">
+        <v>1320</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>663</v>
       </c>
@@ -10503,8 +10667,11 @@
       <c r="J32" s="4" t="s">
         <v>666</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K32" s="4" t="s">
+        <v>1321</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>667</v>
       </c>
@@ -10532,8 +10699,11 @@
       <c r="J33" s="4" t="s">
         <v>670</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K33" s="4" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>671</v>
       </c>
@@ -10561,8 +10731,11 @@
       <c r="J34" s="4" t="s">
         <v>674</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K34" s="4" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>675</v>
       </c>
@@ -10590,8 +10763,11 @@
       <c r="J35" s="4" t="s">
         <v>674</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K35" s="4" t="s">
+        <v>1324</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>678</v>
       </c>
@@ -10619,8 +10795,11 @@
       <c r="J36" s="4" t="s">
         <v>674</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K36" s="4" t="s">
+        <v>1325</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>681</v>
       </c>
@@ -10648,8 +10827,11 @@
       <c r="J37" s="4" t="s">
         <v>684</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K37" s="4" t="s">
+        <v>1326</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>685</v>
       </c>
@@ -10677,8 +10859,11 @@
       <c r="J38" s="4" t="s">
         <v>688</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K38" s="4" t="s">
+        <v>1327</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>689</v>
       </c>
@@ -10706,8 +10891,11 @@
       <c r="J39" s="4" t="s">
         <v>688</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K39" s="4" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>692</v>
       </c>
@@ -10735,8 +10923,11 @@
       <c r="J40" s="4" t="s">
         <v>695</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K40" s="4" t="s">
+        <v>1329</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>696</v>
       </c>
@@ -10759,7 +10950,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>700</v>
       </c>
@@ -10787,8 +10978,11 @@
       <c r="J42" s="4" t="s">
         <v>703</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K42" s="4" t="s">
+        <v>1330</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>704</v>
       </c>
@@ -10816,8 +11010,11 @@
       <c r="J43" s="4" t="s">
         <v>703</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K43" s="4" t="s">
+        <v>1331</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>707</v>
       </c>
@@ -10845,8 +11042,11 @@
       <c r="J44" s="4" t="s">
         <v>703</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K44" s="4" t="s">
+        <v>1332</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>710</v>
       </c>
@@ -10869,7 +11069,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>713</v>
       </c>
@@ -10897,8 +11097,11 @@
       <c r="J46" s="4" t="s">
         <v>716</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K46" s="4" t="s">
+        <v>1333</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>717</v>
       </c>
@@ -10926,8 +11129,11 @@
       <c r="J47" s="4" t="s">
         <v>720</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K47" s="4" t="s">
+        <v>1334</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>721</v>
       </c>
@@ -10947,7 +11153,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>725</v>
       </c>
@@ -10970,7 +11176,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>729</v>
       </c>
@@ -10993,7 +11199,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>733</v>
       </c>
@@ -11016,7 +11222,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>736</v>
       </c>
@@ -11044,8 +11250,11 @@
       <c r="J52" s="4" t="s">
         <v>739</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K52" s="4" t="s">
+        <v>1335</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>740</v>
       </c>
@@ -11073,8 +11282,11 @@
       <c r="J53" s="4" t="s">
         <v>739</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K53" s="4" t="s">
+        <v>1336</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>743</v>
       </c>
@@ -11102,8 +11314,11 @@
       <c r="J54" s="4" t="s">
         <v>746</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K54" s="4" t="s">
+        <v>1337</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>747</v>
       </c>
@@ -11126,7 +11341,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>751</v>
       </c>
@@ -11149,7 +11364,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>755</v>
       </c>
@@ -11163,7 +11378,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>758</v>
       </c>
@@ -11177,7 +11392,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>761</v>
       </c>
@@ -11191,7 +11406,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>764</v>
       </c>
@@ -11205,7 +11420,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>767</v>
       </c>
@@ -11219,7 +11434,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>770</v>
       </c>
@@ -11242,7 +11457,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>774</v>
       </c>
@@ -11256,7 +11471,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>777</v>
       </c>
@@ -11270,7 +11485,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>780</v>
       </c>
@@ -11284,7 +11499,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>783</v>
       </c>
@@ -11298,7 +11513,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>786</v>
       </c>
@@ -11321,7 +11536,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>790</v>
       </c>
@@ -11344,7 +11559,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>793</v>
       </c>
@@ -11367,7 +11582,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>796</v>
       </c>
@@ -11390,7 +11605,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
         <v>799</v>
       </c>
@@ -11413,7 +11628,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>802</v>
       </c>
@@ -11436,7 +11651,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="73" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>805</v>
       </c>
@@ -11459,7 +11674,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>808</v>
       </c>
@@ -11482,7 +11697,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>811</v>
       </c>
@@ -11505,7 +11720,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>814</v>
       </c>
@@ -11528,7 +11743,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>817</v>
       </c>
@@ -11551,7 +11766,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>820</v>
       </c>
@@ -11574,7 +11789,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="79" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>823</v>
       </c>
@@ -11597,7 +11812,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>826</v>
       </c>
@@ -11620,7 +11835,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>829</v>
       </c>
@@ -11643,7 +11858,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="82" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>832</v>
       </c>
@@ -11666,7 +11881,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="83" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
         <v>835</v>
       </c>
@@ -11689,7 +11904,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
         <v>838</v>
       </c>
@@ -11712,7 +11927,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="85" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
         <v>841</v>
       </c>
@@ -11735,7 +11950,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
         <v>844</v>
       </c>
@@ -11758,7 +11973,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="87" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
         <v>847</v>
       </c>
@@ -11789,8 +12004,11 @@
       <c r="J87" s="4" t="s">
         <v>851</v>
       </c>
-    </row>
-    <row r="88" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K87" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
         <v>852</v>
       </c>
@@ -11821,8 +12039,11 @@
       <c r="J88" s="4" t="s">
         <v>851</v>
       </c>
-    </row>
-    <row r="89" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K88" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
         <v>855</v>
       </c>
@@ -11853,8 +12074,11 @@
       <c r="J89" s="4" t="s">
         <v>851</v>
       </c>
-    </row>
-    <row r="90" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K89" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
         <v>858</v>
       </c>
@@ -11885,8 +12109,11 @@
       <c r="J90" s="4" t="s">
         <v>851</v>
       </c>
-    </row>
-    <row r="91" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K90" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
         <v>861</v>
       </c>
@@ -11917,8 +12144,11 @@
       <c r="J91" s="4" t="s">
         <v>851</v>
       </c>
-    </row>
-    <row r="92" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K91" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
         <v>864</v>
       </c>
@@ -11949,8 +12179,11 @@
       <c r="J92" s="4" t="s">
         <v>851</v>
       </c>
-    </row>
-    <row r="93" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K92" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
         <v>867</v>
       </c>
@@ -11981,8 +12214,11 @@
       <c r="J93" s="4" t="s">
         <v>851</v>
       </c>
-    </row>
-    <row r="94" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K93" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
         <v>870</v>
       </c>
@@ -12013,8 +12249,11 @@
       <c r="J94" s="4" t="s">
         <v>851</v>
       </c>
-    </row>
-    <row r="95" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K94" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
         <v>873</v>
       </c>
@@ -12045,8 +12284,11 @@
       <c r="J95" s="4" t="s">
         <v>851</v>
       </c>
-    </row>
-    <row r="96" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K95" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
         <v>876</v>
       </c>
@@ -12077,8 +12319,11 @@
       <c r="J96" s="4" t="s">
         <v>851</v>
       </c>
-    </row>
-    <row r="97" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K96" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
         <v>879</v>
       </c>
@@ -12109,8 +12354,11 @@
       <c r="J97" s="4" t="s">
         <v>851</v>
       </c>
-    </row>
-    <row r="98" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K97" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
         <v>882</v>
       </c>
@@ -12141,8 +12389,11 @@
       <c r="J98" s="4" t="s">
         <v>851</v>
       </c>
-    </row>
-    <row r="99" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K98" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
         <v>885</v>
       </c>
@@ -12173,8 +12424,11 @@
       <c r="J99" s="4" t="s">
         <v>851</v>
       </c>
-    </row>
-    <row r="100" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K99" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
         <v>888</v>
       </c>
@@ -12205,8 +12459,11 @@
       <c r="J100" s="4" t="s">
         <v>851</v>
       </c>
-    </row>
-    <row r="101" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K100" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
         <v>891</v>
       </c>
@@ -12237,8 +12494,11 @@
       <c r="J101" s="4" t="s">
         <v>851</v>
       </c>
-    </row>
-    <row r="102" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K101" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
         <v>894</v>
       </c>
@@ -12269,8 +12529,11 @@
       <c r="J102" s="4" t="s">
         <v>851</v>
       </c>
-    </row>
-    <row r="103" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K102" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
         <v>897</v>
       </c>
@@ -12301,8 +12564,11 @@
       <c r="J103" s="4" t="s">
         <v>851</v>
       </c>
-    </row>
-    <row r="104" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K103" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
         <v>900</v>
       </c>
@@ -12333,8 +12599,11 @@
       <c r="J104" s="4" t="s">
         <v>851</v>
       </c>
-    </row>
-    <row r="105" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K104" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
         <v>903</v>
       </c>
@@ -12365,8 +12634,11 @@
       <c r="J105" s="4" t="s">
         <v>851</v>
       </c>
-    </row>
-    <row r="106" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K105" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
         <v>906</v>
       </c>
@@ -12397,8 +12669,11 @@
       <c r="J106" s="4" t="s">
         <v>851</v>
       </c>
-    </row>
-    <row r="107" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K106" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
         <v>909</v>
       </c>
@@ -12429,8 +12704,11 @@
       <c r="J107" s="4" t="s">
         <v>851</v>
       </c>
-    </row>
-    <row r="108" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K107" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
         <v>912</v>
       </c>
@@ -12461,8 +12739,11 @@
       <c r="J108" s="4" t="s">
         <v>851</v>
       </c>
-    </row>
-    <row r="109" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K108" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
         <v>915</v>
       </c>
@@ -12493,8 +12774,11 @@
       <c r="J109" s="4" t="s">
         <v>851</v>
       </c>
-    </row>
-    <row r="110" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K109" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
         <v>918</v>
       </c>
@@ -12525,8 +12809,11 @@
       <c r="J110" s="4" t="s">
         <v>851</v>
       </c>
-    </row>
-    <row r="111" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K110" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
         <v>921</v>
       </c>
@@ -12557,8 +12844,11 @@
       <c r="J111" s="4" t="s">
         <v>851</v>
       </c>
-    </row>
-    <row r="112" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K111" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
         <v>924</v>
       </c>
@@ -12589,8 +12879,11 @@
       <c r="J112" s="4" t="s">
         <v>851</v>
       </c>
-    </row>
-    <row r="113" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K112" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
         <v>927</v>
       </c>
@@ -12621,8 +12914,11 @@
       <c r="J113" s="4" t="s">
         <v>851</v>
       </c>
-    </row>
-    <row r="114" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K113" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
         <v>930</v>
       </c>
@@ -12653,8 +12949,11 @@
       <c r="J114" s="4" t="s">
         <v>851</v>
       </c>
-    </row>
-    <row r="115" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K114" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
         <v>933</v>
       </c>
@@ -12685,8 +12984,11 @@
       <c r="J115" s="4" t="s">
         <v>851</v>
       </c>
-    </row>
-    <row r="116" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K115" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
         <v>936</v>
       </c>
@@ -12717,8 +13019,11 @@
       <c r="J116" s="4" t="s">
         <v>851</v>
       </c>
-    </row>
-    <row r="117" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K116" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
         <v>939</v>
       </c>
@@ -12749,8 +13054,11 @@
       <c r="J117" s="4" t="s">
         <v>943</v>
       </c>
-    </row>
-    <row r="118" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K117" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
         <v>944</v>
       </c>
@@ -12781,8 +13089,11 @@
       <c r="J118" s="4" t="s">
         <v>943</v>
       </c>
-    </row>
-    <row r="119" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K118" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
         <v>948</v>
       </c>
@@ -12813,8 +13124,11 @@
       <c r="J119" s="4" t="s">
         <v>943</v>
       </c>
-    </row>
-    <row r="120" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K119" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
         <v>952</v>
       </c>
@@ -12845,8 +13159,11 @@
       <c r="J120" s="4" t="s">
         <v>943</v>
       </c>
-    </row>
-    <row r="121" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K120" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="s">
         <v>956</v>
       </c>
@@ -12877,8 +13194,11 @@
       <c r="J121" s="4" t="s">
         <v>943</v>
       </c>
-    </row>
-    <row r="122" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K121" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
         <v>960</v>
       </c>
@@ -12909,8 +13229,11 @@
       <c r="J122" s="4" t="s">
         <v>943</v>
       </c>
-    </row>
-    <row r="123" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K122" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="s">
         <v>964</v>
       </c>
@@ -12941,8 +13264,11 @@
       <c r="J123" s="4" t="s">
         <v>943</v>
       </c>
-    </row>
-    <row r="124" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K123" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="s">
         <v>968</v>
       </c>
@@ -12973,8 +13299,11 @@
       <c r="J124" s="4" t="s">
         <v>943</v>
       </c>
-    </row>
-    <row r="125" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K124" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="s">
         <v>972</v>
       </c>
@@ -13005,8 +13334,11 @@
       <c r="J125" s="4" t="s">
         <v>943</v>
       </c>
-    </row>
-    <row r="126" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K125" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="s">
         <v>976</v>
       </c>
@@ -13037,8 +13369,11 @@
       <c r="J126" s="4" t="s">
         <v>943</v>
       </c>
-    </row>
-    <row r="127" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K126" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="s">
         <v>980</v>
       </c>
@@ -13069,8 +13404,11 @@
       <c r="J127" s="4" t="s">
         <v>943</v>
       </c>
-    </row>
-    <row r="128" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K127" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="s">
         <v>984</v>
       </c>
@@ -13101,8 +13439,11 @@
       <c r="J128" s="4" t="s">
         <v>943</v>
       </c>
-    </row>
-    <row r="129" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K128" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="4" t="s">
         <v>988</v>
       </c>
@@ -13133,8 +13474,11 @@
       <c r="J129" s="4" t="s">
         <v>943</v>
       </c>
-    </row>
-    <row r="130" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K129" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="s">
         <v>992</v>
       </c>
@@ -13165,8 +13509,11 @@
       <c r="J130" s="4" t="s">
         <v>943</v>
       </c>
-    </row>
-    <row r="131" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K130" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="4" t="s">
         <v>996</v>
       </c>
@@ -13197,8 +13544,11 @@
       <c r="J131" s="4" t="s">
         <v>943</v>
       </c>
-    </row>
-    <row r="132" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K131" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="s">
         <v>1000</v>
       </c>
@@ -13229,8 +13579,11 @@
       <c r="J132" s="4" t="s">
         <v>943</v>
       </c>
-    </row>
-    <row r="133" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K132" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="4" t="s">
         <v>1004</v>
       </c>
@@ -13261,8 +13614,11 @@
       <c r="J133" s="4" t="s">
         <v>943</v>
       </c>
-    </row>
-    <row r="134" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K133" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="4" t="s">
         <v>1008</v>
       </c>
@@ -13293,8 +13649,11 @@
       <c r="J134" s="4" t="s">
         <v>943</v>
       </c>
-    </row>
-    <row r="135" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K134" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="4" t="s">
         <v>1012</v>
       </c>
@@ -13325,8 +13684,11 @@
       <c r="J135" s="4" t="s">
         <v>943</v>
       </c>
-    </row>
-    <row r="136" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K135" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="4" t="s">
         <v>1016</v>
       </c>
@@ -13357,8 +13719,11 @@
       <c r="J136" s="4" t="s">
         <v>943</v>
       </c>
-    </row>
-    <row r="137" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K136" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="4" t="s">
         <v>1020</v>
       </c>
@@ -13389,8 +13754,11 @@
       <c r="J137" s="4" t="s">
         <v>943</v>
       </c>
-    </row>
-    <row r="138" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K137" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="4" t="s">
         <v>1024</v>
       </c>
@@ -13421,8 +13789,11 @@
       <c r="J138" s="4" t="s">
         <v>943</v>
       </c>
-    </row>
-    <row r="139" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K138" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="4" t="s">
         <v>1028</v>
       </c>
@@ -13453,8 +13824,11 @@
       <c r="J139" s="4" t="s">
         <v>943</v>
       </c>
-    </row>
-    <row r="140" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K139" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="4" t="s">
         <v>1032</v>
       </c>
@@ -13485,8 +13859,11 @@
       <c r="J140" s="4" t="s">
         <v>943</v>
       </c>
-    </row>
-    <row r="141" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K140" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="4" t="s">
         <v>1036</v>
       </c>
@@ -13517,8 +13894,11 @@
       <c r="J141" s="4" t="s">
         <v>943</v>
       </c>
-    </row>
-    <row r="142" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K141" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="4" t="s">
         <v>1040</v>
       </c>
@@ -13549,8 +13929,11 @@
       <c r="J142" s="4" t="s">
         <v>943</v>
       </c>
-    </row>
-    <row r="143" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K142" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="4" t="s">
         <v>1044</v>
       </c>
@@ -13581,8 +13964,11 @@
       <c r="J143" s="4" t="s">
         <v>943</v>
       </c>
-    </row>
-    <row r="144" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K143" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="4" t="s">
         <v>1048</v>
       </c>
@@ -13613,8 +13999,11 @@
       <c r="J144" s="4" t="s">
         <v>943</v>
       </c>
-    </row>
-    <row r="145" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K144" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="145" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="4" t="s">
         <v>1052</v>
       </c>
@@ -13645,8 +14034,11 @@
       <c r="J145" s="4" t="s">
         <v>943</v>
       </c>
-    </row>
-    <row r="146" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K145" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="146" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="4" t="s">
         <v>1056</v>
       </c>
@@ -13677,8 +14069,11 @@
       <c r="J146" s="4" t="s">
         <v>943</v>
       </c>
-    </row>
-    <row r="147" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K146" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="147" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="4" t="s">
         <v>1060</v>
       </c>
@@ -13709,8 +14104,11 @@
       <c r="J147" s="4" t="s">
         <v>1064</v>
       </c>
-    </row>
-    <row r="148" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K147" s="4" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="148" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="4" t="s">
         <v>1065</v>
       </c>
@@ -13741,8 +14139,11 @@
       <c r="J148" s="4" t="s">
         <v>1064</v>
       </c>
-    </row>
-    <row r="149" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K148" s="4" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="149" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="4" t="s">
         <v>1069</v>
       </c>
@@ -13773,8 +14174,11 @@
       <c r="J149" s="4" t="s">
         <v>1064</v>
       </c>
-    </row>
-    <row r="150" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K149" s="4" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="150" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="4" t="s">
         <v>1073</v>
       </c>
@@ -13805,8 +14209,11 @@
       <c r="J150" s="4" t="s">
         <v>1064</v>
       </c>
-    </row>
-    <row r="151" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K150" s="4" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="151" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="4" t="s">
         <v>1077</v>
       </c>
@@ -13837,8 +14244,11 @@
       <c r="J151" s="4" t="s">
         <v>1064</v>
       </c>
-    </row>
-    <row r="152" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K151" s="4" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="152" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="4" t="s">
         <v>1081</v>
       </c>
@@ -13869,8 +14279,11 @@
       <c r="J152" s="4" t="s">
         <v>1064</v>
       </c>
-    </row>
-    <row r="153" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K152" s="4" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="4" t="s">
         <v>1085</v>
       </c>
@@ -13901,8 +14314,11 @@
       <c r="J153" s="4" t="s">
         <v>1064</v>
       </c>
-    </row>
-    <row r="154" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K153" s="4" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="4" t="s">
         <v>1089</v>
       </c>
@@ -13933,8 +14349,11 @@
       <c r="J154" s="4" t="s">
         <v>1064</v>
       </c>
-    </row>
-    <row r="155" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K154" s="4" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="155" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="4" t="s">
         <v>1093</v>
       </c>
@@ -13965,8 +14384,11 @@
       <c r="J155" s="4" t="s">
         <v>1064</v>
       </c>
-    </row>
-    <row r="156" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K155" s="4" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="156" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="4" t="s">
         <v>1097</v>
       </c>
@@ -13997,8 +14419,11 @@
       <c r="J156" s="4" t="s">
         <v>1064</v>
       </c>
-    </row>
-    <row r="157" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K156" s="4" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="157" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="4" t="s">
         <v>1101</v>
       </c>
@@ -14029,8 +14454,11 @@
       <c r="J157" s="4" t="s">
         <v>1064</v>
       </c>
-    </row>
-    <row r="158" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K157" s="4" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="158" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="4" t="s">
         <v>1105</v>
       </c>
@@ -14061,8 +14489,11 @@
       <c r="J158" s="4" t="s">
         <v>1064</v>
       </c>
-    </row>
-    <row r="159" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K158" s="4" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="159" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="4" t="s">
         <v>1109</v>
       </c>
@@ -14093,8 +14524,11 @@
       <c r="J159" s="4" t="s">
         <v>1064</v>
       </c>
-    </row>
-    <row r="160" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K159" s="4" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="160" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="4" t="s">
         <v>1113</v>
       </c>
@@ -14125,8 +14559,11 @@
       <c r="J160" s="4" t="s">
         <v>1064</v>
       </c>
-    </row>
-    <row r="161" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K160" s="4" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="161" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="4" t="s">
         <v>1117</v>
       </c>
@@ -14157,8 +14594,11 @@
       <c r="J161" s="4" t="s">
         <v>1064</v>
       </c>
-    </row>
-    <row r="162" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K161" s="4" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="162" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="4" t="s">
         <v>1121</v>
       </c>
@@ -14189,8 +14629,11 @@
       <c r="J162" s="4" t="s">
         <v>1064</v>
       </c>
-    </row>
-    <row r="163" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K162" s="4" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="4" t="s">
         <v>1125</v>
       </c>
@@ -14221,8 +14664,11 @@
       <c r="J163" s="4" t="s">
         <v>1064</v>
       </c>
-    </row>
-    <row r="164" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K163" s="4" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="164" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="4" t="s">
         <v>1129</v>
       </c>
@@ -14253,8 +14699,11 @@
       <c r="J164" s="4" t="s">
         <v>1064</v>
       </c>
-    </row>
-    <row r="165" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K164" s="4" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="165" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="4" t="s">
         <v>1133</v>
       </c>
@@ -14285,8 +14734,11 @@
       <c r="J165" s="4" t="s">
         <v>1064</v>
       </c>
-    </row>
-    <row r="166" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K165" s="4" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="166" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="4" t="s">
         <v>1137</v>
       </c>
@@ -14317,8 +14769,11 @@
       <c r="J166" s="4" t="s">
         <v>1064</v>
       </c>
-    </row>
-    <row r="167" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K166" s="4" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="167" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="4" t="s">
         <v>1141</v>
       </c>
@@ -14349,8 +14804,11 @@
       <c r="J167" s="4" t="s">
         <v>1064</v>
       </c>
-    </row>
-    <row r="168" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K167" s="4" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="168" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="4" t="s">
         <v>1145</v>
       </c>
@@ -14381,8 +14839,11 @@
       <c r="J168" s="4" t="s">
         <v>1064</v>
       </c>
-    </row>
-    <row r="169" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K168" s="4" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="169" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="4" t="s">
         <v>1149</v>
       </c>
@@ -14413,8 +14874,11 @@
       <c r="J169" s="4" t="s">
         <v>1064</v>
       </c>
-    </row>
-    <row r="170" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K169" s="4" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="170" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="4" t="s">
         <v>1153</v>
       </c>
@@ -14445,8 +14909,11 @@
       <c r="J170" s="4" t="s">
         <v>1064</v>
       </c>
-    </row>
-    <row r="171" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K170" s="4" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="171" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="4" t="s">
         <v>1157</v>
       </c>
@@ -14477,8 +14944,11 @@
       <c r="J171" s="4" t="s">
         <v>1064</v>
       </c>
-    </row>
-    <row r="172" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K171" s="4" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="172" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="4" t="s">
         <v>1161</v>
       </c>
@@ -14509,8 +14979,11 @@
       <c r="J172" s="4" t="s">
         <v>1064</v>
       </c>
-    </row>
-    <row r="173" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K172" s="4" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="173" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="4" t="s">
         <v>1165</v>
       </c>
@@ -14541,8 +15014,11 @@
       <c r="J173" s="4" t="s">
         <v>1064</v>
       </c>
-    </row>
-    <row r="174" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K173" s="4" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="174" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="4" t="s">
         <v>1169</v>
       </c>
@@ -14573,8 +15049,11 @@
       <c r="J174" s="4" t="s">
         <v>1064</v>
       </c>
-    </row>
-    <row r="175" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K174" s="4" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="175" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="4" t="s">
         <v>1173</v>
       </c>
@@ -14605,8 +15084,11 @@
       <c r="J175" s="4" t="s">
         <v>1064</v>
       </c>
-    </row>
-    <row r="176" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K175" s="4" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="176" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="4" t="s">
         <v>1177</v>
       </c>
@@ -14637,8 +15119,11 @@
       <c r="J176" s="4" t="s">
         <v>1064</v>
       </c>
-    </row>
-    <row r="177" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K176" s="4" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="4" t="s">
         <v>1181</v>
       </c>
@@ -14653,7 +15138,66 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J177"/>
+  <autoFilter xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" ref="A1:K177">
+    <filterColumn colId="10">
+      <filters>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <x14:filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;0.105&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #30207&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;U/mg&quot;, &quot;species&quot;: &quot;Rattus norvegicus&quot;}"/>
+            <x14:filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;1.58&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #15484&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;U/mg&quot;, &quot;species&quot;: &quot;Homo sapiens&quot;}"/>
+            <x14:filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;10.48&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #10179&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;1/s&quot;, &quot;species&quot;: &quot;Homo sapiens&quot;}"/>
+            <x14:filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;1247&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #13276&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;U/mg&quot;, &quot;species&quot;: &quot;Escherichia coli&quot;}"/>
+            <x14:filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;1480&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #22933&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;1/s&quot;, &quot;species&quot;: &quot;Escherichia coli&quot;}"/>
+            <x14:filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;1511&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #32322&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;U/mg&quot;, &quot;species&quot;: &quot;Escherichia coli&quot;}"/>
+            <x14:filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;160&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #9571&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;1/s&quot;, &quot;species&quot;: &quot;Escherichia coli&quot;}"/>
+            <x14:filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;167&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #36109&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;1/s&quot;, &quot;species&quot;: &quot;Escherichia coli&quot;}"/>
+            <x14:filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;180&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #7357&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;U/mg&quot;, &quot;species&quot;: &quot;Escherichia coli&quot;}"/>
+            <x14:filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;2&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #28897&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;1/s&quot;, &quot;species&quot;: &quot;Escherichia coli&quot;}"/>
+            <x14:filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;200&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #24532&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;U/mg&quot;, &quot;species&quot;: &quot;Streptococcus mutans&quot;}"/>
+            <x14:filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;21667.0&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #26928&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;1/min&quot;, &quot;species&quot;: &quot;Enterococcus faecalis&quot;}"/>
+            <x14:filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;220&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #16538&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;U/mg&quot;, &quot;species&quot;: &quot;Lactobacillus curvatus&quot;}"/>
+            <x14:filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;220&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #27646&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;1/s&quot;, &quot;species&quot;: &quot;Escherichia coli&quot;}"/>
+            <x14:filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;250&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #17213&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;U/mg&quot;, &quot;species&quot;: &quot;Escherichia coli&quot;}"/>
+            <x14:filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;340&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #21262&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;U/mg&quot;, &quot;species&quot;: &quot;Saccharomyces cerevisiae&quot;}"/>
+            <x14:filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;3550&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #224&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;1/s&quot;, &quot;species&quot;: &quot;Streptococcus gordonii&quot;}"/>
+            <x14:filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;47&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #45990&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;U/mg&quot;, &quot;species&quot;: &quot;Escherichia coli&quot;}"/>
+            <x14:filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;52&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #40418&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;U/mg&quot;, &quot;species&quot;: &quot;Bacillus subtilis&quot;}"/>
+            <x14:filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;6.5&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #39676&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;U/mg&quot;, &quot;species&quot;: &quot;Homo sapiens&quot;}"/>
+            <x14:filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;69&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #24910&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;1/s&quot;, &quot;species&quot;: &quot;Escherichia coli&quot;}"/>
+            <x14:filter val="{&quot;species&quot;: &quot;Escherichia coli K12&quot;, &quot;species_component&quot;: &quot;P0A796&quot;, &quot;value&quot;: 12, &quot;units&quot;: &quot;U/mg&quot;, &quot;comments&quot;: &quot;SABIO-RK entry #21873.&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;]}"/>
+            <x14:filter val="{&quot;species&quot;: &quot;Escherichia coli K12&quot;, &quot;species_component&quot;: &quot;P0A796&quot;, &quot;value&quot;: 30.6, &quot;units&quot;: &quot;U/mg&quot;, &quot;comments&quot;: &quot;SABIO-RK entry #21872.&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;]}"/>
+            <x14:filter val="{&quot;value&quot;: 16.76, &quot;units&quot;: &quot;1/s&quot;, &quot;is_experimentally_constrained&quot;: true, &quot;species&quot;: &quot;Staphylococcus carnosus&quot;, &quot;references&quot;: [&quot;PUB_1177&quot;]},_x000a_{&quot;value&quot;: 1820, &quot;units&quot;: &quot;1/min&quot;, &quot;is_experimentally_constrained&quot;: true, &quot;species&quot;: &quot;Escherichia coli&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #343243&quot;, &quot;references&quot;: [&quot;PUB_1176&quot;]}"/>
+            <x14:filter val="{&quot;value&quot;: 70, &quot;units&quot;: &quot;1/s&quot;, &quot;is_experimentally_constrained&quot;: true, &quot;species&quot;: &quot;Lactococcus lactis subsp. lactis&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #20212&quot;, &quot;references&quot;: [&quot;PUB_1186&quot;]},_x000a_{&quot;value&quot;: 112, &quot;units&quot;: &quot;1/s&quot;, &quot;is_experimentally_constrained&quot;: true, &quot;species&quot;: &quot;Geobacillus stearothermophilus&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #43582&quot;, &quot;references&quot;: [&quot;PUB_1185&quot;]},_x000a_{&quot;value&quot;: 305, &quot;units&quot;: &quot;U/mg&quot;, &quot;is_experimentally_constrained&quot;: true, &quot;species&quot;: &quot;Streptococcus mutans&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #20980&quot;, &quot;references&quot;: [&quot;PUB_1187&quot;]},_x000a_{&quot;value&quot;: 0.12, &quot;units&quot;: &quot;1/s&quot;, &quot;is_experimentally_constrained&quot;: true, &quot;species&quot;: &quot;Escherichia coli&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #37150&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;]}"/>
+          </mc:Choice>
+          <mc:Fallback>
+            <filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;0.105&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #30207&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;U/mg&quot;, &quot;species&quot;: &quot;Rattus norvegicus&quot;}"/>
+            <filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;1.58&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #15484&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;U/mg&quot;, &quot;species&quot;: &quot;Homo sapiens&quot;}"/>
+            <filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;10.48&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #10179&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;1/s&quot;, &quot;species&quot;: &quot;Homo sapiens&quot;}"/>
+            <filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;1247&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #13276&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;U/mg&quot;, &quot;species&quot;: &quot;Escherichia coli&quot;}"/>
+            <filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;1480&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #22933&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;1/s&quot;, &quot;species&quot;: &quot;Escherichia coli&quot;}"/>
+            <filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;1511&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #32322&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;U/mg&quot;, &quot;species&quot;: &quot;Escherichia coli&quot;}"/>
+            <filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;160&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #9571&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;1/s&quot;, &quot;species&quot;: &quot;Escherichia coli&quot;}"/>
+            <filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;167&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #36109&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;1/s&quot;, &quot;species&quot;: &quot;Escherichia coli&quot;}"/>
+            <filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;180&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #7357&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;U/mg&quot;, &quot;species&quot;: &quot;Escherichia coli&quot;}"/>
+            <filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;2&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #28897&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;1/s&quot;, &quot;species&quot;: &quot;Escherichia coli&quot;}"/>
+            <filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;200&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #24532&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;U/mg&quot;, &quot;species&quot;: &quot;Streptococcus mutans&quot;}"/>
+            <filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;21667.0&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #26928&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;1/min&quot;, &quot;species&quot;: &quot;Enterococcus faecalis&quot;}"/>
+            <filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;220&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #16538&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;U/mg&quot;, &quot;species&quot;: &quot;Lactobacillus curvatus&quot;}"/>
+            <filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;220&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #27646&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;1/s&quot;, &quot;species&quot;: &quot;Escherichia coli&quot;}"/>
+            <filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;250&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #17213&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;U/mg&quot;, &quot;species&quot;: &quot;Escherichia coli&quot;}"/>
+            <filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;340&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #21262&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;U/mg&quot;, &quot;species&quot;: &quot;Saccharomyces cerevisiae&quot;}"/>
+            <filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;3550&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #224&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;1/s&quot;, &quot;species&quot;: &quot;Streptococcus gordonii&quot;}"/>
+            <filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;47&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #45990&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;U/mg&quot;, &quot;species&quot;: &quot;Escherichia coli&quot;}"/>
+            <filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;52&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #40418&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;U/mg&quot;, &quot;species&quot;: &quot;Bacillus subtilis&quot;}"/>
+            <filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;6.5&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #39676&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;U/mg&quot;, &quot;species&quot;: &quot;Homo sapiens&quot;}"/>
+            <filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;69&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #24910&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;1/s&quot;, &quot;species&quot;: &quot;Escherichia coli&quot;}"/>
+            <filter val="{&quot;species&quot;: &quot;Escherichia coli K12&quot;, &quot;species_component&quot;: &quot;P0A796&quot;, &quot;value&quot;: 12, &quot;units&quot;: &quot;U/mg&quot;, &quot;comments&quot;: &quot;SABIO-RK entry #21873.&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;]}"/>
+            <filter val="{&quot;species&quot;: &quot;Escherichia coli K12&quot;, &quot;species_component&quot;: &quot;P0A796&quot;, &quot;value&quot;: 30.6, &quot;units&quot;: &quot;U/mg&quot;, &quot;comments&quot;: &quot;SABIO-RK entry #21872.&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;]}"/>
+          </mc:Fallback>
+        </mc:AlternateContent>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
@@ -14797,9 +15341,9 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -14919,6 +15463,90 @@
         <v>815332823</v>
       </c>
     </row>
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>1314</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>1355</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>1196</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>1356</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>1338</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>1345</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>1196</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>1339</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>1346</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>1196</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>1353</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>1342</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>1347</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>1196</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>1352</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>1343</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>1348</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>1196</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>1351</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>1344</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>1349</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>1354</v>
+      </c>
+      <c r="D13" s="4">
+        <v>33184</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
fitting metabolite enzyme kinetics
</commit_message>
<xml_diff>
--- a/data/Model.xlsx
+++ b/data/Model.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="989" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="989" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Submodels" sheetId="1" r:id="rId1"/>
@@ -4010,9 +4010,6 @@
     <t>Vmax: 220 1/s [Ref-0007].</t>
   </si>
   <si>
-    <t>Vmax: 0.105 U/mg [Ref-0007].</t>
-  </si>
-  <si>
     <t>Vmax: 10.48 1/s [Ref-0007].</t>
   </si>
   <si>
@@ -4122,6 +4119,9 @@
   </si>
   <si>
     <t>10.1007/11799511_9</t>
+  </si>
+  <si>
+    <t>Vmax: Fit to 27.3 1/s, observed 105 U/mg [Ref-0007].</t>
   </si>
 </sst>
 </file>
@@ -4736,7 +4736,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O167"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -9878,14 +9878,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:K177"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A170" sqref="A170"/>
-      <selection pane="bottomRight" activeCell="K28" sqref="K28"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9969,7 +9968,7 @@
         <v>1315</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>565</v>
       </c>
@@ -9992,7 +9991,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>568</v>
       </c>
@@ -10047,7 +10046,7 @@
         <v>1316</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>576</v>
       </c>
@@ -10067,7 +10066,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>580</v>
       </c>
@@ -10087,7 +10086,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>584</v>
       </c>
@@ -10107,7 +10106,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>587</v>
       </c>
@@ -10127,7 +10126,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>590</v>
       </c>
@@ -10147,7 +10146,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>593</v>
       </c>
@@ -10167,7 +10166,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>596</v>
       </c>
@@ -10187,7 +10186,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>600</v>
       </c>
@@ -10207,7 +10206,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>603</v>
       </c>
@@ -10227,7 +10226,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>606</v>
       </c>
@@ -10247,7 +10246,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>609</v>
       </c>
@@ -10267,7 +10266,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>612</v>
       </c>
@@ -10287,7 +10286,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>615</v>
       </c>
@@ -10307,7 +10306,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>618</v>
       </c>
@@ -10327,7 +10326,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>621</v>
       </c>
@@ -10347,7 +10346,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>624</v>
       </c>
@@ -10367,7 +10366,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>627</v>
       </c>
@@ -10387,7 +10386,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>630</v>
       </c>
@@ -10407,7 +10406,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>633</v>
       </c>
@@ -10427,7 +10426,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>636</v>
       </c>
@@ -10508,7 +10507,7 @@
         <v>646</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -10540,7 +10539,7 @@
         <v>650</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -10595,7 +10594,7 @@
         <v>1288</v>
       </c>
       <c r="G30" s="5">
-        <v>0.105</v>
+        <v>27.3</v>
       </c>
       <c r="I30" s="4" t="s">
         <v>563</v>
@@ -10604,7 +10603,7 @@
         <v>658</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>1319</v>
+        <v>1356</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -10636,7 +10635,7 @@
         <v>662</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -10668,7 +10667,7 @@
         <v>666</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -10700,7 +10699,7 @@
         <v>670</v>
       </c>
       <c r="K33" s="4" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -10732,7 +10731,7 @@
         <v>674</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -10764,7 +10763,7 @@
         <v>674</v>
       </c>
       <c r="K35" s="4" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -10796,7 +10795,7 @@
         <v>674</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -10828,7 +10827,7 @@
         <v>684</v>
       </c>
       <c r="K37" s="4" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -10860,7 +10859,7 @@
         <v>688</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -10892,7 +10891,7 @@
         <v>688</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -10924,10 +10923,10 @@
         <v>695</v>
       </c>
       <c r="K40" s="4" t="s">
-        <v>1329</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>696</v>
       </c>
@@ -10979,7 +10978,7 @@
         <v>703</v>
       </c>
       <c r="K42" s="4" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -11011,7 +11010,7 @@
         <v>703</v>
       </c>
       <c r="K43" s="4" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -11043,10 +11042,10 @@
         <v>703</v>
       </c>
       <c r="K44" s="4" t="s">
-        <v>1332</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1331</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>710</v>
       </c>
@@ -11098,7 +11097,7 @@
         <v>716</v>
       </c>
       <c r="K46" s="4" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -11130,10 +11129,10 @@
         <v>720</v>
       </c>
       <c r="K47" s="4" t="s">
-        <v>1334</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1333</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>721</v>
       </c>
@@ -11153,7 +11152,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>725</v>
       </c>
@@ -11176,7 +11175,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>729</v>
       </c>
@@ -11199,7 +11198,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>733</v>
       </c>
@@ -11251,7 +11250,7 @@
         <v>739</v>
       </c>
       <c r="K52" s="4" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
     </row>
     <row r="53" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -11283,7 +11282,7 @@
         <v>739</v>
       </c>
       <c r="K53" s="4" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
     </row>
     <row r="54" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -11315,10 +11314,10 @@
         <v>746</v>
       </c>
       <c r="K54" s="4" t="s">
-        <v>1337</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1336</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>747</v>
       </c>
@@ -11341,7 +11340,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>751</v>
       </c>
@@ -11364,7 +11363,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>755</v>
       </c>
@@ -11378,7 +11377,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>758</v>
       </c>
@@ -11392,7 +11391,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>761</v>
       </c>
@@ -11406,7 +11405,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>764</v>
       </c>
@@ -11420,7 +11419,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>767</v>
       </c>
@@ -11434,7 +11433,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>770</v>
       </c>
@@ -11457,7 +11456,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="63" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>774</v>
       </c>
@@ -11471,7 +11470,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="64" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>777</v>
       </c>
@@ -11485,7 +11484,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>780</v>
       </c>
@@ -11499,7 +11498,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>783</v>
       </c>
@@ -11513,7 +11512,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>786</v>
       </c>
@@ -11536,7 +11535,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>790</v>
       </c>
@@ -11559,7 +11558,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>793</v>
       </c>
@@ -11582,7 +11581,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>796</v>
       </c>
@@ -11605,7 +11604,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
         <v>799</v>
       </c>
@@ -11628,7 +11627,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>802</v>
       </c>
@@ -11651,7 +11650,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="73" spans="1:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>805</v>
       </c>
@@ -11674,7 +11673,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>808</v>
       </c>
@@ -11697,7 +11696,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>811</v>
       </c>
@@ -11720,7 +11719,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>814</v>
       </c>
@@ -11743,7 +11742,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>817</v>
       </c>
@@ -11766,7 +11765,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>820</v>
       </c>
@@ -11789,7 +11788,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="79" spans="1:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>823</v>
       </c>
@@ -11812,7 +11811,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>826</v>
       </c>
@@ -11835,7 +11834,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="81" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>829</v>
       </c>
@@ -11858,7 +11857,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="82" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>832</v>
       </c>
@@ -11881,7 +11880,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="83" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
         <v>835</v>
       </c>
@@ -11904,7 +11903,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="84" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
         <v>838</v>
       </c>
@@ -11927,7 +11926,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="85" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
         <v>841</v>
       </c>
@@ -11950,7 +11949,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="86" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
         <v>844</v>
       </c>
@@ -11973,7 +11972,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="87" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
         <v>847</v>
       </c>
@@ -12008,7 +12007,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="88" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
         <v>852</v>
       </c>
@@ -12043,7 +12042,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="89" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
         <v>855</v>
       </c>
@@ -12078,7 +12077,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="90" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
         <v>858</v>
       </c>
@@ -12113,7 +12112,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="91" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
         <v>861</v>
       </c>
@@ -12148,7 +12147,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="92" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
         <v>864</v>
       </c>
@@ -12183,7 +12182,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="93" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
         <v>867</v>
       </c>
@@ -12218,7 +12217,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="94" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
         <v>870</v>
       </c>
@@ -12253,7 +12252,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="95" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
         <v>873</v>
       </c>
@@ -12288,7 +12287,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="96" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
         <v>876</v>
       </c>
@@ -12323,7 +12322,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="97" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
         <v>879</v>
       </c>
@@ -12358,7 +12357,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="98" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
         <v>882</v>
       </c>
@@ -12393,7 +12392,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="99" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
         <v>885</v>
       </c>
@@ -12428,7 +12427,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="100" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
         <v>888</v>
       </c>
@@ -12463,7 +12462,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="101" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
         <v>891</v>
       </c>
@@ -12498,7 +12497,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="102" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
         <v>894</v>
       </c>
@@ -12533,7 +12532,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="103" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
         <v>897</v>
       </c>
@@ -12568,7 +12567,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="104" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
         <v>900</v>
       </c>
@@ -12603,7 +12602,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="105" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
         <v>903</v>
       </c>
@@ -12638,7 +12637,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="106" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
         <v>906</v>
       </c>
@@ -12673,7 +12672,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="107" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
         <v>909</v>
       </c>
@@ -12708,7 +12707,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="108" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
         <v>912</v>
       </c>
@@ -12743,7 +12742,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="109" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
         <v>915</v>
       </c>
@@ -12778,7 +12777,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="110" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
         <v>918</v>
       </c>
@@ -12813,7 +12812,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="111" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
         <v>921</v>
       </c>
@@ -12848,7 +12847,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="112" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
         <v>924</v>
       </c>
@@ -12883,7 +12882,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="113" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
         <v>927</v>
       </c>
@@ -12918,7 +12917,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="114" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
         <v>930</v>
       </c>
@@ -12953,7 +12952,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="115" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
         <v>933</v>
       </c>
@@ -12988,7 +12987,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="116" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
         <v>936</v>
       </c>
@@ -13023,7 +13022,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="117" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
         <v>939</v>
       </c>
@@ -13058,7 +13057,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="118" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
         <v>944</v>
       </c>
@@ -13093,7 +13092,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="119" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
         <v>948</v>
       </c>
@@ -13128,7 +13127,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="120" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
         <v>952</v>
       </c>
@@ -13163,7 +13162,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="121" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="s">
         <v>956</v>
       </c>
@@ -13198,7 +13197,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="122" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
         <v>960</v>
       </c>
@@ -13233,7 +13232,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="123" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="s">
         <v>964</v>
       </c>
@@ -13268,7 +13267,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="124" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="s">
         <v>968</v>
       </c>
@@ -13303,7 +13302,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="125" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="s">
         <v>972</v>
       </c>
@@ -13338,7 +13337,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="126" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="s">
         <v>976</v>
       </c>
@@ -13373,7 +13372,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="127" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="s">
         <v>980</v>
       </c>
@@ -13408,7 +13407,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="128" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="s">
         <v>984</v>
       </c>
@@ -13443,7 +13442,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="129" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="4" t="s">
         <v>988</v>
       </c>
@@ -13478,7 +13477,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="130" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="s">
         <v>992</v>
       </c>
@@ -13513,7 +13512,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="131" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="4" t="s">
         <v>996</v>
       </c>
@@ -13548,7 +13547,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="132" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="s">
         <v>1000</v>
       </c>
@@ -13583,7 +13582,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="133" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="4" t="s">
         <v>1004</v>
       </c>
@@ -13618,7 +13617,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="134" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="4" t="s">
         <v>1008</v>
       </c>
@@ -13653,7 +13652,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="135" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="4" t="s">
         <v>1012</v>
       </c>
@@ -13688,7 +13687,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="136" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="4" t="s">
         <v>1016</v>
       </c>
@@ -13723,7 +13722,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="137" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="4" t="s">
         <v>1020</v>
       </c>
@@ -13758,7 +13757,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="138" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="4" t="s">
         <v>1024</v>
       </c>
@@ -13793,7 +13792,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="139" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="4" t="s">
         <v>1028</v>
       </c>
@@ -13828,7 +13827,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="140" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="4" t="s">
         <v>1032</v>
       </c>
@@ -13863,7 +13862,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="141" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="4" t="s">
         <v>1036</v>
       </c>
@@ -13898,7 +13897,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="142" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="4" t="s">
         <v>1040</v>
       </c>
@@ -13933,7 +13932,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="143" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="4" t="s">
         <v>1044</v>
       </c>
@@ -13968,7 +13967,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="144" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="4" t="s">
         <v>1048</v>
       </c>
@@ -14003,7 +14002,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="145" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="4" t="s">
         <v>1052</v>
       </c>
@@ -14038,7 +14037,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="146" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="4" t="s">
         <v>1056</v>
       </c>
@@ -14073,7 +14072,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="147" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="4" t="s">
         <v>1060</v>
       </c>
@@ -14108,7 +14107,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="148" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="4" t="s">
         <v>1065</v>
       </c>
@@ -14143,7 +14142,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="149" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="4" t="s">
         <v>1069</v>
       </c>
@@ -14178,7 +14177,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="150" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="4" t="s">
         <v>1073</v>
       </c>
@@ -14213,7 +14212,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="151" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="4" t="s">
         <v>1077</v>
       </c>
@@ -14248,7 +14247,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="152" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="4" t="s">
         <v>1081</v>
       </c>
@@ -14283,7 +14282,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="153" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="4" t="s">
         <v>1085</v>
       </c>
@@ -14318,7 +14317,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="154" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="4" t="s">
         <v>1089</v>
       </c>
@@ -14353,7 +14352,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="155" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="4" t="s">
         <v>1093</v>
       </c>
@@ -14388,7 +14387,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="156" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="4" t="s">
         <v>1097</v>
       </c>
@@ -14423,7 +14422,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="157" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="4" t="s">
         <v>1101</v>
       </c>
@@ -14458,7 +14457,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="158" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="4" t="s">
         <v>1105</v>
       </c>
@@ -14493,7 +14492,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="159" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="4" t="s">
         <v>1109</v>
       </c>
@@ -14528,7 +14527,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="160" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="4" t="s">
         <v>1113</v>
       </c>
@@ -14563,7 +14562,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="161" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="4" t="s">
         <v>1117</v>
       </c>
@@ -14598,7 +14597,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="162" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="4" t="s">
         <v>1121</v>
       </c>
@@ -14633,7 +14632,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="163" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="4" t="s">
         <v>1125</v>
       </c>
@@ -14668,7 +14667,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="164" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="4" t="s">
         <v>1129</v>
       </c>
@@ -14703,7 +14702,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="165" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="4" t="s">
         <v>1133</v>
       </c>
@@ -14738,7 +14737,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="166" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="4" t="s">
         <v>1137</v>
       </c>
@@ -14773,7 +14772,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="167" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="4" t="s">
         <v>1141</v>
       </c>
@@ -14808,7 +14807,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="168" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="4" t="s">
         <v>1145</v>
       </c>
@@ -14843,7 +14842,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="169" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="4" t="s">
         <v>1149</v>
       </c>
@@ -14878,7 +14877,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="170" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="4" t="s">
         <v>1153</v>
       </c>
@@ -14913,7 +14912,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="171" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="4" t="s">
         <v>1157</v>
       </c>
@@ -14948,7 +14947,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="172" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="4" t="s">
         <v>1161</v>
       </c>
@@ -14983,7 +14982,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="173" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="4" t="s">
         <v>1165</v>
       </c>
@@ -15018,7 +15017,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="174" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="4" t="s">
         <v>1169</v>
       </c>
@@ -15053,7 +15052,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="175" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="4" t="s">
         <v>1173</v>
       </c>
@@ -15088,7 +15087,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="176" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="4" t="s">
         <v>1177</v>
       </c>
@@ -15123,7 +15122,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="177" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="4" t="s">
         <v>1181</v>
       </c>
@@ -15138,66 +15137,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" ref="A1:K177">
-    <filterColumn colId="10">
-      <filters>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <x14:filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;0.105&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #30207&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;U/mg&quot;, &quot;species&quot;: &quot;Rattus norvegicus&quot;}"/>
-            <x14:filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;1.58&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #15484&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;U/mg&quot;, &quot;species&quot;: &quot;Homo sapiens&quot;}"/>
-            <x14:filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;10.48&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #10179&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;1/s&quot;, &quot;species&quot;: &quot;Homo sapiens&quot;}"/>
-            <x14:filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;1247&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #13276&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;U/mg&quot;, &quot;species&quot;: &quot;Escherichia coli&quot;}"/>
-            <x14:filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;1480&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #22933&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;1/s&quot;, &quot;species&quot;: &quot;Escherichia coli&quot;}"/>
-            <x14:filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;1511&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #32322&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;U/mg&quot;, &quot;species&quot;: &quot;Escherichia coli&quot;}"/>
-            <x14:filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;160&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #9571&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;1/s&quot;, &quot;species&quot;: &quot;Escherichia coli&quot;}"/>
-            <x14:filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;167&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #36109&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;1/s&quot;, &quot;species&quot;: &quot;Escherichia coli&quot;}"/>
-            <x14:filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;180&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #7357&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;U/mg&quot;, &quot;species&quot;: &quot;Escherichia coli&quot;}"/>
-            <x14:filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;2&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #28897&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;1/s&quot;, &quot;species&quot;: &quot;Escherichia coli&quot;}"/>
-            <x14:filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;200&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #24532&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;U/mg&quot;, &quot;species&quot;: &quot;Streptococcus mutans&quot;}"/>
-            <x14:filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;21667.0&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #26928&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;1/min&quot;, &quot;species&quot;: &quot;Enterococcus faecalis&quot;}"/>
-            <x14:filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;220&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #16538&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;U/mg&quot;, &quot;species&quot;: &quot;Lactobacillus curvatus&quot;}"/>
-            <x14:filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;220&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #27646&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;1/s&quot;, &quot;species&quot;: &quot;Escherichia coli&quot;}"/>
-            <x14:filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;250&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #17213&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;U/mg&quot;, &quot;species&quot;: &quot;Escherichia coli&quot;}"/>
-            <x14:filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;340&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #21262&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;U/mg&quot;, &quot;species&quot;: &quot;Saccharomyces cerevisiae&quot;}"/>
-            <x14:filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;3550&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #224&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;1/s&quot;, &quot;species&quot;: &quot;Streptococcus gordonii&quot;}"/>
-            <x14:filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;47&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #45990&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;U/mg&quot;, &quot;species&quot;: &quot;Escherichia coli&quot;}"/>
-            <x14:filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;52&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #40418&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;U/mg&quot;, &quot;species&quot;: &quot;Bacillus subtilis&quot;}"/>
-            <x14:filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;6.5&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #39676&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;U/mg&quot;, &quot;species&quot;: &quot;Homo sapiens&quot;}"/>
-            <x14:filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;69&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #24910&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;1/s&quot;, &quot;species&quot;: &quot;Escherichia coli&quot;}"/>
-            <x14:filter val="{&quot;species&quot;: &quot;Escherichia coli K12&quot;, &quot;species_component&quot;: &quot;P0A796&quot;, &quot;value&quot;: 12, &quot;units&quot;: &quot;U/mg&quot;, &quot;comments&quot;: &quot;SABIO-RK entry #21873.&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;]}"/>
-            <x14:filter val="{&quot;species&quot;: &quot;Escherichia coli K12&quot;, &quot;species_component&quot;: &quot;P0A796&quot;, &quot;value&quot;: 30.6, &quot;units&quot;: &quot;U/mg&quot;, &quot;comments&quot;: &quot;SABIO-RK entry #21872.&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;]}"/>
-            <x14:filter val="{&quot;value&quot;: 16.76, &quot;units&quot;: &quot;1/s&quot;, &quot;is_experimentally_constrained&quot;: true, &quot;species&quot;: &quot;Staphylococcus carnosus&quot;, &quot;references&quot;: [&quot;PUB_1177&quot;]},_x000a_{&quot;value&quot;: 1820, &quot;units&quot;: &quot;1/min&quot;, &quot;is_experimentally_constrained&quot;: true, &quot;species&quot;: &quot;Escherichia coli&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #343243&quot;, &quot;references&quot;: [&quot;PUB_1176&quot;]}"/>
-            <x14:filter val="{&quot;value&quot;: 70, &quot;units&quot;: &quot;1/s&quot;, &quot;is_experimentally_constrained&quot;: true, &quot;species&quot;: &quot;Lactococcus lactis subsp. lactis&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #20212&quot;, &quot;references&quot;: [&quot;PUB_1186&quot;]},_x000a_{&quot;value&quot;: 112, &quot;units&quot;: &quot;1/s&quot;, &quot;is_experimentally_constrained&quot;: true, &quot;species&quot;: &quot;Geobacillus stearothermophilus&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #43582&quot;, &quot;references&quot;: [&quot;PUB_1185&quot;]},_x000a_{&quot;value&quot;: 305, &quot;units&quot;: &quot;U/mg&quot;, &quot;is_experimentally_constrained&quot;: true, &quot;species&quot;: &quot;Streptococcus mutans&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #20980&quot;, &quot;references&quot;: [&quot;PUB_1187&quot;]},_x000a_{&quot;value&quot;: 0.12, &quot;units&quot;: &quot;1/s&quot;, &quot;is_experimentally_constrained&quot;: true, &quot;species&quot;: &quot;Escherichia coli&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #37150&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;]}"/>
-          </mc:Choice>
-          <mc:Fallback>
-            <filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;0.105&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #30207&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;U/mg&quot;, &quot;species&quot;: &quot;Rattus norvegicus&quot;}"/>
-            <filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;1.58&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #15484&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;U/mg&quot;, &quot;species&quot;: &quot;Homo sapiens&quot;}"/>
-            <filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;10.48&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #10179&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;1/s&quot;, &quot;species&quot;: &quot;Homo sapiens&quot;}"/>
-            <filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;1247&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #13276&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;U/mg&quot;, &quot;species&quot;: &quot;Escherichia coli&quot;}"/>
-            <filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;1480&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #22933&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;1/s&quot;, &quot;species&quot;: &quot;Escherichia coli&quot;}"/>
-            <filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;1511&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #32322&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;U/mg&quot;, &quot;species&quot;: &quot;Escherichia coli&quot;}"/>
-            <filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;160&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #9571&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;1/s&quot;, &quot;species&quot;: &quot;Escherichia coli&quot;}"/>
-            <filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;167&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #36109&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;1/s&quot;, &quot;species&quot;: &quot;Escherichia coli&quot;}"/>
-            <filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;180&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #7357&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;U/mg&quot;, &quot;species&quot;: &quot;Escherichia coli&quot;}"/>
-            <filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;2&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #28897&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;1/s&quot;, &quot;species&quot;: &quot;Escherichia coli&quot;}"/>
-            <filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;200&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #24532&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;U/mg&quot;, &quot;species&quot;: &quot;Streptococcus mutans&quot;}"/>
-            <filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;21667.0&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #26928&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;1/min&quot;, &quot;species&quot;: &quot;Enterococcus faecalis&quot;}"/>
-            <filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;220&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #16538&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;U/mg&quot;, &quot;species&quot;: &quot;Lactobacillus curvatus&quot;}"/>
-            <filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;220&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #27646&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;1/s&quot;, &quot;species&quot;: &quot;Escherichia coli&quot;}"/>
-            <filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;250&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #17213&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;U/mg&quot;, &quot;species&quot;: &quot;Escherichia coli&quot;}"/>
-            <filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;340&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #21262&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;U/mg&quot;, &quot;species&quot;: &quot;Saccharomyces cerevisiae&quot;}"/>
-            <filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;3550&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #224&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;1/s&quot;, &quot;species&quot;: &quot;Streptococcus gordonii&quot;}"/>
-            <filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;47&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #45990&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;U/mg&quot;, &quot;species&quot;: &quot;Escherichia coli&quot;}"/>
-            <filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;52&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #40418&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;U/mg&quot;, &quot;species&quot;: &quot;Bacillus subtilis&quot;}"/>
-            <filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;6.5&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #39676&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;U/mg&quot;, &quot;species&quot;: &quot;Homo sapiens&quot;}"/>
-            <filter val="{&quot;is_experimentally_constrained&quot;: true, &quot;value&quot;: &quot;69&quot;, &quot;comments&quot;: &quot;Sabio-RK entry #24910&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;], &quot;units&quot;: &quot;1/s&quot;, &quot;species&quot;: &quot;Escherichia coli&quot;}"/>
-            <filter val="{&quot;species&quot;: &quot;Escherichia coli K12&quot;, &quot;species_component&quot;: &quot;P0A796&quot;, &quot;value&quot;: 12, &quot;units&quot;: &quot;U/mg&quot;, &quot;comments&quot;: &quot;SABIO-RK entry #21873.&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;]}"/>
-            <filter val="{&quot;species&quot;: &quot;Escherichia coli K12&quot;, &quot;species_component&quot;: &quot;P0A796&quot;, &quot;value&quot;: 30.6, &quot;units&quot;: &quot;U/mg&quot;, &quot;comments&quot;: &quot;SABIO-RK entry #21872.&quot;, &quot;references&quot;: [&quot;PUB_0100&quot;]}"/>
-          </mc:Fallback>
-        </mc:AlternateContent>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:K177"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
@@ -15468,80 +15408,80 @@
         <v>1314</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>1196</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>1196</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>1196</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>1196</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>1196</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="D13" s="4">
         <v>33184</v>

</xml_diff>

<commit_message>
deleting junk, removing filter
</commit_message>
<xml_diff>
--- a/data/Model.xlsx
+++ b/data/Model.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="470" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="470" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Submodels" sheetId="1" r:id="rId1"/>
@@ -13,14 +13,12 @@
     <sheet name="Reactions" sheetId="4" r:id="rId4"/>
     <sheet name="Parameters" sheetId="5" r:id="rId5"/>
     <sheet name="References" sheetId="6" r:id="rId6"/>
-    <sheet name="Sheet1" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1">Compartments!$A$1:$C$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4">Parameters!$A$1:$F$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Reactions!$A$1:$K$177</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5">References!$A$1:$E$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Sheet1!$A$2:$CD$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Species!$A$1:$O$167</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">Submodels!$A$1:$C$5</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="1">Compartments!$A$1:$C$3</definedName>
@@ -53,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2804" uniqueCount="1397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2627" uniqueCount="1380">
   <si>
     <t>ID</t>
   </si>
@@ -4192,58 +4190,7 @@
     <t>Media concentration set according to ~5% CO2 = 38 mmHg [Ref-0019]. Equilbrium constant of solvation is 29.49 L*atm/mol [Ref-0019].</t>
   </si>
   <si>
-    <t>source</t>
-  </si>
-  <si>
-    <t xml:space="preserve">: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">, </t>
-  </si>
-  <si>
-    <t>xid</t>
-  </si>
-  <si>
-    <t>}, {</t>
-  </si>
-  <si>
     <t>PubChem</t>
-  </si>
-  <si>
-    <t>CAS</t>
-  </si>
-  <si>
-    <t>KEGG</t>
-  </si>
-  <si>
-    <t>}</t>
-  </si>
-  <si>
-    <t>15483-27-9</t>
-  </si>
-  <si>
-    <t>3929-61-1</t>
-  </si>
-  <si>
-    <t>C01425</t>
-  </si>
-  <si>
-    <t>3303-31-9</t>
-  </si>
-  <si>
-    <t>13184-13-9</t>
-  </si>
-  <si>
-    <t>6620-95-7</t>
-  </si>
-  <si>
-    <t>20696-60-0</t>
-  </si>
-  <si>
-    <t>1050-28-8</t>
-  </si>
-  <si>
-    <t>3918-94-3</t>
   </si>
 </sst>
 </file>
@@ -4865,7 +4812,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O167"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="I104" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -8494,7 +8441,7 @@
         <v>4381318144000.0005</v>
       </c>
       <c r="M101" s="4" t="s">
-        <v>1384</v>
+        <v>1379</v>
       </c>
       <c r="N101" s="4">
         <v>6197512</v>
@@ -8532,7 +8479,7 @@
         <v>1839985968000</v>
       </c>
       <c r="M102" s="4" t="s">
-        <v>1384</v>
+        <v>1379</v>
       </c>
       <c r="N102" s="4">
         <v>77638054</v>
@@ -8570,7 +8517,7 @@
         <v>120440000000.00002</v>
       </c>
       <c r="M103" s="4" t="s">
-        <v>1384</v>
+        <v>1379</v>
       </c>
       <c r="N103" s="4">
         <v>28724627</v>
@@ -8608,7 +8555,7 @@
         <v>4708975164000</v>
       </c>
       <c r="M104" s="4" t="s">
-        <v>1384</v>
+        <v>1379</v>
       </c>
       <c r="N104" s="4">
         <v>10306892</v>
@@ -8780,7 +8727,7 @@
         <v>1915821014000</v>
       </c>
       <c r="M109" s="4" t="s">
-        <v>1384</v>
+        <v>1379</v>
       </c>
       <c r="N109" s="4">
         <v>10251455</v>
@@ -9216,7 +9163,7 @@
         <v>8116210720000.001</v>
       </c>
       <c r="M123" s="4" t="s">
-        <v>1384</v>
+        <v>1379</v>
       </c>
       <c r="N123" s="4">
         <v>4610</v>
@@ -9321,7 +9268,7 @@
         <v>1437174388000</v>
       </c>
       <c r="M126" s="4" t="s">
-        <v>1384</v>
+        <v>1379</v>
       </c>
       <c r="N126" s="4">
         <v>51795710</v>
@@ -9507,7 +9454,7 @@
         <v>4708764394000.001</v>
       </c>
       <c r="M132" s="4" t="s">
-        <v>1384</v>
+        <v>1379</v>
       </c>
       <c r="N132" s="4">
         <v>8198360</v>
@@ -9545,7 +9492,7 @@
         <v>3795762952000</v>
       </c>
       <c r="M133" s="4" t="s">
-        <v>1384</v>
+        <v>1379</v>
       </c>
       <c r="N133" s="4">
         <v>10242166</v>
@@ -9612,7 +9559,7 @@
         <v>1080930934000</v>
       </c>
       <c r="M135" s="4" t="s">
-        <v>1384</v>
+        <v>1379</v>
       </c>
       <c r="N135" s="4">
         <v>10233351</v>
@@ -9967,7 +9914,7 @@
         <v>2049798470000</v>
       </c>
       <c r="M146" s="4" t="s">
-        <v>1384</v>
+        <v>1379</v>
       </c>
       <c r="N146" s="4">
         <v>8189514</v>
@@ -10153,7 +10100,7 @@
         <v>3237487420000</v>
       </c>
       <c r="M152" s="4" t="s">
-        <v>1384</v>
+        <v>1379</v>
       </c>
       <c r="N152" s="4">
         <v>10246126</v>
@@ -10368,7 +10315,7 @@
         <v>188589769600</v>
       </c>
       <c r="M159" s="4" t="s">
-        <v>1384</v>
+        <v>1379</v>
       </c>
       <c r="N159" s="4">
         <v>8888253</v>
@@ -10406,7 +10353,7 @@
         <v>677794166000</v>
       </c>
       <c r="M160" s="4" t="s">
-        <v>1384</v>
+        <v>1379</v>
       </c>
       <c r="N160" s="4">
         <v>8546048</v>
@@ -10569,7 +10516,7 @@
         <v>3535522222000</v>
       </c>
       <c r="M165" s="4" t="s">
-        <v>1384</v>
+        <v>1379</v>
       </c>
       <c r="N165" s="4">
         <v>10285797</v>
@@ -10621,14 +10568,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:K177"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="C73" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A170" sqref="A170"/>
-      <selection pane="bottomRight" activeCell="K31" sqref="K31"/>
+      <selection pane="bottomRight" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -10680,7 +10626,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>560</v>
       </c>
@@ -10712,7 +10658,7 @@
         <v>1315</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>565</v>
       </c>
@@ -10735,7 +10681,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>568</v>
       </c>
@@ -10758,7 +10704,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>572</v>
       </c>
@@ -10790,7 +10736,7 @@
         <v>1316</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>576</v>
       </c>
@@ -10810,7 +10756,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>580</v>
       </c>
@@ -10830,7 +10776,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>584</v>
       </c>
@@ -10850,7 +10796,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>587</v>
       </c>
@@ -10870,7 +10816,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>590</v>
       </c>
@@ -10890,7 +10836,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>593</v>
       </c>
@@ -10910,7 +10856,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>596</v>
       </c>
@@ -10930,7 +10876,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>600</v>
       </c>
@@ -10950,7 +10896,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>603</v>
       </c>
@@ -10970,7 +10916,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>606</v>
       </c>
@@ -10990,7 +10936,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>609</v>
       </c>
@@ -11010,7 +10956,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>612</v>
       </c>
@@ -11030,7 +10976,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>615</v>
       </c>
@@ -11050,7 +10996,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>618</v>
       </c>
@@ -11070,7 +11016,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>621</v>
       </c>
@@ -11090,7 +11036,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>624</v>
       </c>
@@ -11110,7 +11056,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>627</v>
       </c>
@@ -11130,7 +11076,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>630</v>
       </c>
@@ -11150,7 +11096,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>633</v>
       </c>
@@ -11170,7 +11116,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>636</v>
       </c>
@@ -11190,7 +11136,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>639</v>
       </c>
@@ -11222,7 +11168,7 @@
         <v>1317</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>643</v>
       </c>
@@ -11254,7 +11200,7 @@
         <v>1339</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>647</v>
       </c>
@@ -11286,7 +11232,7 @@
         <v>1340</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>651</v>
       </c>
@@ -11318,7 +11264,7 @@
         <v>1318</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>655</v>
       </c>
@@ -11350,7 +11296,7 @@
         <v>1356</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>659</v>
       </c>
@@ -11382,7 +11328,7 @@
         <v>1319</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>663</v>
       </c>
@@ -11414,7 +11360,7 @@
         <v>1320</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>667</v>
       </c>
@@ -11446,7 +11392,7 @@
         <v>1321</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>671</v>
       </c>
@@ -11478,7 +11424,7 @@
         <v>1322</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>675</v>
       </c>
@@ -11510,7 +11456,7 @@
         <v>1323</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>678</v>
       </c>
@@ -11542,7 +11488,7 @@
         <v>1324</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>681</v>
       </c>
@@ -11574,7 +11520,7 @@
         <v>1325</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>685</v>
       </c>
@@ -11606,7 +11552,7 @@
         <v>1326</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>689</v>
       </c>
@@ -11638,7 +11584,7 @@
         <v>1327</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>692</v>
       </c>
@@ -11670,7 +11616,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>696</v>
       </c>
@@ -11693,7 +11639,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>700</v>
       </c>
@@ -11725,7 +11671,7 @@
         <v>1329</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>704</v>
       </c>
@@ -11757,7 +11703,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>707</v>
       </c>
@@ -11789,7 +11735,7 @@
         <v>1331</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>710</v>
       </c>
@@ -11812,7 +11758,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>713</v>
       </c>
@@ -11844,7 +11790,7 @@
         <v>1332</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>717</v>
       </c>
@@ -11876,7 +11822,7 @@
         <v>1333</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>721</v>
       </c>
@@ -11896,7 +11842,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>725</v>
       </c>
@@ -11919,7 +11865,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>729</v>
       </c>
@@ -11942,7 +11888,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>733</v>
       </c>
@@ -11965,7 +11911,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>736</v>
       </c>
@@ -11997,7 +11943,7 @@
         <v>1334</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>740</v>
       </c>
@@ -12029,7 +11975,7 @@
         <v>1335</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>743</v>
       </c>
@@ -12061,7 +12007,7 @@
         <v>1336</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>747</v>
       </c>
@@ -12716,7 +12662,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="87" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
         <v>847</v>
       </c>
@@ -12751,7 +12697,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="88" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
         <v>852</v>
       </c>
@@ -12786,7 +12732,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="89" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
         <v>855</v>
       </c>
@@ -12821,7 +12767,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="90" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
         <v>858</v>
       </c>
@@ -12856,7 +12802,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="91" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
         <v>861</v>
       </c>
@@ -12891,7 +12837,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="92" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
         <v>864</v>
       </c>
@@ -12926,7 +12872,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="93" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
         <v>867</v>
       </c>
@@ -12961,7 +12907,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="94" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
         <v>870</v>
       </c>
@@ -12996,7 +12942,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="95" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
         <v>873</v>
       </c>
@@ -13031,7 +12977,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="96" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
         <v>876</v>
       </c>
@@ -13066,7 +13012,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="97" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
         <v>879</v>
       </c>
@@ -13101,7 +13047,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="98" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
         <v>882</v>
       </c>
@@ -13136,7 +13082,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="99" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
         <v>885</v>
       </c>
@@ -13171,7 +13117,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="100" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
         <v>888</v>
       </c>
@@ -13206,7 +13152,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="101" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
         <v>891</v>
       </c>
@@ -13241,7 +13187,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="102" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
         <v>894</v>
       </c>
@@ -13276,7 +13222,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="103" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
         <v>897</v>
       </c>
@@ -13311,7 +13257,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="104" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
         <v>900</v>
       </c>
@@ -13346,7 +13292,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="105" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
         <v>903</v>
       </c>
@@ -13381,7 +13327,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="106" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
         <v>906</v>
       </c>
@@ -13416,7 +13362,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="107" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
         <v>909</v>
       </c>
@@ -13451,7 +13397,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="108" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
         <v>912</v>
       </c>
@@ -13486,7 +13432,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="109" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
         <v>915</v>
       </c>
@@ -13521,7 +13467,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="110" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
         <v>918</v>
       </c>
@@ -13556,7 +13502,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="111" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
         <v>921</v>
       </c>
@@ -13591,7 +13537,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="112" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
         <v>924</v>
       </c>
@@ -13626,7 +13572,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="113" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
         <v>927</v>
       </c>
@@ -13661,7 +13607,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="114" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
         <v>930</v>
       </c>
@@ -13696,7 +13642,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="115" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
         <v>933</v>
       </c>
@@ -13731,7 +13677,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="116" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
         <v>936</v>
       </c>
@@ -13766,7 +13712,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="117" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
         <v>939</v>
       </c>
@@ -13801,7 +13747,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="118" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
         <v>944</v>
       </c>
@@ -13836,7 +13782,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="119" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
         <v>948</v>
       </c>
@@ -13871,7 +13817,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="120" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
         <v>952</v>
       </c>
@@ -13906,7 +13852,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="121" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="s">
         <v>956</v>
       </c>
@@ -13941,7 +13887,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="122" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
         <v>960</v>
       </c>
@@ -13976,7 +13922,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="123" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="s">
         <v>964</v>
       </c>
@@ -14011,7 +13957,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="124" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="s">
         <v>968</v>
       </c>
@@ -14046,7 +13992,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="125" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="s">
         <v>972</v>
       </c>
@@ -14081,7 +14027,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="126" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="s">
         <v>976</v>
       </c>
@@ -14116,7 +14062,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="127" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="s">
         <v>980</v>
       </c>
@@ -14151,7 +14097,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="128" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="s">
         <v>984</v>
       </c>
@@ -14186,7 +14132,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="129" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="4" t="s">
         <v>988</v>
       </c>
@@ -14221,7 +14167,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="130" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="s">
         <v>992</v>
       </c>
@@ -14256,7 +14202,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="131" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="4" t="s">
         <v>996</v>
       </c>
@@ -14291,7 +14237,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="132" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="s">
         <v>1000</v>
       </c>
@@ -14326,7 +14272,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="133" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="4" t="s">
         <v>1004</v>
       </c>
@@ -14361,7 +14307,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="134" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="4" t="s">
         <v>1008</v>
       </c>
@@ -14396,7 +14342,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="135" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="4" t="s">
         <v>1012</v>
       </c>
@@ -14431,7 +14377,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="136" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="4" t="s">
         <v>1016</v>
       </c>
@@ -14466,7 +14412,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="137" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="4" t="s">
         <v>1020</v>
       </c>
@@ -14501,7 +14447,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="138" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="4" t="s">
         <v>1024</v>
       </c>
@@ -14536,7 +14482,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="139" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="4" t="s">
         <v>1028</v>
       </c>
@@ -14571,7 +14517,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="140" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="4" t="s">
         <v>1032</v>
       </c>
@@ -14606,7 +14552,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="141" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="4" t="s">
         <v>1036</v>
       </c>
@@ -14641,7 +14587,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="142" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="4" t="s">
         <v>1040</v>
       </c>
@@ -14676,7 +14622,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="143" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="4" t="s">
         <v>1044</v>
       </c>
@@ -14711,7 +14657,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="144" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="4" t="s">
         <v>1048</v>
       </c>
@@ -14746,7 +14692,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="145" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="4" t="s">
         <v>1052</v>
       </c>
@@ -14781,7 +14727,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="146" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="4" t="s">
         <v>1056</v>
       </c>
@@ -14816,7 +14762,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="147" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="4" t="s">
         <v>1060</v>
       </c>
@@ -14851,7 +14797,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="148" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="4" t="s">
         <v>1065</v>
       </c>
@@ -14886,7 +14832,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="149" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="4" t="s">
         <v>1069</v>
       </c>
@@ -14921,7 +14867,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="150" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="4" t="s">
         <v>1073</v>
       </c>
@@ -14956,7 +14902,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="151" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="4" t="s">
         <v>1077</v>
       </c>
@@ -14991,7 +14937,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="152" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="4" t="s">
         <v>1081</v>
       </c>
@@ -15026,7 +14972,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="153" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="4" t="s">
         <v>1085</v>
       </c>
@@ -15061,7 +15007,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="154" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="4" t="s">
         <v>1089</v>
       </c>
@@ -15096,7 +15042,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="155" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="4" t="s">
         <v>1093</v>
       </c>
@@ -15131,7 +15077,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="156" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="4" t="s">
         <v>1097</v>
       </c>
@@ -15166,7 +15112,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="157" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="4" t="s">
         <v>1101</v>
       </c>
@@ -15201,7 +15147,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="158" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="4" t="s">
         <v>1105</v>
       </c>
@@ -15236,7 +15182,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="159" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="4" t="s">
         <v>1109</v>
       </c>
@@ -15271,7 +15217,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="160" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="4" t="s">
         <v>1113</v>
       </c>
@@ -15306,7 +15252,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="161" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="4" t="s">
         <v>1117</v>
       </c>
@@ -15341,7 +15287,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="162" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="4" t="s">
         <v>1121</v>
       </c>
@@ -15376,7 +15322,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="163" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="4" t="s">
         <v>1125</v>
       </c>
@@ -15411,7 +15357,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="164" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="4" t="s">
         <v>1129</v>
       </c>
@@ -15446,7 +15392,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="165" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="4" t="s">
         <v>1133</v>
       </c>
@@ -15481,7 +15427,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="166" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="4" t="s">
         <v>1137</v>
       </c>
@@ -15516,7 +15462,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="167" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="4" t="s">
         <v>1141</v>
       </c>
@@ -15551,7 +15497,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="168" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="4" t="s">
         <v>1145</v>
       </c>
@@ -15586,7 +15532,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="169" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="4" t="s">
         <v>1149</v>
       </c>
@@ -15621,7 +15567,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="170" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="4" t="s">
         <v>1153</v>
       </c>
@@ -15656,7 +15602,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="171" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="4" t="s">
         <v>1157</v>
       </c>
@@ -15691,7 +15637,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="172" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="4" t="s">
         <v>1161</v>
       </c>
@@ -15726,7 +15672,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="173" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="4" t="s">
         <v>1165</v>
       </c>
@@ -15761,7 +15707,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="174" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="4" t="s">
         <v>1169</v>
       </c>
@@ -15796,7 +15742,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="175" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="4" t="s">
         <v>1173</v>
       </c>
@@ -15831,7 +15777,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="176" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="4" t="s">
         <v>1177</v>
       </c>
@@ -15866,7 +15812,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="177" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="4" t="s">
         <v>1181</v>
       </c>
@@ -15881,43 +15827,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K177">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="AD[e] + H[e] &lt;==&gt; H[c] + AD[c]"/>
-        <filter val="AlaAla[e] + ATP[c] + H2O[c] ==&gt; PI[c] + H[c] + AlaAla[c] + ADP[c]"/>
-        <filter val="AspAsp[e] + ATP[c] + H2O[c] ==&gt; PI[c] + H[c] + ADP[c] + AspAsp[c]"/>
-        <filter val="ATP[c] + ArgArg[e] + H2O[c] ==&gt; ArgArg[c] + PI[c] + H[c] + ADP[c]"/>
-        <filter val="ATP[c] + AsnAsn[e] + H2O[c] ==&gt; PI[c] + H[c] + ADP[c] + AsnAsn[c]"/>
-        <filter val="ATP[c] + GluGlu[e] + H2O[c] ==&gt; PI[c] + H[c] + ADP[c] + GluGlu[c]"/>
-        <filter val="ATP[c] + LeuLeu[e] + H2O[c] ==&gt; PI[c] + H[c] + ADP[c] + LeuLeu[c]"/>
-        <filter val="ATP[c] + SerSer[e] + H2O[c] ==&gt; SerSer[c] + PI[c] + H[c] + ADP[c]"/>
-        <filter val="ATP[c] + TrpTrp[e] + H2O[c] ==&gt; TrpTrp[c] + PI[c] + H[c] + ADP[c]"/>
-        <filter val="ATP[c] + ValVal[e] + H2O[c] ==&gt; PI[c] + H[c] + ValVal[c] + ADP[c]"/>
-        <filter val="CO2[e] &lt;==&gt; CO2[c]"/>
-        <filter val="CysCys[e] + ATP[c] + H2O[c] ==&gt; CysCys[c] + PI[c] + H[c] + ADP[c]"/>
-        <filter val="GLC[e] + PEP[c] ==&gt; G6P[c] + PYR[c]"/>
-        <filter val="GlnGln[e] + ATP[c] + H2O[c] ==&gt; PI[c] + H[c] + ADP[c] + GlnGln[c]"/>
-        <filter val="GlyGly[e] + ATP[c] + H2O[c] ==&gt; PI[c] + H[c] + ADP[c] + GlyGly[c]"/>
-        <filter val="GN[e] + H[e] ==&gt; H[c] + GN[c]"/>
-        <filter val="H[c] + LAC[c] ==&gt; LAC[e] + H[e]"/>
-        <filter val="H[e] + CYTD[e] &lt;==&gt; H[c] + CYTD[c]"/>
-        <filter val="H[e] &lt;==&gt; H[c]"/>
-        <filter val="H2O[e] &lt;==&gt; H2O[c]"/>
-        <filter val="HisHis[e] + ATP[c] + H2O[c] ==&gt; PI[c] + H[c] + ADP[c] + HisHis[c]"/>
-        <filter val="IleIle[e] + ATP[c] + H2O[c] ==&gt; IleIle[c] + PI[c] + H[c] + ADP[c]"/>
-        <filter val="LysLys[e] + ATP[c] + H2O[c] ==&gt; PI[c] + LysLys[c] + H[c] + ADP[c]"/>
-        <filter val="MetMet[e] + ATP[c] + H2O[c] ==&gt; PI[c] + H[c] + MetMet[c] + ADP[c]"/>
-        <filter val="O2[e] &lt;==&gt; O2[c]"/>
-        <filter val="PhePhe[e] + ATP[c] + H2O[c] ==&gt; PhePhe[c] + PI[c] + H[c] + ADP[c]"/>
-        <filter val="PI[e] + ATP[c] + H2O[c] ==&gt; (2) PI[c] + H[c] + ADP[c]"/>
-        <filter val="ProPro[e] + ATP[c] + H2O[c] ==&gt; ProPro[c] + PI[c] + H[c] + ADP[c]"/>
-        <filter val="ThrThr[e] + ATP[c] + H2O[c] ==&gt; PI[c] + H[c] + ADP[c] + ThrThr[c]"/>
-        <filter val="TyrTyr[e] + ATP[c] + H2O[c] ==&gt; PI[c] + H[c] + TyrTyr[c] + ADP[c]"/>
-        <filter val="URA[e] + H[e] &lt;==&gt; URA[c] + H[c]"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:K177"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
@@ -16329,630 +16239,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:Z17"/>
-  <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>361</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1384</v>
-      </c>
-      <c r="C3">
-        <v>77638054</v>
-      </c>
-      <c r="D3" t="s">
-        <v>1380</v>
-      </c>
-      <c r="E3" t="s">
-        <v>1385</v>
-      </c>
-      <c r="F3" t="s">
-        <v>1381</v>
-      </c>
-      <c r="G3" t="s">
-        <v>1382</v>
-      </c>
-      <c r="H3" t="s">
-        <v>1380</v>
-      </c>
-      <c r="I3" t="s">
-        <v>1388</v>
-      </c>
-      <c r="J3" t="s">
-        <v>1383</v>
-      </c>
-      <c r="K3" t="s">
-        <v>1379</v>
-      </c>
-      <c r="L3" t="s">
-        <v>1380</v>
-      </c>
-      <c r="N3" t="s">
-        <v>1381</v>
-      </c>
-      <c r="O3" t="s">
-        <v>1382</v>
-      </c>
-      <c r="P3" t="s">
-        <v>1380</v>
-      </c>
-      <c r="R3" t="s">
-        <v>1387</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>423</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1384</v>
-      </c>
-      <c r="C4">
-        <v>4610</v>
-      </c>
-      <c r="D4" t="s">
-        <v>1380</v>
-      </c>
-      <c r="E4" t="s">
-        <v>1385</v>
-      </c>
-      <c r="F4" t="s">
-        <v>1381</v>
-      </c>
-      <c r="G4" t="s">
-        <v>1382</v>
-      </c>
-      <c r="H4" t="s">
-        <v>1380</v>
-      </c>
-      <c r="I4" t="s">
-        <v>1389</v>
-      </c>
-      <c r="J4" t="s">
-        <v>1383</v>
-      </c>
-      <c r="K4" t="s">
-        <v>1379</v>
-      </c>
-      <c r="L4" t="s">
-        <v>1380</v>
-      </c>
-      <c r="N4" t="s">
-        <v>1381</v>
-      </c>
-      <c r="O4" t="s">
-        <v>1382</v>
-      </c>
-      <c r="P4" t="s">
-        <v>1380</v>
-      </c>
-      <c r="R4" t="s">
-        <v>1383</v>
-      </c>
-      <c r="S4" t="s">
-        <v>1379</v>
-      </c>
-      <c r="T4" t="s">
-        <v>1380</v>
-      </c>
-      <c r="U4" t="s">
-        <v>1386</v>
-      </c>
-      <c r="V4" t="s">
-        <v>1381</v>
-      </c>
-      <c r="W4" t="s">
-        <v>1382</v>
-      </c>
-      <c r="X4" t="s">
-        <v>1380</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>1390</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>1387</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>450</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1384</v>
-      </c>
-      <c r="C5">
-        <v>8198360</v>
-      </c>
-      <c r="D5" t="s">
-        <v>1380</v>
-      </c>
-      <c r="E5" t="s">
-        <v>1385</v>
-      </c>
-      <c r="F5" t="s">
-        <v>1381</v>
-      </c>
-      <c r="G5" t="s">
-        <v>1382</v>
-      </c>
-      <c r="H5" t="s">
-        <v>1380</v>
-      </c>
-      <c r="I5" t="s">
-        <v>1391</v>
-      </c>
-      <c r="J5" t="s">
-        <v>1383</v>
-      </c>
-      <c r="K5" t="s">
-        <v>1379</v>
-      </c>
-      <c r="L5" t="s">
-        <v>1380</v>
-      </c>
-      <c r="N5" t="s">
-        <v>1381</v>
-      </c>
-      <c r="O5" t="s">
-        <v>1382</v>
-      </c>
-      <c r="P5" t="s">
-        <v>1380</v>
-      </c>
-      <c r="R5" t="s">
-        <v>1387</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>531</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1384</v>
-      </c>
-      <c r="C6">
-        <v>8888253</v>
-      </c>
-      <c r="D6" t="s">
-        <v>1380</v>
-      </c>
-      <c r="E6" t="s">
-        <v>1385</v>
-      </c>
-      <c r="F6" t="s">
-        <v>1381</v>
-      </c>
-      <c r="G6" t="s">
-        <v>1382</v>
-      </c>
-      <c r="H6" t="s">
-        <v>1380</v>
-      </c>
-      <c r="I6" t="s">
-        <v>1394</v>
-      </c>
-      <c r="J6" t="s">
-        <v>1383</v>
-      </c>
-      <c r="K6" t="s">
-        <v>1379</v>
-      </c>
-      <c r="L6" t="s">
-        <v>1380</v>
-      </c>
-      <c r="N6" t="s">
-        <v>1381</v>
-      </c>
-      <c r="O6" t="s">
-        <v>1382</v>
-      </c>
-      <c r="P6" t="s">
-        <v>1380</v>
-      </c>
-      <c r="R6" t="s">
-        <v>1387</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>534</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1384</v>
-      </c>
-      <c r="C7">
-        <v>8546048</v>
-      </c>
-      <c r="D7" t="s">
-        <v>1380</v>
-      </c>
-      <c r="E7" t="s">
-        <v>1385</v>
-      </c>
-      <c r="F7" t="s">
-        <v>1381</v>
-      </c>
-      <c r="G7" t="s">
-        <v>1382</v>
-      </c>
-      <c r="H7" t="s">
-        <v>1380</v>
-      </c>
-      <c r="I7" t="s">
-        <v>1395</v>
-      </c>
-      <c r="J7" t="s">
-        <v>1383</v>
-      </c>
-      <c r="K7" t="s">
-        <v>1379</v>
-      </c>
-      <c r="L7" t="s">
-        <v>1380</v>
-      </c>
-      <c r="N7" t="s">
-        <v>1381</v>
-      </c>
-      <c r="O7" t="s">
-        <v>1382</v>
-      </c>
-      <c r="P7" t="s">
-        <v>1380</v>
-      </c>
-      <c r="R7" t="s">
-        <v>1387</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>358</v>
-      </c>
-      <c r="B8" t="s">
-        <v>1384</v>
-      </c>
-      <c r="C8">
-        <v>6197512</v>
-      </c>
-      <c r="D8" t="s">
-        <v>1380</v>
-      </c>
-      <c r="F8" t="s">
-        <v>1381</v>
-      </c>
-      <c r="G8" t="s">
-        <v>1382</v>
-      </c>
-      <c r="H8" t="s">
-        <v>1380</v>
-      </c>
-      <c r="J8" t="s">
-        <v>1387</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>364</v>
-      </c>
-      <c r="B9" t="s">
-        <v>1384</v>
-      </c>
-      <c r="C9">
-        <v>28724627</v>
-      </c>
-      <c r="D9" t="s">
-        <v>1380</v>
-      </c>
-      <c r="F9" t="s">
-        <v>1381</v>
-      </c>
-      <c r="G9" t="s">
-        <v>1382</v>
-      </c>
-      <c r="H9" t="s">
-        <v>1380</v>
-      </c>
-      <c r="J9" t="s">
-        <v>1387</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>367</v>
-      </c>
-      <c r="B10" t="s">
-        <v>1384</v>
-      </c>
-      <c r="C10">
-        <v>10306892</v>
-      </c>
-      <c r="D10" t="s">
-        <v>1380</v>
-      </c>
-      <c r="F10" t="s">
-        <v>1381</v>
-      </c>
-      <c r="G10" t="s">
-        <v>1382</v>
-      </c>
-      <c r="H10" t="s">
-        <v>1380</v>
-      </c>
-      <c r="J10" t="s">
-        <v>1387</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>381</v>
-      </c>
-      <c r="B11" t="s">
-        <v>1384</v>
-      </c>
-      <c r="C11">
-        <v>10251455</v>
-      </c>
-      <c r="D11" t="s">
-        <v>1380</v>
-      </c>
-      <c r="F11" t="s">
-        <v>1381</v>
-      </c>
-      <c r="G11" t="s">
-        <v>1382</v>
-      </c>
-      <c r="H11" t="s">
-        <v>1380</v>
-      </c>
-      <c r="J11" t="s">
-        <v>1387</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>432</v>
-      </c>
-      <c r="B12" t="s">
-        <v>1384</v>
-      </c>
-      <c r="C12">
-        <v>51795710</v>
-      </c>
-      <c r="D12" t="s">
-        <v>1380</v>
-      </c>
-      <c r="F12" t="s">
-        <v>1381</v>
-      </c>
-      <c r="G12" t="s">
-        <v>1382</v>
-      </c>
-      <c r="H12" t="s">
-        <v>1380</v>
-      </c>
-      <c r="J12" t="s">
-        <v>1387</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>453</v>
-      </c>
-      <c r="B13" t="s">
-        <v>1384</v>
-      </c>
-      <c r="C13">
-        <v>10242166</v>
-      </c>
-      <c r="D13" t="s">
-        <v>1380</v>
-      </c>
-      <c r="F13" t="s">
-        <v>1381</v>
-      </c>
-      <c r="G13" t="s">
-        <v>1382</v>
-      </c>
-      <c r="H13" t="s">
-        <v>1380</v>
-      </c>
-      <c r="J13" t="s">
-        <v>1383</v>
-      </c>
-      <c r="K13" t="s">
-        <v>1379</v>
-      </c>
-      <c r="L13" t="s">
-        <v>1380</v>
-      </c>
-      <c r="M13" t="s">
-        <v>1385</v>
-      </c>
-      <c r="N13" t="s">
-        <v>1381</v>
-      </c>
-      <c r="O13" t="s">
-        <v>1382</v>
-      </c>
-      <c r="P13" t="s">
-        <v>1380</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>1392</v>
-      </c>
-      <c r="R13" t="s">
-        <v>1387</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>459</v>
-      </c>
-      <c r="B14" t="s">
-        <v>1384</v>
-      </c>
-      <c r="C14">
-        <v>10233351</v>
-      </c>
-      <c r="D14" t="s">
-        <v>1380</v>
-      </c>
-      <c r="F14" t="s">
-        <v>1381</v>
-      </c>
-      <c r="G14" t="s">
-        <v>1382</v>
-      </c>
-      <c r="H14" t="s">
-        <v>1380</v>
-      </c>
-      <c r="J14" t="s">
-        <v>1387</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>492</v>
-      </c>
-      <c r="B15" t="s">
-        <v>1384</v>
-      </c>
-      <c r="C15">
-        <v>8189514</v>
-      </c>
-      <c r="D15" t="s">
-        <v>1380</v>
-      </c>
-      <c r="F15" t="s">
-        <v>1381</v>
-      </c>
-      <c r="G15" t="s">
-        <v>1382</v>
-      </c>
-      <c r="H15" t="s">
-        <v>1380</v>
-      </c>
-      <c r="J15" t="s">
-        <v>1387</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>510</v>
-      </c>
-      <c r="B16" t="s">
-        <v>1384</v>
-      </c>
-      <c r="C16">
-        <v>10246126</v>
-      </c>
-      <c r="D16" t="s">
-        <v>1380</v>
-      </c>
-      <c r="F16" t="s">
-        <v>1381</v>
-      </c>
-      <c r="G16" t="s">
-        <v>1382</v>
-      </c>
-      <c r="H16" t="s">
-        <v>1380</v>
-      </c>
-      <c r="J16" t="s">
-        <v>1383</v>
-      </c>
-      <c r="K16" t="s">
-        <v>1379</v>
-      </c>
-      <c r="L16" t="s">
-        <v>1380</v>
-      </c>
-      <c r="M16" t="s">
-        <v>1385</v>
-      </c>
-      <c r="N16" t="s">
-        <v>1381</v>
-      </c>
-      <c r="O16" t="s">
-        <v>1382</v>
-      </c>
-      <c r="P16" t="s">
-        <v>1380</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>1393</v>
-      </c>
-      <c r="R16" t="s">
-        <v>1387</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>548</v>
-      </c>
-      <c r="B17" t="s">
-        <v>1384</v>
-      </c>
-      <c r="C17">
-        <v>10285797</v>
-      </c>
-      <c r="D17" t="s">
-        <v>1380</v>
-      </c>
-      <c r="F17" t="s">
-        <v>1381</v>
-      </c>
-      <c r="G17" t="s">
-        <v>1382</v>
-      </c>
-      <c r="H17" t="s">
-        <v>1380</v>
-      </c>
-      <c r="J17" t="s">
-        <v>1383</v>
-      </c>
-      <c r="K17" t="s">
-        <v>1379</v>
-      </c>
-      <c r="L17" t="s">
-        <v>1380</v>
-      </c>
-      <c r="M17" t="s">
-        <v>1385</v>
-      </c>
-      <c r="N17" t="s">
-        <v>1381</v>
-      </c>
-      <c r="O17" t="s">
-        <v>1382</v>
-      </c>
-      <c r="P17" t="s">
-        <v>1380</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>1396</v>
-      </c>
-      <c r="R17" t="s">
-        <v>1387</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A2:CD2">
-    <sortState ref="A3:CD17">
-      <sortCondition ref="E2"/>
-    </sortState>
-  </autoFilter>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
fixing metabolite concentrations from mM to M
</commit_message>
<xml_diff>
--- a/data/Model.xlsx
+++ b/data/Model.xlsx
@@ -144,10 +144,10 @@
     <t>Subtype</t>
   </si>
   <si>
-    <t>Average concentration, cytosol (mM)</t>
-  </si>
-  <si>
-    <t>Average concentration, extracellular</t>
+    <t>Average concentration, cytosol (M)</t>
+  </si>
+  <si>
+    <t>Average concentration, extracellular (M)</t>
   </si>
   <si>
     <t>Average count, cytosol</t>
@@ -3819,7 +3819,7 @@
     <t>Biomass production</t>
   </si>
   <si>
-    <t>[c]: (1.521617e+09) H2O + (1.101856e+06) ATP + (1.164906e+06) CTP + (1.728316e+06) GTP + (1.132896e+06) UTP + (3.419038e+04) ALA + (4.089038e+04) ARG + (2.429038e+04) ASP + (2.319038e+04) ASN + (2.229038e+04) CYS + (2.469038e+04) GLN + (2.269038e+04) GLU + (3.119038e+04) GLY + (2.159038e+04) HIS + (2.929038e+04) ILE + (4.119038e+04) LEU + (2.199038e+04) LYS + (2.139038e+04) MET + (2.389038e+04) PHE + (3.439038e+04) PRO + (4.449038e+04) SER + (3.619038e+04) THR + (2.219038e+04) TRP + (2.199038e+04) TYR + (3.379038e+04) VAL ==&gt; (1.000000e+00) Biomass + (4.972350e+06) H + (5.814192e+05) GDP + (1.035619e+06) AMP + (1.098019e+06) CMP + (1.052899e+06) GMP + (1.066339e+06) UMP + (4.381069e+06) PPI + (4.710962e+05) PI</t>
+    <t>[c]: (1.524425e+09) H2O + (1.101856e+06) ATP + (1.164906e+06) CTP + (7.209316e+06) GTP + (1.132896e+06) UTP + (2.177904e+05) ALA + (2.847904e+05) ARG + (1.187904e+05) ASP + (1.077904e+05) ASN + (9.879038e+04) CYS + (1.227904e+05) GLN + (1.027904e+05) GLU + (1.877904e+05) GLY + (9.179038e+04) HIS + (1.687904e+05) ILE + (2.877904e+05) LEU + (9.579038e+04) LYS + (8.979038e+04) MET + (1.147904e+05) PHE + (2.197904e+05) PRO + (3.207904e+05) SER + (2.377904e+05) THR + (9.779038e+04) TRP + (9.579038e+04) TYR + (2.137904e+05) VAL ==&gt; (1.000000e+00) Biomass + (1.045335e+07) H + (6.062419e+06) GDP + (1.035619e+06) AMP + (1.098019e+06) CMP + (1.052899e+06) GMP + (1.066339e+06) UMP + (4.381069e+06) PPI + (5.952096e+06) PI</t>
   </si>
   <si>
     <t>Value</t>
@@ -4036,11 +4036,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="0.00E+00"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="0.000E+00"/>
+    <numFmt numFmtId="166" formatCode="0.000E+00"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -4162,11 +4161,11 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4174,8 +4173,8 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -4464,11 +4463,11 @@
   <dimension ref="1:147"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B140" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D21" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A140" activeCellId="0" sqref="A140"/>
-      <selection pane="bottomRight" activeCell="G149" activeCellId="0" sqref="G149"/>
+      <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
+      <selection pane="bottomRight" activeCell="I30" activeCellId="0" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -4478,7 +4477,8 @@
     <col collapsed="false" hidden="false" max="5" min="3" style="1" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="7.60728744939271"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="10" min="8" style="1" width="16.497975708502"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="16.497975708502"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="6" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="12" min="11" style="1" width="15.6396761133603"/>
     <col collapsed="false" hidden="false" max="14" min="13" style="1" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="1" width="28.4939271255061"/>
@@ -4511,10 +4511,10 @@
       <c r="H1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="7" t="s">
         <v>25</v>
       </c>
       <c r="K1" s="7" t="s">
@@ -4560,10 +4560,10 @@
         <v>34</v>
       </c>
       <c r="I2" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="J2" s="0"/>
-      <c r="K2" s="9" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J2" s="9"/>
+      <c r="K2" s="8" t="n">
         <v>27580.76</v>
       </c>
       <c r="L2" s="0"/>
@@ -4601,10 +4601,10 @@
         <v>34</v>
       </c>
       <c r="I3" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="J3" s="0"/>
-      <c r="K3" s="9" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J3" s="9"/>
+      <c r="K3" s="8" t="n">
         <v>27580.76</v>
       </c>
       <c r="L3" s="0"/>
@@ -4642,10 +4642,10 @@
         <v>34</v>
       </c>
       <c r="I4" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="J4" s="0"/>
-      <c r="K4" s="9" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J4" s="9"/>
+      <c r="K4" s="8" t="n">
         <v>27580.76</v>
       </c>
       <c r="L4" s="0"/>
@@ -4683,15 +4683,15 @@
         <v>34</v>
       </c>
       <c r="I5" s="8" t="n">
-        <v>1</v>
+        <v>0.001</v>
       </c>
       <c r="J5" s="8" t="n">
-        <v>0.00104143</v>
-      </c>
-      <c r="K5" s="9" t="n">
+        <v>1.04143E-006</v>
+      </c>
+      <c r="K5" s="8" t="n">
         <v>27580.76</v>
       </c>
-      <c r="L5" s="9" t="n">
+      <c r="L5" s="8" t="n">
         <v>627149146</v>
       </c>
       <c r="M5" s="4" t="s">
@@ -4730,10 +4730,10 @@
         <v>49</v>
       </c>
       <c r="I6" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="J6" s="0"/>
-      <c r="K6" s="9" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J6" s="9"/>
+      <c r="K6" s="8" t="n">
         <v>27580.76</v>
       </c>
       <c r="L6" s="0"/>
@@ -4771,10 +4771,10 @@
         <v>53</v>
       </c>
       <c r="I7" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="J7" s="0"/>
-      <c r="K7" s="9" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J7" s="9"/>
+      <c r="K7" s="8" t="n">
         <v>27580.76</v>
       </c>
       <c r="L7" s="0"/>
@@ -4812,10 +4812,10 @@
         <v>53</v>
       </c>
       <c r="I8" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="J8" s="0"/>
-      <c r="K8" s="9" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J8" s="9"/>
+      <c r="K8" s="8" t="n">
         <v>27580.76</v>
       </c>
       <c r="L8" s="0"/>
@@ -4853,10 +4853,10 @@
         <v>53</v>
       </c>
       <c r="I9" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="J9" s="0"/>
-      <c r="K9" s="9" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J9" s="9"/>
+      <c r="K9" s="8" t="n">
         <v>27580.76</v>
       </c>
       <c r="L9" s="0"/>
@@ -4894,10 +4894,10 @@
         <v>53</v>
       </c>
       <c r="I10" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="J10" s="0"/>
-      <c r="K10" s="9" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J10" s="9"/>
+      <c r="K10" s="8" t="n">
         <v>27580.76</v>
       </c>
       <c r="L10" s="0"/>
@@ -4933,15 +4933,15 @@
       </c>
       <c r="H11" s="0"/>
       <c r="I11" s="8" t="n">
-        <v>1.122E-005</v>
+        <v>1.122E-008</v>
       </c>
       <c r="J11" s="8" t="n">
-        <v>1.7783E-005</v>
-      </c>
-      <c r="K11" s="9" t="n">
+        <v>1.7783E-008</v>
+      </c>
+      <c r="K11" s="8" t="n">
         <v>0.3094561272</v>
       </c>
-      <c r="L11" s="9" t="n">
+      <c r="L11" s="8" t="n">
         <v>10708922.6</v>
       </c>
       <c r="M11" s="4" t="s">
@@ -4978,10 +4978,10 @@
       </c>
       <c r="H12" s="0"/>
       <c r="I12" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="J12" s="0"/>
-      <c r="K12" s="9" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J12" s="9"/>
+      <c r="K12" s="8" t="n">
         <v>27580.76</v>
       </c>
       <c r="L12" s="0"/>
@@ -5017,15 +5017,15 @@
       </c>
       <c r="H13" s="0"/>
       <c r="I13" s="8" t="n">
-        <v>5</v>
+        <v>0.005</v>
       </c>
       <c r="J13" s="8" t="n">
-        <v>20</v>
-      </c>
-      <c r="K13" s="9" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="K13" s="8" t="n">
         <v>137903.8</v>
       </c>
-      <c r="L13" s="9" t="n">
+      <c r="L13" s="8" t="n">
         <v>12044000000000</v>
       </c>
       <c r="M13" s="4" t="s">
@@ -5062,15 +5062,15 @@
       </c>
       <c r="H14" s="0"/>
       <c r="I14" s="8" t="n">
-        <v>55000</v>
+        <v>55</v>
       </c>
       <c r="J14" s="8" t="n">
-        <v>55000</v>
-      </c>
-      <c r="K14" s="9" t="n">
+        <v>55</v>
+      </c>
+      <c r="K14" s="8" t="n">
         <v>1516941800</v>
       </c>
-      <c r="L14" s="9" t="n">
+      <c r="L14" s="8" t="n">
         <v>33121000000000000</v>
       </c>
       <c r="M14" s="4" t="s">
@@ -5109,10 +5109,10 @@
         <v>81</v>
       </c>
       <c r="I15" s="8" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="J15" s="0"/>
-      <c r="K15" s="9" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="J15" s="9"/>
+      <c r="K15" s="8" t="n">
         <v>13790.38</v>
       </c>
       <c r="L15" s="0"/>
@@ -5150,10 +5150,10 @@
         <v>81</v>
       </c>
       <c r="I16" s="8" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="J16" s="0"/>
-      <c r="K16" s="9" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="J16" s="9"/>
+      <c r="K16" s="8" t="n">
         <v>13790.38</v>
       </c>
       <c r="L16" s="0"/>
@@ -5191,10 +5191,10 @@
         <v>81</v>
       </c>
       <c r="I17" s="8" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="J17" s="0"/>
-      <c r="K17" s="9" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="J17" s="9"/>
+      <c r="K17" s="8" t="n">
         <v>13790.38</v>
       </c>
       <c r="L17" s="0"/>
@@ -5232,10 +5232,10 @@
         <v>81</v>
       </c>
       <c r="I18" s="8" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="J18" s="0"/>
-      <c r="K18" s="9" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="J18" s="9"/>
+      <c r="K18" s="8" t="n">
         <v>13790.38</v>
       </c>
       <c r="L18" s="0"/>
@@ -5273,10 +5273,10 @@
         <v>81</v>
       </c>
       <c r="I19" s="8" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="J19" s="0"/>
-      <c r="K19" s="9" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="J19" s="9"/>
+      <c r="K19" s="8" t="n">
         <v>13790.38</v>
       </c>
       <c r="L19" s="0"/>
@@ -5314,10 +5314,10 @@
         <v>81</v>
       </c>
       <c r="I20" s="8" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="J20" s="0"/>
-      <c r="K20" s="9" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="J20" s="9"/>
+      <c r="K20" s="8" t="n">
         <v>13790.38</v>
       </c>
       <c r="L20" s="0"/>
@@ -5355,10 +5355,10 @@
         <v>81</v>
       </c>
       <c r="I21" s="8" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="J21" s="0"/>
-      <c r="K21" s="9" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="J21" s="9"/>
+      <c r="K21" s="8" t="n">
         <v>13790.38</v>
       </c>
       <c r="L21" s="0"/>
@@ -5396,10 +5396,10 @@
         <v>81</v>
       </c>
       <c r="I22" s="8" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="J22" s="0"/>
-      <c r="K22" s="9" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="J22" s="9"/>
+      <c r="K22" s="8" t="n">
         <v>13790.38</v>
       </c>
       <c r="L22" s="0"/>
@@ -5437,10 +5437,10 @@
         <v>81</v>
       </c>
       <c r="I23" s="8" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="J23" s="0"/>
-      <c r="K23" s="9" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="J23" s="9"/>
+      <c r="K23" s="8" t="n">
         <v>13790.38</v>
       </c>
       <c r="L23" s="0"/>
@@ -5478,10 +5478,10 @@
         <v>81</v>
       </c>
       <c r="I24" s="8" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="J24" s="0"/>
-      <c r="K24" s="9" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="J24" s="9"/>
+      <c r="K24" s="8" t="n">
         <v>13790.38</v>
       </c>
       <c r="L24" s="0"/>
@@ -5519,10 +5519,10 @@
         <v>81</v>
       </c>
       <c r="I25" s="8" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="J25" s="0"/>
-      <c r="K25" s="9" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="J25" s="9"/>
+      <c r="K25" s="8" t="n">
         <v>13790.38</v>
       </c>
       <c r="L25" s="0"/>
@@ -5560,10 +5560,10 @@
         <v>81</v>
       </c>
       <c r="I26" s="8" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="J26" s="0"/>
-      <c r="K26" s="9" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="J26" s="9"/>
+      <c r="K26" s="8" t="n">
         <v>13790.38</v>
       </c>
       <c r="L26" s="0"/>
@@ -5601,10 +5601,10 @@
         <v>81</v>
       </c>
       <c r="I27" s="8" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="J27" s="0"/>
-      <c r="K27" s="9" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="J27" s="9"/>
+      <c r="K27" s="8" t="n">
         <v>13790.38</v>
       </c>
       <c r="L27" s="0"/>
@@ -5642,10 +5642,10 @@
         <v>81</v>
       </c>
       <c r="I28" s="8" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="J28" s="0"/>
-      <c r="K28" s="9" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="J28" s="9"/>
+      <c r="K28" s="8" t="n">
         <v>13790.38</v>
       </c>
       <c r="L28" s="0"/>
@@ -5683,10 +5683,10 @@
         <v>81</v>
       </c>
       <c r="I29" s="8" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="J29" s="0"/>
-      <c r="K29" s="9" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="J29" s="9"/>
+      <c r="K29" s="8" t="n">
         <v>13790.38</v>
       </c>
       <c r="L29" s="0"/>
@@ -5724,10 +5724,10 @@
         <v>81</v>
       </c>
       <c r="I30" s="8" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="J30" s="0"/>
-      <c r="K30" s="9" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="J30" s="9"/>
+      <c r="K30" s="8" t="n">
         <v>13790.38</v>
       </c>
       <c r="L30" s="0"/>
@@ -5765,10 +5765,10 @@
         <v>81</v>
       </c>
       <c r="I31" s="8" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="J31" s="0"/>
-      <c r="K31" s="9" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="J31" s="9"/>
+      <c r="K31" s="8" t="n">
         <v>13790.38</v>
       </c>
       <c r="L31" s="0"/>
@@ -5806,10 +5806,10 @@
         <v>81</v>
       </c>
       <c r="I32" s="8" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="J32" s="0"/>
-      <c r="K32" s="9" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="J32" s="9"/>
+      <c r="K32" s="8" t="n">
         <v>13790.38</v>
       </c>
       <c r="L32" s="0"/>
@@ -5847,10 +5847,10 @@
         <v>81</v>
       </c>
       <c r="I33" s="8" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="J33" s="0"/>
-      <c r="K33" s="9" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="J33" s="9"/>
+      <c r="K33" s="8" t="n">
         <v>13790.38</v>
       </c>
       <c r="L33" s="0"/>
@@ -5888,10 +5888,10 @@
         <v>81</v>
       </c>
       <c r="I34" s="8" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="J34" s="0"/>
-      <c r="K34" s="9" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="J34" s="9"/>
+      <c r="K34" s="8" t="n">
         <v>13790.38</v>
       </c>
       <c r="L34" s="0"/>
@@ -5927,8 +5927,8 @@
       <c r="I35" s="8" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J35" s="0"/>
-      <c r="K35" s="9" t="n">
+      <c r="J35" s="9"/>
+      <c r="K35" s="8" t="n">
         <v>5</v>
       </c>
       <c r="L35" s="0"/>
@@ -5964,8 +5964,8 @@
       <c r="I36" s="8" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J36" s="0"/>
-      <c r="K36" s="9" t="n">
+      <c r="J36" s="9"/>
+      <c r="K36" s="8" t="n">
         <v>5</v>
       </c>
       <c r="L36" s="0"/>
@@ -6001,8 +6001,8 @@
       <c r="I37" s="8" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J37" s="0"/>
-      <c r="K37" s="9" t="n">
+      <c r="J37" s="9"/>
+      <c r="K37" s="8" t="n">
         <v>5</v>
       </c>
       <c r="L37" s="0"/>
@@ -6036,8 +6036,8 @@
       <c r="I38" s="8" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J38" s="0"/>
-      <c r="K38" s="9" t="n">
+      <c r="J38" s="9"/>
+      <c r="K38" s="8" t="n">
         <v>5</v>
       </c>
       <c r="L38" s="0"/>
@@ -6075,8 +6075,8 @@
       <c r="I39" s="8" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J39" s="0"/>
-      <c r="K39" s="9" t="n">
+      <c r="J39" s="9"/>
+      <c r="K39" s="8" t="n">
         <v>5</v>
       </c>
       <c r="L39" s="0"/>
@@ -6114,8 +6114,8 @@
       <c r="I40" s="8" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J40" s="0"/>
-      <c r="K40" s="9" t="n">
+      <c r="J40" s="9"/>
+      <c r="K40" s="8" t="n">
         <v>5</v>
       </c>
       <c r="L40" s="0"/>
@@ -6153,8 +6153,8 @@
       <c r="I41" s="8" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J41" s="0"/>
-      <c r="K41" s="9" t="n">
+      <c r="J41" s="9"/>
+      <c r="K41" s="8" t="n">
         <v>5</v>
       </c>
       <c r="L41" s="0"/>
@@ -6192,8 +6192,8 @@
       <c r="I42" s="8" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J42" s="0"/>
-      <c r="K42" s="9" t="n">
+      <c r="J42" s="9"/>
+      <c r="K42" s="8" t="n">
         <v>5</v>
       </c>
       <c r="L42" s="0"/>
@@ -6231,8 +6231,8 @@
       <c r="I43" s="8" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J43" s="0"/>
-      <c r="K43" s="9" t="n">
+      <c r="J43" s="9"/>
+      <c r="K43" s="8" t="n">
         <v>5</v>
       </c>
       <c r="L43" s="0"/>
@@ -6270,8 +6270,8 @@
       <c r="I44" s="8" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J44" s="0"/>
-      <c r="K44" s="9" t="n">
+      <c r="J44" s="9"/>
+      <c r="K44" s="8" t="n">
         <v>5</v>
       </c>
       <c r="L44" s="0"/>
@@ -6309,8 +6309,8 @@
       <c r="I45" s="8" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J45" s="0"/>
-      <c r="K45" s="9" t="n">
+      <c r="J45" s="9"/>
+      <c r="K45" s="8" t="n">
         <v>5</v>
       </c>
       <c r="L45" s="0"/>
@@ -6348,8 +6348,8 @@
       <c r="I46" s="8" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J46" s="0"/>
-      <c r="K46" s="9" t="n">
+      <c r="J46" s="9"/>
+      <c r="K46" s="8" t="n">
         <v>5</v>
       </c>
       <c r="L46" s="0"/>
@@ -6387,8 +6387,8 @@
       <c r="I47" s="8" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J47" s="0"/>
-      <c r="K47" s="9" t="n">
+      <c r="J47" s="9"/>
+      <c r="K47" s="8" t="n">
         <v>5</v>
       </c>
       <c r="L47" s="0"/>
@@ -6426,8 +6426,8 @@
       <c r="I48" s="8" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J48" s="0"/>
-      <c r="K48" s="9" t="n">
+      <c r="J48" s="9"/>
+      <c r="K48" s="8" t="n">
         <v>5</v>
       </c>
       <c r="L48" s="0"/>
@@ -6465,8 +6465,8 @@
       <c r="I49" s="8" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J49" s="0"/>
-      <c r="K49" s="9" t="n">
+      <c r="J49" s="9"/>
+      <c r="K49" s="8" t="n">
         <v>5</v>
       </c>
       <c r="L49" s="0"/>
@@ -6504,8 +6504,8 @@
       <c r="I50" s="8" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J50" s="0"/>
-      <c r="K50" s="9" t="n">
+      <c r="J50" s="9"/>
+      <c r="K50" s="8" t="n">
         <v>5</v>
       </c>
       <c r="L50" s="0"/>
@@ -6543,8 +6543,8 @@
       <c r="I51" s="8" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J51" s="0"/>
-      <c r="K51" s="9" t="n">
+      <c r="J51" s="9"/>
+      <c r="K51" s="8" t="n">
         <v>5</v>
       </c>
       <c r="L51" s="0"/>
@@ -6582,8 +6582,8 @@
       <c r="I52" s="8" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J52" s="0"/>
-      <c r="K52" s="9" t="n">
+      <c r="J52" s="9"/>
+      <c r="K52" s="8" t="n">
         <v>5</v>
       </c>
       <c r="L52" s="0"/>
@@ -6621,8 +6621,8 @@
       <c r="I53" s="8" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J53" s="0"/>
-      <c r="K53" s="9" t="n">
+      <c r="J53" s="9"/>
+      <c r="K53" s="8" t="n">
         <v>5</v>
       </c>
       <c r="L53" s="0"/>
@@ -6660,8 +6660,8 @@
       <c r="I54" s="8" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J54" s="0"/>
-      <c r="K54" s="9" t="n">
+      <c r="J54" s="9"/>
+      <c r="K54" s="8" t="n">
         <v>5</v>
       </c>
       <c r="L54" s="0"/>
@@ -6699,8 +6699,8 @@
       <c r="I55" s="8" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J55" s="0"/>
-      <c r="K55" s="9" t="n">
+      <c r="J55" s="9"/>
+      <c r="K55" s="8" t="n">
         <v>5</v>
       </c>
       <c r="L55" s="0"/>
@@ -6738,8 +6738,8 @@
       <c r="I56" s="8" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J56" s="0"/>
-      <c r="K56" s="9" t="n">
+      <c r="J56" s="9"/>
+      <c r="K56" s="8" t="n">
         <v>5</v>
       </c>
       <c r="L56" s="0"/>
@@ -6777,8 +6777,8 @@
       <c r="I57" s="8" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J57" s="0"/>
-      <c r="K57" s="9" t="n">
+      <c r="J57" s="9"/>
+      <c r="K57" s="8" t="n">
         <v>5</v>
       </c>
       <c r="L57" s="0"/>
@@ -6816,8 +6816,8 @@
       <c r="I58" s="8" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J58" s="0"/>
-      <c r="K58" s="9" t="n">
+      <c r="J58" s="9"/>
+      <c r="K58" s="8" t="n">
         <v>5</v>
       </c>
       <c r="L58" s="0"/>
@@ -6855,8 +6855,8 @@
       <c r="I59" s="8" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J59" s="0"/>
-      <c r="K59" s="9" t="n">
+      <c r="J59" s="9"/>
+      <c r="K59" s="8" t="n">
         <v>5</v>
       </c>
       <c r="L59" s="0"/>
@@ -6894,8 +6894,8 @@
       <c r="I60" s="8" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J60" s="0"/>
-      <c r="K60" s="9" t="n">
+      <c r="J60" s="9"/>
+      <c r="K60" s="8" t="n">
         <v>5</v>
       </c>
       <c r="L60" s="0"/>
@@ -6933,8 +6933,8 @@
       <c r="I61" s="8" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J61" s="0"/>
-      <c r="K61" s="9" t="n">
+      <c r="J61" s="9"/>
+      <c r="K61" s="8" t="n">
         <v>5</v>
       </c>
       <c r="L61" s="0"/>
@@ -6972,8 +6972,8 @@
       <c r="I62" s="8" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J62" s="0"/>
-      <c r="K62" s="9" t="n">
+      <c r="J62" s="9"/>
+      <c r="K62" s="8" t="n">
         <v>5</v>
       </c>
       <c r="L62" s="0"/>
@@ -7011,8 +7011,8 @@
       <c r="I63" s="8" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J63" s="0"/>
-      <c r="K63" s="9" t="n">
+      <c r="J63" s="9"/>
+      <c r="K63" s="8" t="n">
         <v>5</v>
       </c>
       <c r="L63" s="0"/>
@@ -7050,8 +7050,8 @@
       <c r="I64" s="8" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J64" s="0"/>
-      <c r="K64" s="9" t="n">
+      <c r="J64" s="9"/>
+      <c r="K64" s="8" t="n">
         <v>5</v>
       </c>
       <c r="L64" s="0"/>
@@ -7087,8 +7087,8 @@
       <c r="I65" s="8" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J65" s="0"/>
-      <c r="K65" s="9" t="n">
+      <c r="J65" s="9"/>
+      <c r="K65" s="8" t="n">
         <v>1000</v>
       </c>
       <c r="L65" s="0"/>
@@ -7124,8 +7124,8 @@
       <c r="I66" s="8" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J66" s="0"/>
-      <c r="K66" s="9" t="n">
+      <c r="J66" s="9"/>
+      <c r="K66" s="8" t="n">
         <v>1000</v>
       </c>
       <c r="L66" s="0"/>
@@ -7161,8 +7161,8 @@
       <c r="I67" s="8" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J67" s="0"/>
-      <c r="K67" s="9" t="n">
+      <c r="J67" s="9"/>
+      <c r="K67" s="8" t="n">
         <v>1000</v>
       </c>
       <c r="L67" s="0"/>
@@ -7196,8 +7196,8 @@
       <c r="I68" s="8" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J68" s="0"/>
-      <c r="K68" s="9" t="n">
+      <c r="J68" s="9"/>
+      <c r="K68" s="8" t="n">
         <v>1000</v>
       </c>
       <c r="L68" s="0"/>
@@ -7235,8 +7235,8 @@
       <c r="I69" s="8" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J69" s="0"/>
-      <c r="K69" s="9" t="n">
+      <c r="J69" s="9"/>
+      <c r="K69" s="8" t="n">
         <v>1000</v>
       </c>
       <c r="L69" s="0"/>
@@ -7274,8 +7274,8 @@
       <c r="I70" s="8" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J70" s="0"/>
-      <c r="K70" s="9" t="n">
+      <c r="J70" s="9"/>
+      <c r="K70" s="8" t="n">
         <v>1000</v>
       </c>
       <c r="L70" s="0"/>
@@ -7313,8 +7313,8 @@
       <c r="I71" s="8" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J71" s="0"/>
-      <c r="K71" s="9" t="n">
+      <c r="J71" s="9"/>
+      <c r="K71" s="8" t="n">
         <v>1000</v>
       </c>
       <c r="L71" s="0"/>
@@ -7352,8 +7352,8 @@
       <c r="I72" s="8" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J72" s="0"/>
-      <c r="K72" s="9" t="n">
+      <c r="J72" s="9"/>
+      <c r="K72" s="8" t="n">
         <v>1000</v>
       </c>
       <c r="L72" s="0"/>
@@ -7391,8 +7391,8 @@
       <c r="I73" s="8" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J73" s="0"/>
-      <c r="K73" s="9" t="n">
+      <c r="J73" s="9"/>
+      <c r="K73" s="8" t="n">
         <v>1000</v>
       </c>
       <c r="L73" s="0"/>
@@ -7430,8 +7430,8 @@
       <c r="I74" s="8" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J74" s="0"/>
-      <c r="K74" s="9" t="n">
+      <c r="J74" s="9"/>
+      <c r="K74" s="8" t="n">
         <v>1000</v>
       </c>
       <c r="L74" s="0"/>
@@ -7469,8 +7469,8 @@
       <c r="I75" s="8" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J75" s="0"/>
-      <c r="K75" s="9" t="n">
+      <c r="J75" s="9"/>
+      <c r="K75" s="8" t="n">
         <v>1000</v>
       </c>
       <c r="L75" s="0"/>
@@ -7508,8 +7508,8 @@
       <c r="I76" s="8" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J76" s="0"/>
-      <c r="K76" s="9" t="n">
+      <c r="J76" s="9"/>
+      <c r="K76" s="8" t="n">
         <v>1000</v>
       </c>
       <c r="L76" s="0"/>
@@ -7547,8 +7547,8 @@
       <c r="I77" s="8" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J77" s="0"/>
-      <c r="K77" s="9" t="n">
+      <c r="J77" s="9"/>
+      <c r="K77" s="8" t="n">
         <v>1000</v>
       </c>
       <c r="L77" s="0"/>
@@ -7586,8 +7586,8 @@
       <c r="I78" s="8" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J78" s="0"/>
-      <c r="K78" s="9" t="n">
+      <c r="J78" s="9"/>
+      <c r="K78" s="8" t="n">
         <v>1000</v>
       </c>
       <c r="L78" s="0"/>
@@ -7625,8 +7625,8 @@
       <c r="I79" s="8" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J79" s="0"/>
-      <c r="K79" s="9" t="n">
+      <c r="J79" s="9"/>
+      <c r="K79" s="8" t="n">
         <v>1000</v>
       </c>
       <c r="L79" s="0"/>
@@ -7664,8 +7664,8 @@
       <c r="I80" s="8" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J80" s="0"/>
-      <c r="K80" s="9" t="n">
+      <c r="J80" s="9"/>
+      <c r="K80" s="8" t="n">
         <v>1000</v>
       </c>
       <c r="L80" s="0"/>
@@ -7703,8 +7703,8 @@
       <c r="I81" s="8" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J81" s="0"/>
-      <c r="K81" s="9" t="n">
+      <c r="J81" s="9"/>
+      <c r="K81" s="8" t="n">
         <v>1000</v>
       </c>
       <c r="L81" s="0"/>
@@ -7742,8 +7742,8 @@
       <c r="I82" s="8" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J82" s="0"/>
-      <c r="K82" s="9" t="n">
+      <c r="J82" s="9"/>
+      <c r="K82" s="8" t="n">
         <v>1000</v>
       </c>
       <c r="L82" s="0"/>
@@ -7781,8 +7781,8 @@
       <c r="I83" s="8" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J83" s="0"/>
-      <c r="K83" s="9" t="n">
+      <c r="J83" s="9"/>
+      <c r="K83" s="8" t="n">
         <v>1000</v>
       </c>
       <c r="L83" s="0"/>
@@ -7820,8 +7820,8 @@
       <c r="I84" s="8" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J84" s="0"/>
-      <c r="K84" s="9" t="n">
+      <c r="J84" s="9"/>
+      <c r="K84" s="8" t="n">
         <v>1000</v>
       </c>
       <c r="L84" s="0"/>
@@ -7859,8 +7859,8 @@
       <c r="I85" s="8" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J85" s="0"/>
-      <c r="K85" s="9" t="n">
+      <c r="J85" s="9"/>
+      <c r="K85" s="8" t="n">
         <v>1000</v>
       </c>
       <c r="L85" s="0"/>
@@ -7898,8 +7898,8 @@
       <c r="I86" s="8" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J86" s="0"/>
-      <c r="K86" s="9" t="n">
+      <c r="J86" s="9"/>
+      <c r="K86" s="8" t="n">
         <v>1000</v>
       </c>
       <c r="L86" s="0"/>
@@ -7937,8 +7937,8 @@
       <c r="I87" s="8" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J87" s="0"/>
-      <c r="K87" s="9" t="n">
+      <c r="J87" s="9"/>
+      <c r="K87" s="8" t="n">
         <v>1000</v>
       </c>
       <c r="L87" s="0"/>
@@ -7976,8 +7976,8 @@
       <c r="I88" s="8" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J88" s="0"/>
-      <c r="K88" s="9" t="n">
+      <c r="J88" s="9"/>
+      <c r="K88" s="8" t="n">
         <v>1000</v>
       </c>
       <c r="L88" s="0"/>
@@ -8015,8 +8015,8 @@
       <c r="I89" s="8" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J89" s="0"/>
-      <c r="K89" s="9" t="n">
+      <c r="J89" s="9"/>
+      <c r="K89" s="8" t="n">
         <v>1000</v>
       </c>
       <c r="L89" s="0"/>
@@ -8054,8 +8054,8 @@
       <c r="I90" s="8" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J90" s="0"/>
-      <c r="K90" s="9" t="n">
+      <c r="J90" s="9"/>
+      <c r="K90" s="8" t="n">
         <v>1000</v>
       </c>
       <c r="L90" s="0"/>
@@ -8093,8 +8093,8 @@
       <c r="I91" s="8" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J91" s="0"/>
-      <c r="K91" s="9" t="n">
+      <c r="J91" s="9"/>
+      <c r="K91" s="8" t="n">
         <v>1000</v>
       </c>
       <c r="L91" s="0"/>
@@ -8132,8 +8132,8 @@
       <c r="I92" s="8" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J92" s="0"/>
-      <c r="K92" s="9" t="n">
+      <c r="J92" s="9"/>
+      <c r="K92" s="8" t="n">
         <v>1000</v>
       </c>
       <c r="L92" s="0"/>
@@ -8171,8 +8171,8 @@
       <c r="I93" s="8" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J93" s="0"/>
-      <c r="K93" s="9" t="n">
+      <c r="J93" s="9"/>
+      <c r="K93" s="8" t="n">
         <v>1000</v>
       </c>
       <c r="L93" s="0"/>
@@ -8210,8 +8210,8 @@
       <c r="I94" s="8" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J94" s="0"/>
-      <c r="K94" s="9" t="n">
+      <c r="J94" s="9"/>
+      <c r="K94" s="8" t="n">
         <v>1000</v>
       </c>
       <c r="L94" s="0"/>
@@ -8245,10 +8245,11 @@
       <c r="G95" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="I95" s="8"/>
       <c r="J95" s="8" t="n">
-        <v>0.148</v>
-      </c>
-      <c r="L95" s="9" t="n">
+        <v>0.000148</v>
+      </c>
+      <c r="L95" s="8" t="n">
         <v>89125600000</v>
       </c>
       <c r="M95" s="4" t="s">
@@ -8283,7 +8284,8 @@
       <c r="G96" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J96" s="0"/>
+      <c r="I96" s="8"/>
+      <c r="J96" s="9"/>
       <c r="L96" s="0"/>
       <c r="M96" s="4" t="s">
         <v>35</v>
@@ -8315,10 +8317,11 @@
       <c r="G97" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="I97" s="8"/>
       <c r="J97" s="8" t="n">
-        <v>7.27552</v>
-      </c>
-      <c r="L97" s="9" t="n">
+        <v>0.00727552</v>
+      </c>
+      <c r="L97" s="8" t="n">
         <v>4381318144000</v>
       </c>
       <c r="M97" s="4" t="s">
@@ -8353,10 +8356,11 @@
       <c r="G98" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="I98" s="8"/>
       <c r="J98" s="8" t="n">
-        <v>3.05544</v>
-      </c>
-      <c r="L98" s="9" t="n">
+        <v>0.00305544</v>
+      </c>
+      <c r="L98" s="8" t="n">
         <v>1839985968000</v>
       </c>
       <c r="M98" s="4" t="s">
@@ -8391,10 +8395,11 @@
       <c r="G99" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="I99" s="8"/>
       <c r="J99" s="8" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="L99" s="9" t="n">
+        <v>0.0002</v>
+      </c>
+      <c r="L99" s="8" t="n">
         <v>120440000000</v>
       </c>
       <c r="M99" s="4" t="s">
@@ -8429,10 +8434,11 @@
       <c r="G100" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="I100" s="8"/>
       <c r="J100" s="8" t="n">
-        <v>7.81962</v>
-      </c>
-      <c r="L100" s="9" t="n">
+        <v>0.00781962</v>
+      </c>
+      <c r="L100" s="8" t="n">
         <v>4708975164000</v>
       </c>
       <c r="M100" s="4" t="s">
@@ -8467,7 +8473,8 @@
       <c r="G101" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J101" s="0"/>
+      <c r="I101" s="8"/>
+      <c r="J101" s="9"/>
       <c r="L101" s="0"/>
       <c r="M101" s="4" t="s">
         <v>35</v>
@@ -8499,10 +8506,11 @@
       <c r="G102" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="I102" s="8"/>
       <c r="J102" s="8" t="n">
-        <v>1.70010200612037</v>
-      </c>
-      <c r="L102" s="9" t="n">
+        <v>0.00170010200612037</v>
+      </c>
+      <c r="L102" s="8" t="n">
         <v>1023801428085.69</v>
       </c>
       <c r="M102" s="4" t="s">
@@ -8537,10 +8545,11 @@
       <c r="G103" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="I103" s="8"/>
       <c r="J103" s="8" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="L103" s="9" t="n">
+        <v>0.00025</v>
+      </c>
+      <c r="L103" s="8" t="n">
         <v>150550000000</v>
       </c>
       <c r="M103" s="4" t="s">
@@ -8575,10 +8584,11 @@
       <c r="G104" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="I104" s="8"/>
       <c r="J104" s="8" t="n">
-        <v>3.18137</v>
-      </c>
-      <c r="L104" s="9" t="n">
+        <v>0.00318137</v>
+      </c>
+      <c r="L104" s="8" t="n">
         <v>1915821014000</v>
       </c>
       <c r="M104" s="4" t="s">
@@ -8613,7 +8623,8 @@
       <c r="G105" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J105" s="0"/>
+      <c r="I105" s="8"/>
+      <c r="J105" s="9"/>
       <c r="L105" s="0"/>
       <c r="M105" s="4" t="s">
         <v>35</v>
@@ -8645,7 +8656,8 @@
       <c r="G106" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J106" s="0"/>
+      <c r="I106" s="8"/>
+      <c r="J106" s="9"/>
       <c r="L106" s="0"/>
       <c r="M106" s="4" t="s">
         <v>35</v>
@@ -8677,7 +8689,8 @@
       <c r="G107" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J107" s="0"/>
+      <c r="I107" s="8"/>
+      <c r="J107" s="9"/>
       <c r="L107" s="0"/>
       <c r="M107" s="4" t="s">
         <v>35</v>
@@ -8709,7 +8722,8 @@
       <c r="G108" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J108" s="0"/>
+      <c r="I108" s="8"/>
+      <c r="J108" s="9"/>
       <c r="L108" s="0"/>
       <c r="M108" s="4" t="s">
         <v>35</v>
@@ -8741,7 +8755,8 @@
       <c r="G109" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J109" s="0"/>
+      <c r="I109" s="8"/>
+      <c r="J109" s="9"/>
       <c r="L109" s="0"/>
       <c r="M109" s="4" t="s">
         <v>35</v>
@@ -8773,7 +8788,8 @@
       <c r="G110" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J110" s="0"/>
+      <c r="I110" s="8"/>
+      <c r="J110" s="9"/>
       <c r="L110" s="0"/>
       <c r="M110" s="4" t="s">
         <v>35</v>
@@ -8805,7 +8821,8 @@
       <c r="G111" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J111" s="0"/>
+      <c r="I111" s="8"/>
+      <c r="J111" s="9"/>
       <c r="L111" s="0"/>
       <c r="M111" s="4" t="s">
         <v>35</v>
@@ -8837,10 +8854,11 @@
       <c r="G112" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="I112" s="8"/>
       <c r="J112" s="8" t="n">
-        <v>55.0705747828259</v>
-      </c>
-      <c r="L112" s="9" t="n">
+        <v>0.0550705747828259</v>
+      </c>
+      <c r="L112" s="8" t="n">
         <v>33163500134217.8</v>
       </c>
       <c r="M112" s="4" t="s">
@@ -8875,10 +8893,11 @@
       <c r="G113" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="I113" s="8"/>
       <c r="J113" s="8" t="n">
-        <v>0.13234</v>
-      </c>
-      <c r="L113" s="9" t="n">
+        <v>0.00013234</v>
+      </c>
+      <c r="L113" s="8" t="n">
         <v>79695148000</v>
       </c>
       <c r="M113" s="4" t="s">
@@ -8913,10 +8932,11 @@
       <c r="G114" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="I114" s="8"/>
       <c r="J114" s="8" t="n">
-        <v>0.715127</v>
-      </c>
-      <c r="L114" s="9" t="n">
+        <v>0.000715127</v>
+      </c>
+      <c r="L114" s="8" t="n">
         <v>430649479400</v>
       </c>
       <c r="M114" s="0"/>
@@ -8947,10 +8967,11 @@
       <c r="G115" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="I115" s="8"/>
       <c r="J115" s="8" t="n">
-        <v>13.4776</v>
-      </c>
-      <c r="L115" s="9" t="n">
+        <v>0.0134776</v>
+      </c>
+      <c r="L115" s="8" t="n">
         <v>8116210720000</v>
       </c>
       <c r="M115" s="4" t="s">
@@ -8985,10 +9006,11 @@
       <c r="G116" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="I116" s="8"/>
       <c r="J116" s="8" t="n">
-        <v>7.82989</v>
-      </c>
-      <c r="L116" s="9" t="n">
+        <v>0.00782989</v>
+      </c>
+      <c r="L116" s="8" t="n">
         <v>4715159758000</v>
       </c>
       <c r="M116" s="4" t="s">
@@ -9023,10 +9045,11 @@
       <c r="G117" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="I117" s="8"/>
       <c r="J117" s="8" t="n">
-        <v>2.38654</v>
-      </c>
-      <c r="L117" s="9" t="n">
+        <v>0.00238654</v>
+      </c>
+      <c r="L117" s="8" t="n">
         <v>1437174388000</v>
       </c>
       <c r="M117" s="4" t="s">
@@ -9061,10 +9084,11 @@
       <c r="G118" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="I118" s="8"/>
       <c r="J118" s="8" t="n">
-        <v>4.06589</v>
-      </c>
-      <c r="L118" s="9" t="n">
+        <v>0.00406589</v>
+      </c>
+      <c r="L118" s="8" t="n">
         <v>2448478958000</v>
       </c>
       <c r="M118" s="0"/>
@@ -9095,7 +9119,8 @@
       <c r="G119" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J119" s="0"/>
+      <c r="I119" s="8"/>
+      <c r="J119" s="9"/>
       <c r="L119" s="0"/>
       <c r="M119" s="4" t="s">
         <v>35</v>
@@ -9127,10 +9152,11 @@
       <c r="G120" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="I120" s="8"/>
       <c r="J120" s="8" t="n">
-        <v>7.81927</v>
-      </c>
-      <c r="L120" s="9" t="n">
+        <v>0.00781927</v>
+      </c>
+      <c r="L120" s="8" t="n">
         <v>4708764394000</v>
       </c>
       <c r="M120" s="4" t="s">
@@ -9165,10 +9191,11 @@
       <c r="G121" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="I121" s="8"/>
       <c r="J121" s="8" t="n">
-        <v>6.30316</v>
-      </c>
-      <c r="L121" s="9" t="n">
+        <v>0.00630316</v>
+      </c>
+      <c r="L121" s="8" t="n">
         <v>3795762952000</v>
       </c>
       <c r="M121" s="4" t="s">
@@ -9203,10 +9230,11 @@
       <c r="G122" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="I122" s="8"/>
       <c r="J122" s="8" t="n">
-        <v>1.79497</v>
-      </c>
-      <c r="L122" s="9" t="n">
+        <v>0.00179497</v>
+      </c>
+      <c r="L122" s="8" t="n">
         <v>1080930934000</v>
       </c>
       <c r="M122" s="4" t="s">
@@ -9241,10 +9269,11 @@
       <c r="G123" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="I123" s="8"/>
       <c r="J123" s="8" t="n">
-        <v>0.00528369</v>
-      </c>
-      <c r="L123" s="9" t="n">
+        <v>5.28369E-006</v>
+      </c>
+      <c r="L123" s="8" t="n">
         <v>3181838118</v>
       </c>
       <c r="M123" s="4" t="s">
@@ -9279,7 +9308,8 @@
       <c r="G124" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J124" s="0"/>
+      <c r="I124" s="8"/>
+      <c r="J124" s="9"/>
       <c r="L124" s="0"/>
       <c r="M124" s="4" t="s">
         <v>35</v>
@@ -9311,10 +9341,11 @@
       <c r="G125" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="I125" s="8"/>
       <c r="J125" s="8" t="n">
-        <v>0.273010920436817</v>
-      </c>
-      <c r="L125" s="9" t="n">
+        <v>0.000273010920436817</v>
+      </c>
+      <c r="L125" s="8" t="n">
         <v>164407176287.052</v>
       </c>
       <c r="M125" s="4" t="s">
@@ -9349,7 +9380,8 @@
       <c r="G126" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J126" s="0"/>
+      <c r="I126" s="8"/>
+      <c r="J126" s="9"/>
       <c r="L126" s="0"/>
       <c r="M126" s="4" t="s">
         <v>35</v>
@@ -9381,10 +9413,11 @@
       <c r="G127" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="I127" s="8"/>
       <c r="J127" s="8" t="n">
-        <v>20</v>
-      </c>
-      <c r="L127" s="9" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="L127" s="8" t="n">
         <v>12044000000000</v>
       </c>
       <c r="M127" s="4" t="s">
@@ -9419,7 +9452,8 @@
       <c r="G128" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J128" s="0"/>
+      <c r="I128" s="8"/>
+      <c r="J128" s="9"/>
       <c r="L128" s="0"/>
       <c r="M128" s="4" t="s">
         <v>35</v>
@@ -9451,7 +9485,8 @@
       <c r="G129" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J129" s="0"/>
+      <c r="I129" s="8"/>
+      <c r="J129" s="9"/>
       <c r="L129" s="0"/>
       <c r="M129" s="4" t="s">
         <v>35</v>
@@ -9483,7 +9518,8 @@
       <c r="G130" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J130" s="0"/>
+      <c r="I130" s="8"/>
+      <c r="J130" s="9"/>
       <c r="L130" s="0"/>
       <c r="M130" s="4" t="s">
         <v>35</v>
@@ -9515,10 +9551,11 @@
       <c r="G131" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="I131" s="8"/>
       <c r="J131" s="8" t="n">
-        <v>3.40385</v>
-      </c>
-      <c r="L131" s="9" t="n">
+        <v>0.00340385</v>
+      </c>
+      <c r="L131" s="8" t="n">
         <v>2049798470000</v>
       </c>
       <c r="M131" s="4" t="s">
@@ -9553,10 +9590,11 @@
       <c r="G132" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="I132" s="8"/>
       <c r="J132" s="8" t="n">
-        <v>8.24728</v>
-      </c>
-      <c r="L132" s="9" t="n">
+        <v>0.00824728</v>
+      </c>
+      <c r="L132" s="8" t="n">
         <v>4966512016000</v>
       </c>
       <c r="M132" s="0"/>
@@ -9587,7 +9625,8 @@
       <c r="G133" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J133" s="0"/>
+      <c r="I133" s="8"/>
+      <c r="J133" s="9"/>
       <c r="L133" s="0"/>
       <c r="M133" s="4" t="s">
         <v>35</v>
@@ -9619,7 +9658,8 @@
       <c r="G134" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J134" s="0"/>
+      <c r="I134" s="8"/>
+      <c r="J134" s="9"/>
       <c r="L134" s="0"/>
       <c r="M134" s="4" t="s">
         <v>35</v>
@@ -9651,7 +9691,8 @@
       <c r="G135" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J135" s="0"/>
+      <c r="I135" s="8"/>
+      <c r="J135" s="9"/>
       <c r="L135" s="0"/>
       <c r="M135" s="4" t="s">
         <v>35</v>
@@ -9683,10 +9724,11 @@
       <c r="G136" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="I136" s="8"/>
       <c r="J136" s="8" t="n">
-        <v>5.3761</v>
-      </c>
-      <c r="L136" s="9" t="n">
+        <v>0.0053761</v>
+      </c>
+      <c r="L136" s="8" t="n">
         <v>3237487420000</v>
       </c>
       <c r="M136" s="4" t="s">
@@ -9721,7 +9763,8 @@
       <c r="G137" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J137" s="0"/>
+      <c r="I137" s="8"/>
+      <c r="J137" s="9"/>
       <c r="L137" s="0"/>
       <c r="M137" s="4" t="s">
         <v>35</v>
@@ -9753,7 +9796,8 @@
       <c r="G138" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J138" s="0"/>
+      <c r="I138" s="8"/>
+      <c r="J138" s="9"/>
       <c r="L138" s="0"/>
       <c r="M138" s="4" t="s">
         <v>35</v>
@@ -9785,10 +9829,11 @@
       <c r="G139" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="I139" s="8"/>
       <c r="J139" s="8" t="n">
-        <v>4.70492</v>
-      </c>
-      <c r="L139" s="9" t="n">
+        <v>0.00470492</v>
+      </c>
+      <c r="L139" s="8" t="n">
         <v>2833302824000</v>
       </c>
       <c r="M139" s="0"/>
@@ -9819,10 +9864,11 @@
       <c r="G140" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="I140" s="8"/>
       <c r="J140" s="8" t="n">
-        <v>0.313168</v>
-      </c>
-      <c r="L140" s="9" t="n">
+        <v>0.000313168</v>
+      </c>
+      <c r="L140" s="8" t="n">
         <v>188589769600</v>
       </c>
       <c r="M140" s="4" t="s">
@@ -9857,10 +9903,11 @@
       <c r="G141" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="I141" s="8"/>
       <c r="J141" s="8" t="n">
-        <v>1.12553</v>
-      </c>
-      <c r="L141" s="9" t="n">
+        <v>0.00112553</v>
+      </c>
+      <c r="L141" s="8" t="n">
         <v>677794166000</v>
       </c>
       <c r="M141" s="4" t="s">
@@ -9895,7 +9942,8 @@
       <c r="G142" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J142" s="0"/>
+      <c r="I142" s="8"/>
+      <c r="J142" s="9"/>
       <c r="L142" s="0"/>
       <c r="M142" s="4" t="s">
         <v>35</v>
@@ -9927,10 +9975,11 @@
       <c r="G143" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="I143" s="8"/>
       <c r="J143" s="8" t="n">
-        <v>0.178433</v>
-      </c>
-      <c r="L143" s="9" t="n">
+        <v>0.000178433</v>
+      </c>
+      <c r="L143" s="8" t="n">
         <v>107452352600</v>
       </c>
       <c r="M143" s="4" t="s">
@@ -9965,7 +10014,8 @@
       <c r="G144" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J144" s="0"/>
+      <c r="I144" s="8"/>
+      <c r="J144" s="9"/>
       <c r="L144" s="0"/>
       <c r="M144" s="4" t="s">
         <v>35</v>
@@ -9997,10 +10047,11 @@
       <c r="G145" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="I145" s="8"/>
       <c r="J145" s="8" t="n">
-        <v>5.87101</v>
-      </c>
-      <c r="L145" s="9" t="n">
+        <v>0.00587101</v>
+      </c>
+      <c r="L145" s="8" t="n">
         <v>3535522222000</v>
       </c>
       <c r="M145" s="4" t="s">
@@ -10035,6 +10086,7 @@
       <c r="G146" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="I146" s="8"/>
       <c r="M146" s="4" t="s">
         <v>35</v>
       </c>
@@ -10068,11 +10120,11 @@
   <dimension ref="A1:K177"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C28" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C172" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
-      <selection pane="bottomRight" activeCell="G31" activeCellId="0" sqref="G31"/>
+      <selection pane="bottomLeft" activeCell="A172" activeCellId="0" sqref="A172"/>
+      <selection pane="bottomRight" activeCell="D177" activeCellId="0" sqref="D177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
fixing transcription rate law
</commit_message>
<xml_diff>
--- a/data/Model.xlsx
+++ b/data/Model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Submodels" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,18 +28,21 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Submodels!$A$1:$C$5</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Submodels!$A$1:$C$5</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Submodels!$A$1:$C$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Submodels!$A$1:$C$5</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0" vbProcedure="false">Compartments!$A$1:$C$3</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0_0" vbProcedure="false">Compartments!$A$1:$C$3</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0_0_0" vbProcedure="false">Compartments!$A$1:$C$3</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$C$3</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">Compartments!$A$1:$C$3</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Compartments!$A$1:$C$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Compartments!$A$1:$C$3</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_FilterDatabase_0" vbProcedure="false">Species!$A$1:$N$147</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_FilterDatabase_0_0" vbProcedure="false">Species!$A$1:$N$147</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_FilterDatabase_0_0_0" vbProcedure="false">Species!$A$1:$N$147</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Species!$A$1:$O$147</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">Species!$A$1:$O$147</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Species!$A$1:$O$147</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Species!$A$1:$O$147</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0" vbProcedure="false">Reactions!$A$1:$J$177</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0" vbProcedure="false">Reactions!$A$1:$J$177</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0_0" vbProcedure="false">Reactions!$A$1:$J$177</definedName>
@@ -47,18 +50,21 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Reactions!$A$1:$K$177</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">Reactions!$A$1:$K$177</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Reactions!$A$1:$K$177</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Reactions!$A$1:$K$177</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$F$3</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$F$3</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0_0" vbProcedure="false">Parameters!$A$1:$F$3</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$F$3</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$F$3</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$F$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Parameters!$A$1:$F$3</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_FilterDatabase_0" vbProcedure="false">References!$A$1:$E$3</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_FilterDatabase_0_0" vbProcedure="false">References!$A$1:$E$3</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_FilterDatabase_0_0_0" vbProcedure="false">References!$A$1:$E$3</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$E$3</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0" vbProcedure="false">References!$A$1:$E$3</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">References!$A$1:$E$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">References!$A$1:$E$3</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -2814,7 +2820,7 @@
     <t>[c]: (79) ATP + (68) CTP + (70) GTP + (86) UTP + H2O ==&gt; RnaPolymerase-Rna + (303) PPI + H</t>
   </si>
   <si>
-    <t>Vmax * min(ATP[c], CTP[c], GTP[c], UTP[c]) / (Km + min(ATP[c], CTP[c], GTP[c], UTP[c])) * RnaPol-Protein[c]</t>
+    <t>Vmax * min(ATP[c], CTP[c], GTP[c], UTP[c]) / (Km + min(ATP[c], CTP[c], GTP[c], UTP[c])) * RnaPolymerase-Protein[c]</t>
   </si>
   <si>
     <t>2.7.7.6</t>
@@ -4136,7 +4142,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4159,10 +4165,6 @@
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -4298,9 +4300,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.6761133603239"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.4251012145749"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.7813765182186"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.5344129554656"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -4390,9 +4392,9 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="5.1417004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.3522267206478"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="56.3441295546559"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.4615384615385"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="56.7732793522267"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -4462,26 +4464,25 @@
   </sheetPr>
   <dimension ref="1:147"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D21" activePane="bottomRight" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="K21" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topRight" activeCell="K1" activeCellId="0" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="I30" activeCellId="0" sqref="I30"/>
+      <selection pane="bottomRight" activeCell="K30" activeCellId="0" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="31.3846153846154"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="34.3846153846154"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="31.5991902834008"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="34.5991902834008"/>
     <col collapsed="false" hidden="false" max="5" min="3" style="1" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="7.60728744939271"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="6" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="12" min="11" style="1" width="15.6396761133603"/>
+    <col collapsed="false" hidden="false" max="10" min="8" style="1" width="16.497975708502"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="1" width="15.7449392712551"/>
     <col collapsed="false" hidden="false" max="14" min="13" style="1" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="28.4939271255061"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="28.7085020242915"/>
     <col collapsed="false" hidden="false" max="1023" min="16" style="1" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="9.10526315789474"/>
   </cols>
@@ -4511,16 +4512,16 @@
       <c r="H1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="6" t="s">
         <v>27</v>
       </c>
       <c r="M1" s="2" t="s">
@@ -4559,11 +4560,11 @@
       <c r="H2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="I2" s="8" t="n">
+      <c r="I2" s="7" t="n">
         <v>0.001</v>
       </c>
-      <c r="J2" s="9"/>
-      <c r="K2" s="8" t="n">
+      <c r="J2" s="8"/>
+      <c r="K2" s="7" t="n">
         <v>27580.76</v>
       </c>
       <c r="L2" s="0"/>
@@ -4600,11 +4601,11 @@
       <c r="H3" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="I3" s="8" t="n">
+      <c r="I3" s="7" t="n">
         <v>0.001</v>
       </c>
-      <c r="J3" s="9"/>
-      <c r="K3" s="8" t="n">
+      <c r="J3" s="8"/>
+      <c r="K3" s="7" t="n">
         <v>27580.76</v>
       </c>
       <c r="L3" s="0"/>
@@ -4641,11 +4642,11 @@
       <c r="H4" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="I4" s="8" t="n">
+      <c r="I4" s="7" t="n">
         <v>0.001</v>
       </c>
-      <c r="J4" s="9"/>
-      <c r="K4" s="8" t="n">
+      <c r="J4" s="8"/>
+      <c r="K4" s="7" t="n">
         <v>27580.76</v>
       </c>
       <c r="L4" s="0"/>
@@ -4682,16 +4683,16 @@
       <c r="H5" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="I5" s="8" t="n">
+      <c r="I5" s="7" t="n">
         <v>0.001</v>
       </c>
-      <c r="J5" s="8" t="n">
+      <c r="J5" s="7" t="n">
         <v>1.04143E-006</v>
       </c>
-      <c r="K5" s="8" t="n">
+      <c r="K5" s="7" t="n">
         <v>27580.76</v>
       </c>
-      <c r="L5" s="8" t="n">
+      <c r="L5" s="7" t="n">
         <v>627149146</v>
       </c>
       <c r="M5" s="4" t="s">
@@ -4729,11 +4730,11 @@
       <c r="H6" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="I6" s="8" t="n">
+      <c r="I6" s="7" t="n">
         <v>0.001</v>
       </c>
-      <c r="J6" s="9"/>
-      <c r="K6" s="8" t="n">
+      <c r="J6" s="8"/>
+      <c r="K6" s="7" t="n">
         <v>27580.76</v>
       </c>
       <c r="L6" s="0"/>
@@ -4770,11 +4771,11 @@
       <c r="H7" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="I7" s="8" t="n">
+      <c r="I7" s="7" t="n">
         <v>0.001</v>
       </c>
-      <c r="J7" s="9"/>
-      <c r="K7" s="8" t="n">
+      <c r="J7" s="8"/>
+      <c r="K7" s="7" t="n">
         <v>27580.76</v>
       </c>
       <c r="L7" s="0"/>
@@ -4811,11 +4812,11 @@
       <c r="H8" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="I8" s="8" t="n">
+      <c r="I8" s="7" t="n">
         <v>0.001</v>
       </c>
-      <c r="J8" s="9"/>
-      <c r="K8" s="8" t="n">
+      <c r="J8" s="8"/>
+      <c r="K8" s="7" t="n">
         <v>27580.76</v>
       </c>
       <c r="L8" s="0"/>
@@ -4852,11 +4853,11 @@
       <c r="H9" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="I9" s="8" t="n">
+      <c r="I9" s="7" t="n">
         <v>0.001</v>
       </c>
-      <c r="J9" s="9"/>
-      <c r="K9" s="8" t="n">
+      <c r="J9" s="8"/>
+      <c r="K9" s="7" t="n">
         <v>27580.76</v>
       </c>
       <c r="L9" s="0"/>
@@ -4893,11 +4894,11 @@
       <c r="H10" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="I10" s="8" t="n">
+      <c r="I10" s="7" t="n">
         <v>0.001</v>
       </c>
-      <c r="J10" s="9"/>
-      <c r="K10" s="8" t="n">
+      <c r="J10" s="8"/>
+      <c r="K10" s="7" t="n">
         <v>27580.76</v>
       </c>
       <c r="L10" s="0"/>
@@ -4913,7 +4914,7 @@
       <c r="A11" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="9" t="s">
         <v>64</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -4932,16 +4933,16 @@
         <v>33</v>
       </c>
       <c r="H11" s="0"/>
-      <c r="I11" s="8" t="n">
+      <c r="I11" s="7" t="n">
         <v>1.122E-008</v>
       </c>
-      <c r="J11" s="8" t="n">
+      <c r="J11" s="7" t="n">
         <v>1.7783E-008</v>
       </c>
-      <c r="K11" s="8" t="n">
+      <c r="K11" s="7" t="n">
         <v>0.3094561272</v>
       </c>
-      <c r="L11" s="8" t="n">
+      <c r="L11" s="7" t="n">
         <v>10708922.6</v>
       </c>
       <c r="M11" s="4" t="s">
@@ -4977,11 +4978,11 @@
         <v>33</v>
       </c>
       <c r="H12" s="0"/>
-      <c r="I12" s="8" t="n">
+      <c r="I12" s="7" t="n">
         <v>0.001</v>
       </c>
-      <c r="J12" s="9"/>
-      <c r="K12" s="8" t="n">
+      <c r="J12" s="8"/>
+      <c r="K12" s="7" t="n">
         <v>27580.76</v>
       </c>
       <c r="L12" s="0"/>
@@ -5016,16 +5017,16 @@
         <v>33</v>
       </c>
       <c r="H13" s="0"/>
-      <c r="I13" s="8" t="n">
+      <c r="I13" s="7" t="n">
         <v>0.005</v>
       </c>
-      <c r="J13" s="8" t="n">
+      <c r="J13" s="7" t="n">
         <v>0.02</v>
       </c>
-      <c r="K13" s="8" t="n">
+      <c r="K13" s="7" t="n">
         <v>137903.8</v>
       </c>
-      <c r="L13" s="8" t="n">
+      <c r="L13" s="7" t="n">
         <v>12044000000000</v>
       </c>
       <c r="M13" s="4" t="s">
@@ -5061,16 +5062,16 @@
         <v>33</v>
       </c>
       <c r="H14" s="0"/>
-      <c r="I14" s="8" t="n">
+      <c r="I14" s="7" t="n">
         <v>55</v>
       </c>
-      <c r="J14" s="8" t="n">
+      <c r="J14" s="7" t="n">
         <v>55</v>
       </c>
-      <c r="K14" s="8" t="n">
+      <c r="K14" s="7" t="n">
         <v>1516941800</v>
       </c>
-      <c r="L14" s="8" t="n">
+      <c r="L14" s="7" t="n">
         <v>33121000000000000</v>
       </c>
       <c r="M14" s="4" t="s">
@@ -5108,11 +5109,11 @@
       <c r="H15" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="I15" s="8" t="n">
+      <c r="I15" s="7" t="n">
         <v>0.0005</v>
       </c>
-      <c r="J15" s="9"/>
-      <c r="K15" s="8" t="n">
+      <c r="J15" s="8"/>
+      <c r="K15" s="7" t="n">
         <v>13790.38</v>
       </c>
       <c r="L15" s="0"/>
@@ -5149,11 +5150,11 @@
       <c r="H16" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="I16" s="8" t="n">
+      <c r="I16" s="7" t="n">
         <v>0.0005</v>
       </c>
-      <c r="J16" s="9"/>
-      <c r="K16" s="8" t="n">
+      <c r="J16" s="8"/>
+      <c r="K16" s="7" t="n">
         <v>13790.38</v>
       </c>
       <c r="L16" s="0"/>
@@ -5190,11 +5191,11 @@
       <c r="H17" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="I17" s="8" t="n">
+      <c r="I17" s="7" t="n">
         <v>0.0005</v>
       </c>
-      <c r="J17" s="9"/>
-      <c r="K17" s="8" t="n">
+      <c r="J17" s="8"/>
+      <c r="K17" s="7" t="n">
         <v>13790.38</v>
       </c>
       <c r="L17" s="0"/>
@@ -5231,11 +5232,11 @@
       <c r="H18" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="I18" s="8" t="n">
+      <c r="I18" s="7" t="n">
         <v>0.0005</v>
       </c>
-      <c r="J18" s="9"/>
-      <c r="K18" s="8" t="n">
+      <c r="J18" s="8"/>
+      <c r="K18" s="7" t="n">
         <v>13790.38</v>
       </c>
       <c r="L18" s="0"/>
@@ -5272,11 +5273,11 @@
       <c r="H19" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="I19" s="8" t="n">
+      <c r="I19" s="7" t="n">
         <v>0.0005</v>
       </c>
-      <c r="J19" s="9"/>
-      <c r="K19" s="8" t="n">
+      <c r="J19" s="8"/>
+      <c r="K19" s="7" t="n">
         <v>13790.38</v>
       </c>
       <c r="L19" s="0"/>
@@ -5313,11 +5314,11 @@
       <c r="H20" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="I20" s="8" t="n">
+      <c r="I20" s="7" t="n">
         <v>0.0005</v>
       </c>
-      <c r="J20" s="9"/>
-      <c r="K20" s="8" t="n">
+      <c r="J20" s="8"/>
+      <c r="K20" s="7" t="n">
         <v>13790.38</v>
       </c>
       <c r="L20" s="0"/>
@@ -5354,11 +5355,11 @@
       <c r="H21" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="I21" s="8" t="n">
+      <c r="I21" s="7" t="n">
         <v>0.0005</v>
       </c>
-      <c r="J21" s="9"/>
-      <c r="K21" s="8" t="n">
+      <c r="J21" s="8"/>
+      <c r="K21" s="7" t="n">
         <v>13790.38</v>
       </c>
       <c r="L21" s="0"/>
@@ -5395,11 +5396,11 @@
       <c r="H22" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="I22" s="8" t="n">
+      <c r="I22" s="7" t="n">
         <v>0.0005</v>
       </c>
-      <c r="J22" s="9"/>
-      <c r="K22" s="8" t="n">
+      <c r="J22" s="8"/>
+      <c r="K22" s="7" t="n">
         <v>13790.38</v>
       </c>
       <c r="L22" s="0"/>
@@ -5436,11 +5437,11 @@
       <c r="H23" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="I23" s="8" t="n">
+      <c r="I23" s="7" t="n">
         <v>0.0005</v>
       </c>
-      <c r="J23" s="9"/>
-      <c r="K23" s="8" t="n">
+      <c r="J23" s="8"/>
+      <c r="K23" s="7" t="n">
         <v>13790.38</v>
       </c>
       <c r="L23" s="0"/>
@@ -5477,11 +5478,11 @@
       <c r="H24" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="I24" s="8" t="n">
+      <c r="I24" s="7" t="n">
         <v>0.0005</v>
       </c>
-      <c r="J24" s="9"/>
-      <c r="K24" s="8" t="n">
+      <c r="J24" s="8"/>
+      <c r="K24" s="7" t="n">
         <v>13790.38</v>
       </c>
       <c r="L24" s="0"/>
@@ -5518,11 +5519,11 @@
       <c r="H25" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="I25" s="8" t="n">
+      <c r="I25" s="7" t="n">
         <v>0.0005</v>
       </c>
-      <c r="J25" s="9"/>
-      <c r="K25" s="8" t="n">
+      <c r="J25" s="8"/>
+      <c r="K25" s="7" t="n">
         <v>13790.38</v>
       </c>
       <c r="L25" s="0"/>
@@ -5559,11 +5560,11 @@
       <c r="H26" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="I26" s="8" t="n">
+      <c r="I26" s="7" t="n">
         <v>0.0005</v>
       </c>
-      <c r="J26" s="9"/>
-      <c r="K26" s="8" t="n">
+      <c r="J26" s="8"/>
+      <c r="K26" s="7" t="n">
         <v>13790.38</v>
       </c>
       <c r="L26" s="0"/>
@@ -5600,11 +5601,11 @@
       <c r="H27" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="I27" s="8" t="n">
+      <c r="I27" s="7" t="n">
         <v>0.0005</v>
       </c>
-      <c r="J27" s="9"/>
-      <c r="K27" s="8" t="n">
+      <c r="J27" s="8"/>
+      <c r="K27" s="7" t="n">
         <v>13790.38</v>
       </c>
       <c r="L27" s="0"/>
@@ -5641,11 +5642,11 @@
       <c r="H28" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="I28" s="8" t="n">
+      <c r="I28" s="7" t="n">
         <v>0.0005</v>
       </c>
-      <c r="J28" s="9"/>
-      <c r="K28" s="8" t="n">
+      <c r="J28" s="8"/>
+      <c r="K28" s="7" t="n">
         <v>13790.38</v>
       </c>
       <c r="L28" s="0"/>
@@ -5682,11 +5683,11 @@
       <c r="H29" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="I29" s="8" t="n">
+      <c r="I29" s="7" t="n">
         <v>0.0005</v>
       </c>
-      <c r="J29" s="9"/>
-      <c r="K29" s="8" t="n">
+      <c r="J29" s="8"/>
+      <c r="K29" s="7" t="n">
         <v>13790.38</v>
       </c>
       <c r="L29" s="0"/>
@@ -5723,11 +5724,11 @@
       <c r="H30" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="I30" s="8" t="n">
+      <c r="I30" s="7" t="n">
         <v>0.0005</v>
       </c>
-      <c r="J30" s="9"/>
-      <c r="K30" s="8" t="n">
+      <c r="J30" s="8"/>
+      <c r="K30" s="7" t="n">
         <v>13790.38</v>
       </c>
       <c r="L30" s="0"/>
@@ -5764,11 +5765,11 @@
       <c r="H31" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="I31" s="8" t="n">
+      <c r="I31" s="7" t="n">
         <v>0.0005</v>
       </c>
-      <c r="J31" s="9"/>
-      <c r="K31" s="8" t="n">
+      <c r="J31" s="8"/>
+      <c r="K31" s="7" t="n">
         <v>13790.38</v>
       </c>
       <c r="L31" s="0"/>
@@ -5805,11 +5806,11 @@
       <c r="H32" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="I32" s="8" t="n">
+      <c r="I32" s="7" t="n">
         <v>0.0005</v>
       </c>
-      <c r="J32" s="9"/>
-      <c r="K32" s="8" t="n">
+      <c r="J32" s="8"/>
+      <c r="K32" s="7" t="n">
         <v>13790.38</v>
       </c>
       <c r="L32" s="0"/>
@@ -5846,11 +5847,11 @@
       <c r="H33" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="I33" s="8" t="n">
+      <c r="I33" s="7" t="n">
         <v>0.0005</v>
       </c>
-      <c r="J33" s="9"/>
-      <c r="K33" s="8" t="n">
+      <c r="J33" s="8"/>
+      <c r="K33" s="7" t="n">
         <v>13790.38</v>
       </c>
       <c r="L33" s="0"/>
@@ -5887,11 +5888,11 @@
       <c r="H34" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="I34" s="8" t="n">
+      <c r="I34" s="7" t="n">
         <v>0.0005</v>
       </c>
-      <c r="J34" s="9"/>
-      <c r="K34" s="8" t="n">
+      <c r="J34" s="8"/>
+      <c r="K34" s="7" t="n">
         <v>13790.38</v>
       </c>
       <c r="L34" s="0"/>
@@ -5924,11 +5925,11 @@
         <v>160</v>
       </c>
       <c r="H35" s="0"/>
-      <c r="I35" s="8" t="n">
+      <c r="I35" s="7" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J35" s="9"/>
-      <c r="K35" s="8" t="n">
+      <c r="J35" s="8"/>
+      <c r="K35" s="7" t="n">
         <v>5</v>
       </c>
       <c r="L35" s="0"/>
@@ -5961,11 +5962,11 @@
         <v>160</v>
       </c>
       <c r="H36" s="0"/>
-      <c r="I36" s="8" t="n">
+      <c r="I36" s="7" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J36" s="9"/>
-      <c r="K36" s="8" t="n">
+      <c r="J36" s="8"/>
+      <c r="K36" s="7" t="n">
         <v>5</v>
       </c>
       <c r="L36" s="0"/>
@@ -5998,11 +5999,11 @@
         <v>160</v>
       </c>
       <c r="H37" s="0"/>
-      <c r="I37" s="8" t="n">
+      <c r="I37" s="7" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J37" s="9"/>
-      <c r="K37" s="8" t="n">
+      <c r="J37" s="8"/>
+      <c r="K37" s="7" t="n">
         <v>5</v>
       </c>
       <c r="L37" s="0"/>
@@ -6033,11 +6034,11 @@
       <c r="H38" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I38" s="8" t="n">
+      <c r="I38" s="7" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J38" s="9"/>
-      <c r="K38" s="8" t="n">
+      <c r="J38" s="8"/>
+      <c r="K38" s="7" t="n">
         <v>5</v>
       </c>
       <c r="L38" s="0"/>
@@ -6072,11 +6073,11 @@
       <c r="H39" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I39" s="8" t="n">
+      <c r="I39" s="7" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J39" s="9"/>
-      <c r="K39" s="8" t="n">
+      <c r="J39" s="8"/>
+      <c r="K39" s="7" t="n">
         <v>5</v>
       </c>
       <c r="L39" s="0"/>
@@ -6111,11 +6112,11 @@
       <c r="H40" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I40" s="8" t="n">
+      <c r="I40" s="7" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J40" s="9"/>
-      <c r="K40" s="8" t="n">
+      <c r="J40" s="8"/>
+      <c r="K40" s="7" t="n">
         <v>5</v>
       </c>
       <c r="L40" s="0"/>
@@ -6150,11 +6151,11 @@
       <c r="H41" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I41" s="8" t="n">
+      <c r="I41" s="7" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J41" s="9"/>
-      <c r="K41" s="8" t="n">
+      <c r="J41" s="8"/>
+      <c r="K41" s="7" t="n">
         <v>5</v>
       </c>
       <c r="L41" s="0"/>
@@ -6189,11 +6190,11 @@
       <c r="H42" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I42" s="8" t="n">
+      <c r="I42" s="7" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J42" s="9"/>
-      <c r="K42" s="8" t="n">
+      <c r="J42" s="8"/>
+      <c r="K42" s="7" t="n">
         <v>5</v>
       </c>
       <c r="L42" s="0"/>
@@ -6228,11 +6229,11 @@
       <c r="H43" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I43" s="8" t="n">
+      <c r="I43" s="7" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J43" s="9"/>
-      <c r="K43" s="8" t="n">
+      <c r="J43" s="8"/>
+      <c r="K43" s="7" t="n">
         <v>5</v>
       </c>
       <c r="L43" s="0"/>
@@ -6267,11 +6268,11 @@
       <c r="H44" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I44" s="8" t="n">
+      <c r="I44" s="7" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J44" s="9"/>
-      <c r="K44" s="8" t="n">
+      <c r="J44" s="8"/>
+      <c r="K44" s="7" t="n">
         <v>5</v>
       </c>
       <c r="L44" s="0"/>
@@ -6306,11 +6307,11 @@
       <c r="H45" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I45" s="8" t="n">
+      <c r="I45" s="7" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J45" s="9"/>
-      <c r="K45" s="8" t="n">
+      <c r="J45" s="8"/>
+      <c r="K45" s="7" t="n">
         <v>5</v>
       </c>
       <c r="L45" s="0"/>
@@ -6345,11 +6346,11 @@
       <c r="H46" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I46" s="8" t="n">
+      <c r="I46" s="7" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J46" s="9"/>
-      <c r="K46" s="8" t="n">
+      <c r="J46" s="8"/>
+      <c r="K46" s="7" t="n">
         <v>5</v>
       </c>
       <c r="L46" s="0"/>
@@ -6384,11 +6385,11 @@
       <c r="H47" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I47" s="8" t="n">
+      <c r="I47" s="7" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J47" s="9"/>
-      <c r="K47" s="8" t="n">
+      <c r="J47" s="8"/>
+      <c r="K47" s="7" t="n">
         <v>5</v>
       </c>
       <c r="L47" s="0"/>
@@ -6423,11 +6424,11 @@
       <c r="H48" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I48" s="8" t="n">
+      <c r="I48" s="7" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J48" s="9"/>
-      <c r="K48" s="8" t="n">
+      <c r="J48" s="8"/>
+      <c r="K48" s="7" t="n">
         <v>5</v>
       </c>
       <c r="L48" s="0"/>
@@ -6462,11 +6463,11 @@
       <c r="H49" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I49" s="8" t="n">
+      <c r="I49" s="7" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J49" s="9"/>
-      <c r="K49" s="8" t="n">
+      <c r="J49" s="8"/>
+      <c r="K49" s="7" t="n">
         <v>5</v>
       </c>
       <c r="L49" s="0"/>
@@ -6501,11 +6502,11 @@
       <c r="H50" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I50" s="8" t="n">
+      <c r="I50" s="7" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J50" s="9"/>
-      <c r="K50" s="8" t="n">
+      <c r="J50" s="8"/>
+      <c r="K50" s="7" t="n">
         <v>5</v>
       </c>
       <c r="L50" s="0"/>
@@ -6540,11 +6541,11 @@
       <c r="H51" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I51" s="8" t="n">
+      <c r="I51" s="7" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J51" s="9"/>
-      <c r="K51" s="8" t="n">
+      <c r="J51" s="8"/>
+      <c r="K51" s="7" t="n">
         <v>5</v>
       </c>
       <c r="L51" s="0"/>
@@ -6579,11 +6580,11 @@
       <c r="H52" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I52" s="8" t="n">
+      <c r="I52" s="7" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J52" s="9"/>
-      <c r="K52" s="8" t="n">
+      <c r="J52" s="8"/>
+      <c r="K52" s="7" t="n">
         <v>5</v>
       </c>
       <c r="L52" s="0"/>
@@ -6618,11 +6619,11 @@
       <c r="H53" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I53" s="8" t="n">
+      <c r="I53" s="7" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J53" s="9"/>
-      <c r="K53" s="8" t="n">
+      <c r="J53" s="8"/>
+      <c r="K53" s="7" t="n">
         <v>5</v>
       </c>
       <c r="L53" s="0"/>
@@ -6657,11 +6658,11 @@
       <c r="H54" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I54" s="8" t="n">
+      <c r="I54" s="7" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J54" s="9"/>
-      <c r="K54" s="8" t="n">
+      <c r="J54" s="8"/>
+      <c r="K54" s="7" t="n">
         <v>5</v>
       </c>
       <c r="L54" s="0"/>
@@ -6696,11 +6697,11 @@
       <c r="H55" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I55" s="8" t="n">
+      <c r="I55" s="7" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J55" s="9"/>
-      <c r="K55" s="8" t="n">
+      <c r="J55" s="8"/>
+      <c r="K55" s="7" t="n">
         <v>5</v>
       </c>
       <c r="L55" s="0"/>
@@ -6735,11 +6736,11 @@
       <c r="H56" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I56" s="8" t="n">
+      <c r="I56" s="7" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J56" s="9"/>
-      <c r="K56" s="8" t="n">
+      <c r="J56" s="8"/>
+      <c r="K56" s="7" t="n">
         <v>5</v>
       </c>
       <c r="L56" s="0"/>
@@ -6774,11 +6775,11 @@
       <c r="H57" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I57" s="8" t="n">
+      <c r="I57" s="7" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J57" s="9"/>
-      <c r="K57" s="8" t="n">
+      <c r="J57" s="8"/>
+      <c r="K57" s="7" t="n">
         <v>5</v>
       </c>
       <c r="L57" s="0"/>
@@ -6813,11 +6814,11 @@
       <c r="H58" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I58" s="8" t="n">
+      <c r="I58" s="7" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J58" s="9"/>
-      <c r="K58" s="8" t="n">
+      <c r="J58" s="8"/>
+      <c r="K58" s="7" t="n">
         <v>5</v>
       </c>
       <c r="L58" s="0"/>
@@ -6852,11 +6853,11 @@
       <c r="H59" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I59" s="8" t="n">
+      <c r="I59" s="7" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J59" s="9"/>
-      <c r="K59" s="8" t="n">
+      <c r="J59" s="8"/>
+      <c r="K59" s="7" t="n">
         <v>5</v>
       </c>
       <c r="L59" s="0"/>
@@ -6891,11 +6892,11 @@
       <c r="H60" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I60" s="8" t="n">
+      <c r="I60" s="7" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J60" s="9"/>
-      <c r="K60" s="8" t="n">
+      <c r="J60" s="8"/>
+      <c r="K60" s="7" t="n">
         <v>5</v>
       </c>
       <c r="L60" s="0"/>
@@ -6930,11 +6931,11 @@
       <c r="H61" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I61" s="8" t="n">
+      <c r="I61" s="7" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J61" s="9"/>
-      <c r="K61" s="8" t="n">
+      <c r="J61" s="8"/>
+      <c r="K61" s="7" t="n">
         <v>5</v>
       </c>
       <c r="L61" s="0"/>
@@ -6969,11 +6970,11 @@
       <c r="H62" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I62" s="8" t="n">
+      <c r="I62" s="7" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J62" s="9"/>
-      <c r="K62" s="8" t="n">
+      <c r="J62" s="8"/>
+      <c r="K62" s="7" t="n">
         <v>5</v>
       </c>
       <c r="L62" s="0"/>
@@ -7008,11 +7009,11 @@
       <c r="H63" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I63" s="8" t="n">
+      <c r="I63" s="7" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J63" s="9"/>
-      <c r="K63" s="8" t="n">
+      <c r="J63" s="8"/>
+      <c r="K63" s="7" t="n">
         <v>5</v>
       </c>
       <c r="L63" s="0"/>
@@ -7047,11 +7048,11 @@
       <c r="H64" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I64" s="8" t="n">
+      <c r="I64" s="7" t="n">
         <v>1.81285794880199E-007</v>
       </c>
-      <c r="J64" s="9"/>
-      <c r="K64" s="8" t="n">
+      <c r="J64" s="8"/>
+      <c r="K64" s="7" t="n">
         <v>5</v>
       </c>
       <c r="L64" s="0"/>
@@ -7084,11 +7085,11 @@
         <v>257</v>
       </c>
       <c r="H65" s="0"/>
-      <c r="I65" s="8" t="n">
+      <c r="I65" s="7" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J65" s="9"/>
-      <c r="K65" s="8" t="n">
+      <c r="J65" s="8"/>
+      <c r="K65" s="7" t="n">
         <v>1000</v>
       </c>
       <c r="L65" s="0"/>
@@ -7121,11 +7122,11 @@
         <v>257</v>
       </c>
       <c r="H66" s="0"/>
-      <c r="I66" s="8" t="n">
+      <c r="I66" s="7" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J66" s="9"/>
-      <c r="K66" s="8" t="n">
+      <c r="J66" s="8"/>
+      <c r="K66" s="7" t="n">
         <v>1000</v>
       </c>
       <c r="L66" s="0"/>
@@ -7158,11 +7159,11 @@
         <v>257</v>
       </c>
       <c r="H67" s="0"/>
-      <c r="I67" s="8" t="n">
+      <c r="I67" s="7" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J67" s="9"/>
-      <c r="K67" s="8" t="n">
+      <c r="J67" s="8"/>
+      <c r="K67" s="7" t="n">
         <v>1000</v>
       </c>
       <c r="L67" s="0"/>
@@ -7193,11 +7194,11 @@
       <c r="H68" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I68" s="8" t="n">
+      <c r="I68" s="7" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J68" s="9"/>
-      <c r="K68" s="8" t="n">
+      <c r="J68" s="8"/>
+      <c r="K68" s="7" t="n">
         <v>1000</v>
       </c>
       <c r="L68" s="0"/>
@@ -7232,11 +7233,11 @@
       <c r="H69" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I69" s="8" t="n">
+      <c r="I69" s="7" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J69" s="9"/>
-      <c r="K69" s="8" t="n">
+      <c r="J69" s="8"/>
+      <c r="K69" s="7" t="n">
         <v>1000</v>
       </c>
       <c r="L69" s="0"/>
@@ -7271,11 +7272,11 @@
       <c r="H70" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I70" s="8" t="n">
+      <c r="I70" s="7" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J70" s="9"/>
-      <c r="K70" s="8" t="n">
+      <c r="J70" s="8"/>
+      <c r="K70" s="7" t="n">
         <v>1000</v>
       </c>
       <c r="L70" s="0"/>
@@ -7310,11 +7311,11 @@
       <c r="H71" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I71" s="8" t="n">
+      <c r="I71" s="7" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J71" s="9"/>
-      <c r="K71" s="8" t="n">
+      <c r="J71" s="8"/>
+      <c r="K71" s="7" t="n">
         <v>1000</v>
       </c>
       <c r="L71" s="0"/>
@@ -7349,11 +7350,11 @@
       <c r="H72" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I72" s="8" t="n">
+      <c r="I72" s="7" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J72" s="9"/>
-      <c r="K72" s="8" t="n">
+      <c r="J72" s="8"/>
+      <c r="K72" s="7" t="n">
         <v>1000</v>
       </c>
       <c r="L72" s="0"/>
@@ -7388,11 +7389,11 @@
       <c r="H73" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I73" s="8" t="n">
+      <c r="I73" s="7" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J73" s="9"/>
-      <c r="K73" s="8" t="n">
+      <c r="J73" s="8"/>
+      <c r="K73" s="7" t="n">
         <v>1000</v>
       </c>
       <c r="L73" s="0"/>
@@ -7427,11 +7428,11 @@
       <c r="H74" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I74" s="8" t="n">
+      <c r="I74" s="7" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J74" s="9"/>
-      <c r="K74" s="8" t="n">
+      <c r="J74" s="8"/>
+      <c r="K74" s="7" t="n">
         <v>1000</v>
       </c>
       <c r="L74" s="0"/>
@@ -7466,11 +7467,11 @@
       <c r="H75" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I75" s="8" t="n">
+      <c r="I75" s="7" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J75" s="9"/>
-      <c r="K75" s="8" t="n">
+      <c r="J75" s="8"/>
+      <c r="K75" s="7" t="n">
         <v>1000</v>
       </c>
       <c r="L75" s="0"/>
@@ -7505,11 +7506,11 @@
       <c r="H76" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I76" s="8" t="n">
+      <c r="I76" s="7" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J76" s="9"/>
-      <c r="K76" s="8" t="n">
+      <c r="J76" s="8"/>
+      <c r="K76" s="7" t="n">
         <v>1000</v>
       </c>
       <c r="L76" s="0"/>
@@ -7544,11 +7545,11 @@
       <c r="H77" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I77" s="8" t="n">
+      <c r="I77" s="7" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J77" s="9"/>
-      <c r="K77" s="8" t="n">
+      <c r="J77" s="8"/>
+      <c r="K77" s="7" t="n">
         <v>1000</v>
       </c>
       <c r="L77" s="0"/>
@@ -7583,11 +7584,11 @@
       <c r="H78" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I78" s="8" t="n">
+      <c r="I78" s="7" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J78" s="9"/>
-      <c r="K78" s="8" t="n">
+      <c r="J78" s="8"/>
+      <c r="K78" s="7" t="n">
         <v>1000</v>
       </c>
       <c r="L78" s="0"/>
@@ -7622,11 +7623,11 @@
       <c r="H79" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I79" s="8" t="n">
+      <c r="I79" s="7" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J79" s="9"/>
-      <c r="K79" s="8" t="n">
+      <c r="J79" s="8"/>
+      <c r="K79" s="7" t="n">
         <v>1000</v>
       </c>
       <c r="L79" s="0"/>
@@ -7661,11 +7662,11 @@
       <c r="H80" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I80" s="8" t="n">
+      <c r="I80" s="7" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J80" s="9"/>
-      <c r="K80" s="8" t="n">
+      <c r="J80" s="8"/>
+      <c r="K80" s="7" t="n">
         <v>1000</v>
       </c>
       <c r="L80" s="0"/>
@@ -7700,11 +7701,11 @@
       <c r="H81" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I81" s="8" t="n">
+      <c r="I81" s="7" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J81" s="9"/>
-      <c r="K81" s="8" t="n">
+      <c r="J81" s="8"/>
+      <c r="K81" s="7" t="n">
         <v>1000</v>
       </c>
       <c r="L81" s="0"/>
@@ -7739,11 +7740,11 @@
       <c r="H82" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I82" s="8" t="n">
+      <c r="I82" s="7" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J82" s="9"/>
-      <c r="K82" s="8" t="n">
+      <c r="J82" s="8"/>
+      <c r="K82" s="7" t="n">
         <v>1000</v>
       </c>
       <c r="L82" s="0"/>
@@ -7778,11 +7779,11 @@
       <c r="H83" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I83" s="8" t="n">
+      <c r="I83" s="7" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J83" s="9"/>
-      <c r="K83" s="8" t="n">
+      <c r="J83" s="8"/>
+      <c r="K83" s="7" t="n">
         <v>1000</v>
       </c>
       <c r="L83" s="0"/>
@@ -7817,11 +7818,11 @@
       <c r="H84" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I84" s="8" t="n">
+      <c r="I84" s="7" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J84" s="9"/>
-      <c r="K84" s="8" t="n">
+      <c r="J84" s="8"/>
+      <c r="K84" s="7" t="n">
         <v>1000</v>
       </c>
       <c r="L84" s="0"/>
@@ -7856,11 +7857,11 @@
       <c r="H85" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I85" s="8" t="n">
+      <c r="I85" s="7" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J85" s="9"/>
-      <c r="K85" s="8" t="n">
+      <c r="J85" s="8"/>
+      <c r="K85" s="7" t="n">
         <v>1000</v>
       </c>
       <c r="L85" s="0"/>
@@ -7895,11 +7896,11 @@
       <c r="H86" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I86" s="8" t="n">
+      <c r="I86" s="7" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J86" s="9"/>
-      <c r="K86" s="8" t="n">
+      <c r="J86" s="8"/>
+      <c r="K86" s="7" t="n">
         <v>1000</v>
       </c>
       <c r="L86" s="0"/>
@@ -7934,11 +7935,11 @@
       <c r="H87" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I87" s="8" t="n">
+      <c r="I87" s="7" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J87" s="9"/>
-      <c r="K87" s="8" t="n">
+      <c r="J87" s="8"/>
+      <c r="K87" s="7" t="n">
         <v>1000</v>
       </c>
       <c r="L87" s="0"/>
@@ -7973,11 +7974,11 @@
       <c r="H88" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I88" s="8" t="n">
+      <c r="I88" s="7" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J88" s="9"/>
-      <c r="K88" s="8" t="n">
+      <c r="J88" s="8"/>
+      <c r="K88" s="7" t="n">
         <v>1000</v>
       </c>
       <c r="L88" s="0"/>
@@ -8012,11 +8013,11 @@
       <c r="H89" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I89" s="8" t="n">
+      <c r="I89" s="7" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J89" s="9"/>
-      <c r="K89" s="8" t="n">
+      <c r="J89" s="8"/>
+      <c r="K89" s="7" t="n">
         <v>1000</v>
       </c>
       <c r="L89" s="0"/>
@@ -8051,11 +8052,11 @@
       <c r="H90" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I90" s="8" t="n">
+      <c r="I90" s="7" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J90" s="9"/>
-      <c r="K90" s="8" t="n">
+      <c r="J90" s="8"/>
+      <c r="K90" s="7" t="n">
         <v>1000</v>
       </c>
       <c r="L90" s="0"/>
@@ -8090,11 +8091,11 @@
       <c r="H91" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I91" s="8" t="n">
+      <c r="I91" s="7" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J91" s="9"/>
-      <c r="K91" s="8" t="n">
+      <c r="J91" s="8"/>
+      <c r="K91" s="7" t="n">
         <v>1000</v>
       </c>
       <c r="L91" s="0"/>
@@ -8129,11 +8130,11 @@
       <c r="H92" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I92" s="8" t="n">
+      <c r="I92" s="7" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J92" s="9"/>
-      <c r="K92" s="8" t="n">
+      <c r="J92" s="8"/>
+      <c r="K92" s="7" t="n">
         <v>1000</v>
       </c>
       <c r="L92" s="0"/>
@@ -8168,11 +8169,11 @@
       <c r="H93" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I93" s="8" t="n">
+      <c r="I93" s="7" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J93" s="9"/>
-      <c r="K93" s="8" t="n">
+      <c r="J93" s="8"/>
+      <c r="K93" s="7" t="n">
         <v>1000</v>
       </c>
       <c r="L93" s="0"/>
@@ -8207,11 +8208,11 @@
       <c r="H94" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I94" s="8" t="n">
+      <c r="I94" s="7" t="n">
         <v>3.62571589760398E-005</v>
       </c>
-      <c r="J94" s="9"/>
-      <c r="K94" s="8" t="n">
+      <c r="J94" s="8"/>
+      <c r="K94" s="7" t="n">
         <v>1000</v>
       </c>
       <c r="L94" s="0"/>
@@ -8245,11 +8246,11 @@
       <c r="G95" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I95" s="8"/>
-      <c r="J95" s="8" t="n">
+      <c r="I95" s="7"/>
+      <c r="J95" s="7" t="n">
         <v>0.000148</v>
       </c>
-      <c r="L95" s="8" t="n">
+      <c r="L95" s="7" t="n">
         <v>89125600000</v>
       </c>
       <c r="M95" s="4" t="s">
@@ -8284,8 +8285,8 @@
       <c r="G96" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I96" s="8"/>
-      <c r="J96" s="9"/>
+      <c r="I96" s="7"/>
+      <c r="J96" s="8"/>
       <c r="L96" s="0"/>
       <c r="M96" s="4" t="s">
         <v>35</v>
@@ -8317,11 +8318,11 @@
       <c r="G97" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I97" s="8"/>
-      <c r="J97" s="8" t="n">
+      <c r="I97" s="7"/>
+      <c r="J97" s="7" t="n">
         <v>0.00727552</v>
       </c>
-      <c r="L97" s="8" t="n">
+      <c r="L97" s="7" t="n">
         <v>4381318144000</v>
       </c>
       <c r="M97" s="4" t="s">
@@ -8356,11 +8357,11 @@
       <c r="G98" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I98" s="8"/>
-      <c r="J98" s="8" t="n">
+      <c r="I98" s="7"/>
+      <c r="J98" s="7" t="n">
         <v>0.00305544</v>
       </c>
-      <c r="L98" s="8" t="n">
+      <c r="L98" s="7" t="n">
         <v>1839985968000</v>
       </c>
       <c r="M98" s="4" t="s">
@@ -8395,11 +8396,11 @@
       <c r="G99" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I99" s="8"/>
-      <c r="J99" s="8" t="n">
+      <c r="I99" s="7"/>
+      <c r="J99" s="7" t="n">
         <v>0.0002</v>
       </c>
-      <c r="L99" s="8" t="n">
+      <c r="L99" s="7" t="n">
         <v>120440000000</v>
       </c>
       <c r="M99" s="4" t="s">
@@ -8434,11 +8435,11 @@
       <c r="G100" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I100" s="8"/>
-      <c r="J100" s="8" t="n">
+      <c r="I100" s="7"/>
+      <c r="J100" s="7" t="n">
         <v>0.00781962</v>
       </c>
-      <c r="L100" s="8" t="n">
+      <c r="L100" s="7" t="n">
         <v>4708975164000</v>
       </c>
       <c r="M100" s="4" t="s">
@@ -8473,8 +8474,8 @@
       <c r="G101" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I101" s="8"/>
-      <c r="J101" s="9"/>
+      <c r="I101" s="7"/>
+      <c r="J101" s="8"/>
       <c r="L101" s="0"/>
       <c r="M101" s="4" t="s">
         <v>35</v>
@@ -8506,11 +8507,11 @@
       <c r="G102" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I102" s="8"/>
-      <c r="J102" s="8" t="n">
+      <c r="I102" s="7"/>
+      <c r="J102" s="7" t="n">
         <v>0.00170010200612037</v>
       </c>
-      <c r="L102" s="8" t="n">
+      <c r="L102" s="7" t="n">
         <v>1023801428085.69</v>
       </c>
       <c r="M102" s="4" t="s">
@@ -8545,11 +8546,11 @@
       <c r="G103" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I103" s="8"/>
-      <c r="J103" s="8" t="n">
+      <c r="I103" s="7"/>
+      <c r="J103" s="7" t="n">
         <v>0.00025</v>
       </c>
-      <c r="L103" s="8" t="n">
+      <c r="L103" s="7" t="n">
         <v>150550000000</v>
       </c>
       <c r="M103" s="4" t="s">
@@ -8584,11 +8585,11 @@
       <c r="G104" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I104" s="8"/>
-      <c r="J104" s="8" t="n">
+      <c r="I104" s="7"/>
+      <c r="J104" s="7" t="n">
         <v>0.00318137</v>
       </c>
-      <c r="L104" s="8" t="n">
+      <c r="L104" s="7" t="n">
         <v>1915821014000</v>
       </c>
       <c r="M104" s="4" t="s">
@@ -8623,8 +8624,8 @@
       <c r="G105" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I105" s="8"/>
-      <c r="J105" s="9"/>
+      <c r="I105" s="7"/>
+      <c r="J105" s="8"/>
       <c r="L105" s="0"/>
       <c r="M105" s="4" t="s">
         <v>35</v>
@@ -8656,8 +8657,8 @@
       <c r="G106" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I106" s="8"/>
-      <c r="J106" s="9"/>
+      <c r="I106" s="7"/>
+      <c r="J106" s="8"/>
       <c r="L106" s="0"/>
       <c r="M106" s="4" t="s">
         <v>35</v>
@@ -8689,8 +8690,8 @@
       <c r="G107" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I107" s="8"/>
-      <c r="J107" s="9"/>
+      <c r="I107" s="7"/>
+      <c r="J107" s="8"/>
       <c r="L107" s="0"/>
       <c r="M107" s="4" t="s">
         <v>35</v>
@@ -8722,8 +8723,8 @@
       <c r="G108" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I108" s="8"/>
-      <c r="J108" s="9"/>
+      <c r="I108" s="7"/>
+      <c r="J108" s="8"/>
       <c r="L108" s="0"/>
       <c r="M108" s="4" t="s">
         <v>35</v>
@@ -8755,8 +8756,8 @@
       <c r="G109" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I109" s="8"/>
-      <c r="J109" s="9"/>
+      <c r="I109" s="7"/>
+      <c r="J109" s="8"/>
       <c r="L109" s="0"/>
       <c r="M109" s="4" t="s">
         <v>35</v>
@@ -8788,8 +8789,8 @@
       <c r="G110" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I110" s="8"/>
-      <c r="J110" s="9"/>
+      <c r="I110" s="7"/>
+      <c r="J110" s="8"/>
       <c r="L110" s="0"/>
       <c r="M110" s="4" t="s">
         <v>35</v>
@@ -8821,8 +8822,8 @@
       <c r="G111" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I111" s="8"/>
-      <c r="J111" s="9"/>
+      <c r="I111" s="7"/>
+      <c r="J111" s="8"/>
       <c r="L111" s="0"/>
       <c r="M111" s="4" t="s">
         <v>35</v>
@@ -8854,11 +8855,11 @@
       <c r="G112" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I112" s="8"/>
-      <c r="J112" s="8" t="n">
+      <c r="I112" s="7"/>
+      <c r="J112" s="7" t="n">
         <v>0.0550705747828259</v>
       </c>
-      <c r="L112" s="8" t="n">
+      <c r="L112" s="7" t="n">
         <v>33163500134217.8</v>
       </c>
       <c r="M112" s="4" t="s">
@@ -8893,11 +8894,11 @@
       <c r="G113" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I113" s="8"/>
-      <c r="J113" s="8" t="n">
+      <c r="I113" s="7"/>
+      <c r="J113" s="7" t="n">
         <v>0.00013234</v>
       </c>
-      <c r="L113" s="8" t="n">
+      <c r="L113" s="7" t="n">
         <v>79695148000</v>
       </c>
       <c r="M113" s="4" t="s">
@@ -8932,11 +8933,11 @@
       <c r="G114" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I114" s="8"/>
-      <c r="J114" s="8" t="n">
+      <c r="I114" s="7"/>
+      <c r="J114" s="7" t="n">
         <v>0.000715127</v>
       </c>
-      <c r="L114" s="8" t="n">
+      <c r="L114" s="7" t="n">
         <v>430649479400</v>
       </c>
       <c r="M114" s="0"/>
@@ -8967,11 +8968,11 @@
       <c r="G115" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I115" s="8"/>
-      <c r="J115" s="8" t="n">
+      <c r="I115" s="7"/>
+      <c r="J115" s="7" t="n">
         <v>0.0134776</v>
       </c>
-      <c r="L115" s="8" t="n">
+      <c r="L115" s="7" t="n">
         <v>8116210720000</v>
       </c>
       <c r="M115" s="4" t="s">
@@ -9006,11 +9007,11 @@
       <c r="G116" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I116" s="8"/>
-      <c r="J116" s="8" t="n">
+      <c r="I116" s="7"/>
+      <c r="J116" s="7" t="n">
         <v>0.00782989</v>
       </c>
-      <c r="L116" s="8" t="n">
+      <c r="L116" s="7" t="n">
         <v>4715159758000</v>
       </c>
       <c r="M116" s="4" t="s">
@@ -9045,11 +9046,11 @@
       <c r="G117" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I117" s="8"/>
-      <c r="J117" s="8" t="n">
+      <c r="I117" s="7"/>
+      <c r="J117" s="7" t="n">
         <v>0.00238654</v>
       </c>
-      <c r="L117" s="8" t="n">
+      <c r="L117" s="7" t="n">
         <v>1437174388000</v>
       </c>
       <c r="M117" s="4" t="s">
@@ -9084,11 +9085,11 @@
       <c r="G118" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I118" s="8"/>
-      <c r="J118" s="8" t="n">
+      <c r="I118" s="7"/>
+      <c r="J118" s="7" t="n">
         <v>0.00406589</v>
       </c>
-      <c r="L118" s="8" t="n">
+      <c r="L118" s="7" t="n">
         <v>2448478958000</v>
       </c>
       <c r="M118" s="0"/>
@@ -9119,8 +9120,8 @@
       <c r="G119" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I119" s="8"/>
-      <c r="J119" s="9"/>
+      <c r="I119" s="7"/>
+      <c r="J119" s="8"/>
       <c r="L119" s="0"/>
       <c r="M119" s="4" t="s">
         <v>35</v>
@@ -9152,11 +9153,11 @@
       <c r="G120" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I120" s="8"/>
-      <c r="J120" s="8" t="n">
+      <c r="I120" s="7"/>
+      <c r="J120" s="7" t="n">
         <v>0.00781927</v>
       </c>
-      <c r="L120" s="8" t="n">
+      <c r="L120" s="7" t="n">
         <v>4708764394000</v>
       </c>
       <c r="M120" s="4" t="s">
@@ -9191,11 +9192,11 @@
       <c r="G121" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I121" s="8"/>
-      <c r="J121" s="8" t="n">
+      <c r="I121" s="7"/>
+      <c r="J121" s="7" t="n">
         <v>0.00630316</v>
       </c>
-      <c r="L121" s="8" t="n">
+      <c r="L121" s="7" t="n">
         <v>3795762952000</v>
       </c>
       <c r="M121" s="4" t="s">
@@ -9230,11 +9231,11 @@
       <c r="G122" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I122" s="8"/>
-      <c r="J122" s="8" t="n">
+      <c r="I122" s="7"/>
+      <c r="J122" s="7" t="n">
         <v>0.00179497</v>
       </c>
-      <c r="L122" s="8" t="n">
+      <c r="L122" s="7" t="n">
         <v>1080930934000</v>
       </c>
       <c r="M122" s="4" t="s">
@@ -9269,11 +9270,11 @@
       <c r="G123" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I123" s="8"/>
-      <c r="J123" s="8" t="n">
+      <c r="I123" s="7"/>
+      <c r="J123" s="7" t="n">
         <v>5.28369E-006</v>
       </c>
-      <c r="L123" s="8" t="n">
+      <c r="L123" s="7" t="n">
         <v>3181838118</v>
       </c>
       <c r="M123" s="4" t="s">
@@ -9308,8 +9309,8 @@
       <c r="G124" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I124" s="8"/>
-      <c r="J124" s="9"/>
+      <c r="I124" s="7"/>
+      <c r="J124" s="8"/>
       <c r="L124" s="0"/>
       <c r="M124" s="4" t="s">
         <v>35</v>
@@ -9341,11 +9342,11 @@
       <c r="G125" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I125" s="8"/>
-      <c r="J125" s="8" t="n">
+      <c r="I125" s="7"/>
+      <c r="J125" s="7" t="n">
         <v>0.000273010920436817</v>
       </c>
-      <c r="L125" s="8" t="n">
+      <c r="L125" s="7" t="n">
         <v>164407176287.052</v>
       </c>
       <c r="M125" s="4" t="s">
@@ -9380,8 +9381,8 @@
       <c r="G126" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I126" s="8"/>
-      <c r="J126" s="9"/>
+      <c r="I126" s="7"/>
+      <c r="J126" s="8"/>
       <c r="L126" s="0"/>
       <c r="M126" s="4" t="s">
         <v>35</v>
@@ -9413,11 +9414,11 @@
       <c r="G127" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I127" s="8"/>
-      <c r="J127" s="8" t="n">
+      <c r="I127" s="7"/>
+      <c r="J127" s="7" t="n">
         <v>0.02</v>
       </c>
-      <c r="L127" s="8" t="n">
+      <c r="L127" s="7" t="n">
         <v>12044000000000</v>
       </c>
       <c r="M127" s="4" t="s">
@@ -9452,8 +9453,8 @@
       <c r="G128" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I128" s="8"/>
-      <c r="J128" s="9"/>
+      <c r="I128" s="7"/>
+      <c r="J128" s="8"/>
       <c r="L128" s="0"/>
       <c r="M128" s="4" t="s">
         <v>35</v>
@@ -9485,8 +9486,8 @@
       <c r="G129" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I129" s="8"/>
-      <c r="J129" s="9"/>
+      <c r="I129" s="7"/>
+      <c r="J129" s="8"/>
       <c r="L129" s="0"/>
       <c r="M129" s="4" t="s">
         <v>35</v>
@@ -9518,8 +9519,8 @@
       <c r="G130" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I130" s="8"/>
-      <c r="J130" s="9"/>
+      <c r="I130" s="7"/>
+      <c r="J130" s="8"/>
       <c r="L130" s="0"/>
       <c r="M130" s="4" t="s">
         <v>35</v>
@@ -9551,11 +9552,11 @@
       <c r="G131" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I131" s="8"/>
-      <c r="J131" s="8" t="n">
+      <c r="I131" s="7"/>
+      <c r="J131" s="7" t="n">
         <v>0.00340385</v>
       </c>
-      <c r="L131" s="8" t="n">
+      <c r="L131" s="7" t="n">
         <v>2049798470000</v>
       </c>
       <c r="M131" s="4" t="s">
@@ -9590,11 +9591,11 @@
       <c r="G132" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I132" s="8"/>
-      <c r="J132" s="8" t="n">
+      <c r="I132" s="7"/>
+      <c r="J132" s="7" t="n">
         <v>0.00824728</v>
       </c>
-      <c r="L132" s="8" t="n">
+      <c r="L132" s="7" t="n">
         <v>4966512016000</v>
       </c>
       <c r="M132" s="0"/>
@@ -9625,8 +9626,8 @@
       <c r="G133" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I133" s="8"/>
-      <c r="J133" s="9"/>
+      <c r="I133" s="7"/>
+      <c r="J133" s="8"/>
       <c r="L133" s="0"/>
       <c r="M133" s="4" t="s">
         <v>35</v>
@@ -9658,8 +9659,8 @@
       <c r="G134" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I134" s="8"/>
-      <c r="J134" s="9"/>
+      <c r="I134" s="7"/>
+      <c r="J134" s="8"/>
       <c r="L134" s="0"/>
       <c r="M134" s="4" t="s">
         <v>35</v>
@@ -9691,8 +9692,8 @@
       <c r="G135" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I135" s="8"/>
-      <c r="J135" s="9"/>
+      <c r="I135" s="7"/>
+      <c r="J135" s="8"/>
       <c r="L135" s="0"/>
       <c r="M135" s="4" t="s">
         <v>35</v>
@@ -9724,11 +9725,11 @@
       <c r="G136" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I136" s="8"/>
-      <c r="J136" s="8" t="n">
+      <c r="I136" s="7"/>
+      <c r="J136" s="7" t="n">
         <v>0.0053761</v>
       </c>
-      <c r="L136" s="8" t="n">
+      <c r="L136" s="7" t="n">
         <v>3237487420000</v>
       </c>
       <c r="M136" s="4" t="s">
@@ -9763,8 +9764,8 @@
       <c r="G137" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I137" s="8"/>
-      <c r="J137" s="9"/>
+      <c r="I137" s="7"/>
+      <c r="J137" s="8"/>
       <c r="L137" s="0"/>
       <c r="M137" s="4" t="s">
         <v>35</v>
@@ -9796,8 +9797,8 @@
       <c r="G138" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I138" s="8"/>
-      <c r="J138" s="9"/>
+      <c r="I138" s="7"/>
+      <c r="J138" s="8"/>
       <c r="L138" s="0"/>
       <c r="M138" s="4" t="s">
         <v>35</v>
@@ -9829,11 +9830,11 @@
       <c r="G139" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I139" s="8"/>
-      <c r="J139" s="8" t="n">
+      <c r="I139" s="7"/>
+      <c r="J139" s="7" t="n">
         <v>0.00470492</v>
       </c>
-      <c r="L139" s="8" t="n">
+      <c r="L139" s="7" t="n">
         <v>2833302824000</v>
       </c>
       <c r="M139" s="0"/>
@@ -9864,11 +9865,11 @@
       <c r="G140" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I140" s="8"/>
-      <c r="J140" s="8" t="n">
+      <c r="I140" s="7"/>
+      <c r="J140" s="7" t="n">
         <v>0.000313168</v>
       </c>
-      <c r="L140" s="8" t="n">
+      <c r="L140" s="7" t="n">
         <v>188589769600</v>
       </c>
       <c r="M140" s="4" t="s">
@@ -9903,11 +9904,11 @@
       <c r="G141" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I141" s="8"/>
-      <c r="J141" s="8" t="n">
+      <c r="I141" s="7"/>
+      <c r="J141" s="7" t="n">
         <v>0.00112553</v>
       </c>
-      <c r="L141" s="8" t="n">
+      <c r="L141" s="7" t="n">
         <v>677794166000</v>
       </c>
       <c r="M141" s="4" t="s">
@@ -9942,8 +9943,8 @@
       <c r="G142" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I142" s="8"/>
-      <c r="J142" s="9"/>
+      <c r="I142" s="7"/>
+      <c r="J142" s="8"/>
       <c r="L142" s="0"/>
       <c r="M142" s="4" t="s">
         <v>35</v>
@@ -9975,11 +9976,11 @@
       <c r="G143" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I143" s="8"/>
-      <c r="J143" s="8" t="n">
+      <c r="I143" s="7"/>
+      <c r="J143" s="7" t="n">
         <v>0.000178433</v>
       </c>
-      <c r="L143" s="8" t="n">
+      <c r="L143" s="7" t="n">
         <v>107452352600</v>
       </c>
       <c r="M143" s="4" t="s">
@@ -10014,8 +10015,8 @@
       <c r="G144" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I144" s="8"/>
-      <c r="J144" s="9"/>
+      <c r="I144" s="7"/>
+      <c r="J144" s="8"/>
       <c r="L144" s="0"/>
       <c r="M144" s="4" t="s">
         <v>35</v>
@@ -10047,11 +10048,11 @@
       <c r="G145" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I145" s="8"/>
-      <c r="J145" s="8" t="n">
+      <c r="I145" s="7"/>
+      <c r="J145" s="7" t="n">
         <v>0.00587101</v>
       </c>
-      <c r="L145" s="8" t="n">
+      <c r="L145" s="7" t="n">
         <v>3535522222000</v>
       </c>
       <c r="M145" s="4" t="s">
@@ -10086,7 +10087,7 @@
       <c r="G146" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I146" s="8"/>
+      <c r="I146" s="7"/>
       <c r="M146" s="4" t="s">
         <v>35</v>
       </c>
@@ -10119,25 +10120,24 @@
   </sheetPr>
   <dimension ref="A1:K177"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C172" activePane="bottomRight" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B81" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A172" activeCellId="0" sqref="A172"/>
-      <selection pane="bottomRight" activeCell="D177" activeCellId="0" sqref="D177"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A81" activeCellId="0" sqref="A81"/>
+      <selection pane="bottomRight" activeCell="F92" activeCellId="0" sqref="F92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="18.6396761133603"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.9230769230769"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.9959514170041"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="36.3117408906883"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.1052631578947"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="36.6356275303644"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="24.1012145748988"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="9.4251012145749"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="10.2834008097166"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="25.2793522267206"/>
+    <col collapsed="false" hidden="false" max="10" min="8" style="1" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="25.4939271255061"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -10160,10 +10160,10 @@
       <c r="F1" s="2" t="s">
         <v>577</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="10" t="s">
         <v>578</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="10" t="s">
         <v>579</v>
       </c>
       <c r="I1" s="2" t="s">
@@ -15719,9 +15719,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.0323886639676"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="42.9554655870445"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="43.3846153846154"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.9595141700405"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="6" min="5" style="1" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="8.57085020242915"/>
@@ -15868,10 +15868,10 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="28.1740890688259"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="10.2834008097166"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="18.2105263157895"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="28.3846153846154"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.2834008097166"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
fixing translation rate laws
</commit_message>
<xml_diff>
--- a/data/Model.xlsx
+++ b/data/Model.xlsx
@@ -3099,7 +3099,7 @@
     <t>[c]: (2) ALA + (11) ARG + (4) ASP + (2) ASN + (3) CYS + (1) GLN + (4) GLU + (1) GLY + (4) HIS + (7) ILE + (8) LEU + (4) LYS + (3) MET + (2) PHE + (9) PRO + (4) SER + (6) THR + (3) TRP + (7) TYR + (15) VAL + (203) GTP + (104) H2O ==&gt; RnaPolymerase-Protein + (200) GDP + (200) PI + (200) H</t>
   </si>
   <si>
-    <t>Vmax * min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c]) / (Km + min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c])) * RnaPolymerase-Rna[c] * Ribosome-Protein[c]</t>
+    <t>Vmax * min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c]) / (Km + min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c])) * RnaPolymerase-Rna[c] * Ribosome-Protein[c]</t>
   </si>
   <si>
     <t>2.3.2.12</t>
@@ -3114,7 +3114,7 @@
     <t>[c]: (7) ALA + (10) ARG + (3) ASP + (4) ASN + (3) CYS + (3) GLN + (1) GLU + (6) GLY + (1) HIS + (8) ILE + (9) LEU + (3) LYS + (2) MET + (6) PHE + (10) PRO + (7) SER + (9) THR + (3) TRP + (0) TYR + (5) VAL + (203) GTP + (104) H2O ==&gt; Ribosome-Protein + (200) GDP + (200) PI + (200) H</t>
   </si>
   <si>
-    <t>Vmax * min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c]) / (Km + min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c])) * Ribosome-Rna[c] * Ribosome-Protein[c]</t>
+    <t>Vmax * min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c]) / (Km + min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c])) * Ribosome-Rna[c] * Ribosome-Protein[c]</t>
   </si>
   <si>
     <t>Translation-Rnase</t>
@@ -3126,7 +3126,7 @@
     <t>[c]: (10) ALA + (11) ARG + (4) ASP + (2) ASN + (2) CYS + (3) GLN + (6) GLU + (3) GLY + (0) HIS + (3) ILE + (9) LEU + (0) LYS + (4) MET + (2) PHE + (9) PRO + (10) SER + (8) THR + (7) TRP + (0) TYR + (7) VAL + (203) GTP + (104) H2O ==&gt; Rnase-Protein + (200) GDP + (200) PI + (200) H</t>
   </si>
   <si>
-    <t>Vmax * min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c]) / (Km + min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c])) * Rnase-Rna[c] * Ribosome-Protein[c]</t>
+    <t>Vmax * min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c]) / (Km + min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c])) * Rnase-Rna[c] * Ribosome-Protein[c]</t>
   </si>
   <si>
     <t>Translation-Adk</t>
@@ -3138,7 +3138,7 @@
     <t>[c]: (4) ALA + (11) ARG + (5) ASP + (1) ASN + (3) CYS + (3) GLN + (5) GLU + (5) GLY + (3) HIS + (2) ILE + (10) LEU + (3) LYS + (3) MET + (1) PHE + (7) PRO + (9) SER + (14) THR + (1) TRP + (2) TYR + (8) VAL + (203) GTP + (104) H2O ==&gt; Adk-Protein + (200) GDP + (200) PI + (200) H</t>
   </si>
   <si>
-    <t>Vmax * min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c]) / (Km + min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c])) * Adk-Rna[c] * Ribosome-Protein[c]</t>
+    <t>Vmax * min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c]) / (Km + min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c])) * Adk-Rna[c] * Ribosome-Protein[c]</t>
   </si>
   <si>
     <t>Translation-Apt</t>
@@ -3150,7 +3150,7 @@
     <t>[c]: (6) ALA + (13) ARG + (4) ASP + (4) ASN + (7) CYS + (1) GLN + (2) GLU + (4) GLY + (2) HIS + (4) ILE + (10) LEU + (1) LYS + (2) MET + (7) PHE + (2) PRO + (11) SER + (9) THR + (2) TRP + (4) TYR + (5) VAL + (203) GTP + (104) H2O ==&gt; Apt-Protein + (200) GDP + (200) PI + (200) H</t>
   </si>
   <si>
-    <t>Vmax * min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c]) / (Km + min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c])) * Apt-Rna[c] * Ribosome-Protein[c]</t>
+    <t>Vmax * min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c]) / (Km + min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c])) * Apt-Rna[c] * Ribosome-Protein[c]</t>
   </si>
   <si>
     <t>Translation-Cmk</t>
@@ -3162,7 +3162,7 @@
     <t>[c]: (5) ALA + (7) ARG + (3) ASP + (6) ASN + (7) CYS + (4) GLN + (3) GLU + (7) GLY + (3) HIS + (4) ILE + (12) LEU + (2) LYS + (2) MET + (1) PHE + (7) PRO + (7) SER + (7) THR + (4) TRP + (4) TYR + (5) VAL + (203) GTP + (104) H2O ==&gt; Cmk-Protein + (200) GDP + (200) PI + (200) H</t>
   </si>
   <si>
-    <t>Vmax * min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c]) / (Km + min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c])) * Cmk-Rna[c] * Ribosome-Protein[c]</t>
+    <t>Vmax * min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c]) / (Km + min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c])) * Cmk-Rna[c] * Ribosome-Protein[c]</t>
   </si>
   <si>
     <t>Translation-Eno</t>
@@ -3174,7 +3174,7 @@
     <t>[c]: (7) ALA + (8) ARG + (1) ASP + (5) ASN + (4) CYS + (5) GLN + (5) GLU + (4) GLY + (3) HIS + (5) ILE + (8) LEU + (4) LYS + (3) MET + (3) PHE + (8) PRO + (9) SER + (8) THR + (3) TRP + (4) TYR + (3) VAL + (203) GTP + (104) H2O ==&gt; Eno-Protein + (200) GDP + (200) PI + (200) H</t>
   </si>
   <si>
-    <t>Vmax * min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c]) / (Km + min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c])) * Eno-Rna[c] * Ribosome-Protein[c]</t>
+    <t>Vmax * min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c]) / (Km + min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c])) * Eno-Rna[c] * Ribosome-Protein[c]</t>
   </si>
   <si>
     <t>Translation-Fba</t>
@@ -3186,7 +3186,7 @@
     <t>[c]: (4) ALA + (13) ARG + (3) ASP + (1) ASN + (4) CYS + (5) GLN + (0) GLU + (6) GLY + (1) HIS + (4) ILE + (10) LEU + (2) LYS + (1) MET + (5) PHE + (9) PRO + (11) SER + (6) THR + (2) TRP + (2) TYR + (11) VAL + (203) GTP + (104) H2O ==&gt; Fba-Protein + (200) GDP + (200) PI + (200) H</t>
   </si>
   <si>
-    <t>Vmax * min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c]) / (Km + min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c])) * Fba-Rna[c] * Ribosome-Protein[c]</t>
+    <t>Vmax * min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c]) / (Km + min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c])) * Fba-Rna[c] * Ribosome-Protein[c]</t>
   </si>
   <si>
     <t>Translation-Gap</t>
@@ -3198,7 +3198,7 @@
     <t>[c]: (7) ALA + (9) ARG + (3) ASP + (1) ASN + (4) CYS + (5) GLN + (1) GLU + (6) GLY + (6) HIS + (6) ILE + (10) LEU + (2) LYS + (4) MET + (3) PHE + (4) PRO + (7) SER + (9) THR + (4) TRP + (4) TYR + (5) VAL + (203) GTP + (104) H2O ==&gt; Gap-Protein + (200) GDP + (200) PI + (200) H</t>
   </si>
   <si>
-    <t>Vmax * min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c]) / (Km + min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c])) * Gap-Rna[c] * Ribosome-Protein[c]</t>
+    <t>Vmax * min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c]) / (Km + min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c])) * Gap-Rna[c] * Ribosome-Protein[c]</t>
   </si>
   <si>
     <t>Translation-Pgm</t>
@@ -3210,7 +3210,7 @@
     <t>[c]: (6) ALA + (9) ARG + (2) ASP + (6) ASN + (1) CYS + (2) GLN + (4) GLU + (5) GLY + (4) HIS + (4) ILE + (9) LEU + (2) LYS + (2) MET + (6) PHE + (9) PRO + (10) SER + (6) THR + (2) TRP + (4) TYR + (7) VAL + (203) GTP + (104) H2O ==&gt; Pgm-Protein + (200) GDP + (200) PI + (200) H</t>
   </si>
   <si>
-    <t>Vmax * min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c]) / (Km + min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c])) * Pgm-Rna[c] * Ribosome-Protein[c]</t>
+    <t>Vmax * min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c]) / (Km + min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c])) * Pgm-Rna[c] * Ribosome-Protein[c]</t>
   </si>
   <si>
     <t>Translation-Gk</t>
@@ -3222,7 +3222,7 @@
     <t>[c]: (4) ALA + (2) ARG + (3) ASP + (3) ASN + (7) CYS + (5) GLN + (3) GLU + (8) GLY + (1) HIS + (3) ILE + (9) LEU + (3) LYS + (2) MET + (3) PHE + (11) PRO + (13) SER + (7) THR + (4) TRP + (1) TYR + (8) VAL + (203) GTP + (104) H2O ==&gt; Gk-Protein + (200) GDP + (200) PI + (200) H</t>
   </si>
   <si>
-    <t>Vmax * min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c]) / (Km + min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c])) * Gk-Rna[c] * Ribosome-Protein[c]</t>
+    <t>Vmax * min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c]) / (Km + min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c])) * Gk-Rna[c] * Ribosome-Protein[c]</t>
   </si>
   <si>
     <t>Translation-Hpt</t>
@@ -3234,7 +3234,7 @@
     <t>[c]: (11) ALA + (9) ARG + (3) ASP + (1) ASN + (3) CYS + (3) GLN + (6) GLU + (6) GLY + (2) HIS + (3) ILE + (8) LEU + (2) LYS + (7) MET + (3) PHE + (9) PRO + (9) SER + (3) THR + (2) TRP + (5) TYR + (5) VAL + (203) GTP + (104) H2O ==&gt; Hpt-Protein + (200) GDP + (200) PI + (200) H</t>
   </si>
   <si>
-    <t>Vmax * min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c]) / (Km + min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c])) * Hpt-Rna[c] * Ribosome-Protein[c]</t>
+    <t>Vmax * min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c]) / (Km + min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c])) * Hpt-Rna[c] * Ribosome-Protein[c]</t>
   </si>
   <si>
     <t>Translation-Ldh</t>
@@ -3246,7 +3246,7 @@
     <t>[c]: (3) ALA + (7) ARG + (5) ASP + (2) ASN + (2) CYS + (4) GLN + (4) GLU + (8) GLY + (1) HIS + (5) ILE + (11) LEU + (2) LYS + (3) MET + (2) PHE + (9) PRO + (8) SER + (8) THR + (3) TRP + (4) TYR + (9) VAL + (203) GTP + (104) H2O ==&gt; Ldh-Protein + (200) GDP + (200) PI + (200) H</t>
   </si>
   <si>
-    <t>Vmax * min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c]) / (Km + min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c])) * Ldh-Rna[c] * Ribosome-Protein[c]</t>
+    <t>Vmax * min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c]) / (Km + min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c])) * Ldh-Rna[c] * Ribosome-Protein[c]</t>
   </si>
   <si>
     <t>Translation-Nox</t>
@@ -3258,7 +3258,7 @@
     <t>[c]: (11) ALA + (7) ARG + (7) ASP + (1) ASN + (0) CYS + (2) GLN + (5) GLU + (8) GLY + (1) HIS + (7) ILE + (10) LEU + (1) LYS + (3) MET + (6) PHE + (4) PRO + (10) SER + (6) THR + (4) TRP + (3) TYR + (4) VAL + (203) GTP + (104) H2O ==&gt; Nox-Protein + (200) GDP + (200) PI + (200) H</t>
   </si>
   <si>
-    <t>Vmax * min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c]) / (Km + min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c])) * Nox-Rna[c] * Ribosome-Protein[c]</t>
+    <t>Vmax * min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c]) / (Km + min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c])) * Nox-Rna[c] * Ribosome-Protein[c]</t>
   </si>
   <si>
     <t>Translation-Pfk</t>
@@ -3270,7 +3270,7 @@
     <t>[c]: (4) ALA + (10) ARG + (4) ASP + (2) ASN + (2) CYS + (6) GLN + (2) GLU + (7) GLY + (2) HIS + (7) ILE + (9) LEU + (2) LYS + (1) MET + (5) PHE + (1) PRO + (16) SER + (7) THR + (4) TRP + (3) TYR + (6) VAL + (203) GTP + (104) H2O ==&gt; Pfk-Protein + (200) GDP + (200) PI + (200) H</t>
   </si>
   <si>
-    <t>Vmax * min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c]) / (Km + min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c])) * Pfk-Rna[c] * Ribosome-Protein[c]</t>
+    <t>Vmax * min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c]) / (Km + min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c])) * Pfk-Rna[c] * Ribosome-Protein[c]</t>
   </si>
   <si>
     <t>Translation-PgiB</t>
@@ -3282,7 +3282,7 @@
     <t>[c]: (10) ALA + (12) ARG + (3) ASP + (3) ASN + (2) CYS + (5) GLN + (3) GLU + (8) GLY + (3) HIS + (6) ILE + (6) LEU + (2) LYS + (2) MET + (2) PHE + (7) PRO + (9) SER + (7) THR + (2) TRP + (4) TYR + (4) VAL + (203) GTP + (104) H2O ==&gt; PgiB-Protein + (200) GDP + (200) PI + (200) H</t>
   </si>
   <si>
-    <t>Vmax * min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c]) / (Km + min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c])) * PgiB-Rna[c] * Ribosome-Protein[c]</t>
+    <t>Vmax * min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c]) / (Km + min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c])) * PgiB-Rna[c] * Ribosome-Protein[c]</t>
   </si>
   <si>
     <t>Translation-Pgk</t>
@@ -3294,7 +3294,7 @@
     <t>[c]: (6) ALA + (10) ARG + (3) ASP + (5) ASN + (3) CYS + (3) GLN + (0) GLU + (7) GLY + (4) HIS + (5) ILE + (9) LEU + (1) LYS + (1) MET + (3) PHE + (8) PRO + (13) SER + (8) THR + (2) TRP + (0) TYR + (9) VAL + (203) GTP + (104) H2O ==&gt; Pgk-Protein + (200) GDP + (200) PI + (200) H</t>
   </si>
   <si>
-    <t>Vmax * min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c]) / (Km + min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c])) * Pgk-Rna[c] * Ribosome-Protein[c]</t>
+    <t>Vmax * min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c]) / (Km + min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c])) * Pgk-Rna[c] * Ribosome-Protein[c]</t>
   </si>
   <si>
     <t>Translation-Ppa</t>
@@ -3306,7 +3306,7 @@
     <t>[c]: (4) ALA + (9) ARG + (2) ASP + (3) ASN + (1) CYS + (7) GLN + (3) GLU + (3) GLY + (2) HIS + (6) ILE + (9) LEU + (5) LYS + (3) MET + (4) PHE + (7) PRO + (15) SER + (6) THR + (5) TRP + (2) TYR + (4) VAL + (203) GTP + (104) H2O ==&gt; Ppa-Protein + (200) GDP + (200) PI + (200) H</t>
   </si>
   <si>
-    <t>Vmax * min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c]) / (Km + min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c])) * Ppa-Rna[c] * Ribosome-Protein[c]</t>
+    <t>Vmax * min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c]) / (Km + min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c])) * Ppa-Rna[c] * Ribosome-Protein[c]</t>
   </si>
   <si>
     <t>Translation-Prs</t>
@@ -3318,7 +3318,7 @@
     <t>[c]: (10) ALA + (11) ARG + (0) ASP + (5) ASN + (4) CYS + (3) GLN + (2) GLU + (5) GLY + (2) HIS + (7) ILE + (11) LEU + (2) LYS + (3) MET + (2) PHE + (8) PRO + (14) SER + (1) THR + (3) TRP + (2) TYR + (5) VAL + (203) GTP + (104) H2O ==&gt; Prs-Protein + (200) GDP + (200) PI + (200) H</t>
   </si>
   <si>
-    <t>Vmax * min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c]) / (Km + min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c])) * Prs-Rna[c] * Ribosome-Protein[c]</t>
+    <t>Vmax * min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c]) / (Km + min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c])) * Prs-Rna[c] * Ribosome-Protein[c]</t>
   </si>
   <si>
     <t>Translation-Pyk</t>
@@ -3330,7 +3330,7 @@
     <t>[c]: (9) ALA + (8) ARG + (2) ASP + (2) ASN + (2) CYS + (2) GLN + (2) GLU + (3) GLY + (2) HIS + (4) ILE + (9) LEU + (9) LYS + (3) MET + (4) PHE + (9) PRO + (6) SER + (9) THR + (0) TRP + (4) TYR + (11) VAL + (203) GTP + (104) H2O ==&gt; Pyk-Protein + (200) GDP + (200) PI + (200) H</t>
   </si>
   <si>
-    <t>Vmax * min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c]) / (Km + min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c])) * Pyk-Rna[c] * Ribosome-Protein[c]</t>
+    <t>Vmax * min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c]) / (Km + min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c])) * Pyk-Rna[c] * Ribosome-Protein[c]</t>
   </si>
   <si>
     <t>Translation-Rpe</t>
@@ -3342,7 +3342,7 @@
     <t>[c]: (5) ALA + (12) ARG + (5) ASP + (5) ASN + (1) CYS + (5) GLN + (2) GLU + (3) GLY + (2) HIS + (4) ILE + (8) LEU + (4) LYS + (3) MET + (1) PHE + (7) PRO + (9) SER + (13) THR + (5) TRP + (0) TYR + (6) VAL + (203) GTP + (104) H2O ==&gt; Rpe-Protein + (200) GDP + (200) PI + (200) H</t>
   </si>
   <si>
-    <t>Vmax * min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c]) / (Km + min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c])) * Rpe-Rna[c] * Ribosome-Protein[c]</t>
+    <t>Vmax * min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c]) / (Km + min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c])) * Rpe-Rna[c] * Ribosome-Protein[c]</t>
   </si>
   <si>
     <t>Translation-LacA</t>
@@ -3354,7 +3354,7 @@
     <t>[c]: (5) ALA + (4) ARG + (5) ASP + (6) ASN + (1) CYS + (2) GLN + (4) GLU + (9) GLY + (4) HIS + (8) ILE + (10) LEU + (3) LYS + (2) MET + (4) PHE + (5) PRO + (7) SER + (9) THR + (2) TRP + (1) TYR + (9) VAL + (203) GTP + (104) H2O ==&gt; LacA-Protein + (200) GDP + (200) PI + (200) H</t>
   </si>
   <si>
-    <t>Vmax * min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c]) / (Km + min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c])) * LacA-Rna[c] * Ribosome-Protein[c]</t>
+    <t>Vmax * min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c]) / (Km + min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c])) * LacA-Rna[c] * Ribosome-Protein[c]</t>
   </si>
   <si>
     <t>Translation-Tim</t>
@@ -3366,7 +3366,7 @@
     <t>[c]: (5) ALA + (11) ARG + (3) ASP + (1) ASN + (6) CYS + (5) GLN + (3) GLU + (6) GLY + (2) HIS + (6) ILE + (10) LEU + (0) LYS + (2) MET + (4) PHE + (3) PRO + (10) SER + (9) THR + (5) TRP + (1) TYR + (8) VAL + (203) GTP + (104) H2O ==&gt; Tim-Protein + (200) GDP + (200) PI + (200) H</t>
   </si>
   <si>
-    <t>Vmax * min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c]) / (Km + min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c])) * Tim-Rna[c] * Ribosome-Protein[c]</t>
+    <t>Vmax * min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c]) / (Km + min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c])) * Tim-Rna[c] * Ribosome-Protein[c]</t>
   </si>
   <si>
     <t>Translation-TklB</t>
@@ -3378,7 +3378,7 @@
     <t>[c]: (9) ALA + (9) ARG + (6) ASP + (4) ASN + (0) CYS + (1) GLN + (2) GLU + (7) GLY + (3) HIS + (3) ILE + (9) LEU + (4) LYS + (1) MET + (2) PHE + (8) PRO + (14) SER + (9) THR + (3) TRP + (2) TYR + (4) VAL + (203) GTP + (104) H2O ==&gt; TklB-Protein + (200) GDP + (200) PI + (200) H</t>
   </si>
   <si>
-    <t>Vmax * min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c]) / (Km + min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c])) * TklB-Rna[c] * Ribosome-Protein[c]</t>
+    <t>Vmax * min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c]) / (Km + min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c])) * TklB-Rna[c] * Ribosome-Protein[c]</t>
   </si>
   <si>
     <t>Translation-Udk</t>
@@ -3390,7 +3390,7 @@
     <t>[c]: (9) ALA + (5) ARG + (5) ASP + (2) ASN + (3) CYS + (5) GLN + (1) GLU + (10) GLY + (3) HIS + (8) ILE + (6) LEU + (6) LYS + (5) MET + (3) PHE + (3) PRO + (9) SER + (7) THR + (1) TRP + (3) TYR + (6) VAL + (203) GTP + (104) H2O ==&gt; Udk-Protein + (200) GDP + (200) PI + (200) H</t>
   </si>
   <si>
-    <t>Vmax * min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c]) / (Km + min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c])) * Udk-Rna[c] * Ribosome-Protein[c]</t>
+    <t>Vmax * min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c]) / (Km + min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c])) * Udk-Rna[c] * Ribosome-Protein[c]</t>
   </si>
   <si>
     <t>Translation-PyrH</t>
@@ -3402,7 +3402,7 @@
     <t>[c]: (5) ALA + (11) ARG + (3) ASP + (3) ASN + (2) CYS + (1) GLN + (3) GLU + (3) GLY + (2) HIS + (9) ILE + (10) LEU + (3) LYS + (2) MET + (3) PHE + (8) PRO + (14) SER + (9) THR + (1) TRP + (2) TYR + (6) VAL + (203) GTP + (104) H2O ==&gt; PyrH-Protein + (200) GDP + (200) PI + (200) H</t>
   </si>
   <si>
-    <t>Vmax * min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c]) / (Km + min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c])) * PyrH-Rna[c] * Ribosome-Protein[c]</t>
+    <t>Vmax * min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c]) / (Km + min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c])) * PyrH-Rna[c] * Ribosome-Protein[c]</t>
   </si>
   <si>
     <t>Translation-Upp</t>
@@ -3414,7 +3414,7 @@
     <t>[c]: (5) ALA + (8) ARG + (5) ASP + (3) ASN + (2) CYS + (2) GLN + (3) GLU + (5) GLY + (4) HIS + (4) ILE + (8) LEU + (5) LYS + (2) MET + (3) PHE + (12) PRO + (15) SER + (6) THR + (2) TRP + (3) TYR + (3) VAL + (203) GTP + (104) H2O ==&gt; Upp-Protein + (200) GDP + (200) PI + (200) H</t>
   </si>
   <si>
-    <t>Vmax * min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c]) / (Km + min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c])) * Upp-Rna[c] * Ribosome-Protein[c]</t>
+    <t>Vmax * min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c]) / (Km + min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c])) * Upp-Rna[c] * Ribosome-Protein[c]</t>
   </si>
   <si>
     <t>Translation-Pts</t>
@@ -3426,7 +3426,7 @@
     <t>[c]: (10) ALA + (8) ARG + (4) ASP + (4) ASN + (3) CYS + (5) GLN + (4) GLU + (6) GLY + (5) HIS + (4) ILE + (10) LEU + (1) LYS + (2) MET + (4) PHE + (5) PRO + (8) SER + (9) THR + (0) TRP + (3) TYR + (5) VAL + (203) GTP + (104) H2O ==&gt; Pts-Protein + (200) GDP + (200) PI + (200) H</t>
   </si>
   <si>
-    <t>Vmax * min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c]) / (Km + min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c])) * Pts-Rna[c] * Ribosome-Protein[c]</t>
+    <t>Vmax * min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c]) / (Km + min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c])) * Pts-Rna[c] * Ribosome-Protein[c]</t>
   </si>
   <si>
     <t>Translation-PiAbcTransporter</t>
@@ -3438,7 +3438,7 @@
     <t>[c]: (18) ALA + (8) ARG + (5) ASP + (1) ASN + (2) CYS + (3) GLN + (3) GLU + (4) GLY + (3) HIS + (6) ILE + (7) LEU + (3) LYS + (2) MET + (2) PHE + (4) PRO + (13) SER + (5) THR + (2) TRP + (4) TYR + (5) VAL + (203) GTP + (104) H2O ==&gt; PiAbcTransporter-Protein + (200) GDP + (200) PI + (200) H</t>
   </si>
   <si>
-    <t>Vmax * min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c]) / (Km + min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c])) * PiAbcTransporter-Rna[c] * Ribosome-Protein[c]</t>
+    <t>Vmax * min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c]) / (Km + min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c])) * PiAbcTransporter-Rna[c] * Ribosome-Protein[c]</t>
   </si>
   <si>
     <t>Translation-PeptAbcTransporter</t>
@@ -3450,7 +3450,7 @@
     <t>[c]: (3) ALA + (8) ARG + (0) ASP + (6) ASN + (1) CYS + (8) GLN + (3) GLU + (11) GLY + (3) HIS + (3) ILE + (10) LEU + (1) LYS + (1) MET + (5) PHE + (4) PRO + (10) SER + (4) THR + (3) TRP + (4) TYR + (12) VAL + (203) GTP + (104) H2O ==&gt; PeptAbcTransporter-Protein + (200) GDP + (200) PI + (200) H</t>
   </si>
   <si>
-    <t>Vmax * min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c]) / (Km + min(Ala[c], Arg[c], Asp[c], Asn[c], Cys[c], Gln[c], Glu[c], Gly[c], His[c], Ile[c], Leu[c], Lys[c], Met[c], Phe[c], Pro[c], Ser[c], Thr[c], Trp[c], Tyr[c], Val[c])) * PeptAbcTransporter-Rna[c] * Ribosome-Protein[c]</t>
+    <t>Vmax * min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c]) / (Km + min(ALA[c], ARG[c], ASP[c], ASN[c], CYS[c], GLN[c], GLU[c], GLY[c], HIS[c], ILE[c], LEU[c], LYS[c], MET[c], PHE[c], PRO[c], SER[c], THR[c], TRP[c], TYR[c], VAL[c])) * PeptAbcTransporter-Rna[c] * Ribosome-Protein[c]</t>
   </si>
   <si>
     <t>RnaDegradation-RnaPolymerase</t>
@@ -10125,7 +10125,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A81" activeCellId="0" sqref="A81"/>
-      <selection pane="bottomRight" activeCell="F92" activeCellId="0" sqref="F92"/>
+      <selection pane="bottomRight" activeCell="F85" activeCellId="0" sqref="F85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
reducing protein copy number
</commit_message>
<xml_diff>
--- a/data/Model.xlsx
+++ b/data/Model.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="570" windowWidth="19815" windowHeight="5835"/>
+    <workbookView xWindow="390" yWindow="570" windowWidth="19815" windowHeight="5835" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Submodels" sheetId="1" r:id="rId1"/>
@@ -3773,9 +3773,6 @@
     <t>Biomass production</t>
   </si>
   <si>
-    <t>[c]: (1.524425e+09) H2O + (1.101856e+06) ATP + (1.164906e+06) CTP + (7.209316e+06) GTP + (1.132896e+06) UTP + (2.177904e+05) ALA + (2.847904e+05) ARG + (1.187904e+05) ASP + (1.077904e+05) ASN + (9.879038e+04) CYS + (1.227904e+05) GLN + (1.027904e+05) GLU + (1.877904e+05) GLY + (9.179038e+04) HIS + (1.687904e+05) ILE + (2.877904e+05) LEU + (9.579038e+04) LYS + (8.979038e+04) MET + (1.147904e+05) PHE + (2.197904e+05) PRO + (3.207904e+05) SER + (2.377904e+05) THR + (9.779038e+04) TRP + (9.579038e+04) TYR + (2.137904e+05) VAL ==&gt; (1.000000e+00) Biomass + (1.045335e+07) H + (6.062419e+06) GDP + (1.035619e+06) AMP + (1.098019e+06) CMP + (1.052899e+06) GMP + (1.066339e+06) UMP + (4.381069e+06) PPI + (5.952096e+06) PI</t>
-  </si>
-  <si>
     <t>Value</t>
   </si>
   <si>
@@ -4029,6 +4026,9 @@
       </rPr>
       <t>+</t>
     </r>
+  </si>
+  <si>
+    <t>[c]: (1.521617e+09) H2O + (1.101856e+06) ATP + (1.164906e+06) CTP + (1.728316e+06) GTP + (1.132896e+06) UTP + (3.419038e+04) ALA + (4.089038e+04) ARG + (2.429038e+04) ASP + (2.319038e+04) ASN + (2.229038e+04) CYS + (2.469038e+04) GLN + (2.269038e+04) GLU + (3.119038e+04) GLY + (2.159038e+04) HIS + (2.929038e+04) ILE + (4.119038e+04) LEU + (2.199038e+04) LYS + (2.139038e+04) MET + (2.389038e+04) PHE + (3.439038e+04) PRO + (4.449038e+04) SER + (3.619038e+04) THR + (2.219038e+04) TRP + (2.199038e+04) TYR + (3.379038e+04) VAL ==&gt; (1.000000e+00) Biomass + (4.972350e+06) H + (5.814192e+05) GDP + (1.035619e+06) AMP + (1.098019e+06) CMP + (1.052899e+06) GMP + (1.066339e+06) UMP + (4.381069e+06) PPI + (4.710962e+05) PI</t>
   </si>
 </sst>
 </file>
@@ -4490,7 +4490,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -4642,10 +4642,10 @@
   <dimension ref="A1:O147"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B85" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" sqref="A1:XFD1"/>
+      <selection pane="bottomRight" activeCell="K97" sqref="K97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5075,7 +5075,7 @@
         <v>63</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>64</v>
@@ -6038,7 +6038,7 @@
         <v>159</v>
       </c>
       <c r="I35" s="4">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="J35" s="4"/>
       <c r="K35" s="4">
@@ -6062,7 +6062,7 @@
         <v>164</v>
       </c>
       <c r="E36" s="3">
-        <v>96734.607399999994</v>
+        <v>96734.607400000008</v>
       </c>
       <c r="F36" s="3">
         <v>-304</v>
@@ -6071,7 +6071,7 @@
         <v>159</v>
       </c>
       <c r="I36" s="4">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="J36" s="4"/>
       <c r="K36" s="4">
@@ -6095,7 +6095,7 @@
         <v>168</v>
       </c>
       <c r="E37" s="3">
-        <v>97136.857399999994</v>
+        <v>97136.857400000008</v>
       </c>
       <c r="F37" s="3">
         <v>-304</v>
@@ -6104,7 +6104,7 @@
         <v>159</v>
       </c>
       <c r="I37" s="4">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="J37" s="4"/>
       <c r="K37" s="4">
@@ -6122,7 +6122,7 @@
         <v>171</v>
       </c>
       <c r="E38" s="3">
-        <v>97629.509399999995</v>
+        <v>97629.50940000001</v>
       </c>
       <c r="F38" s="3">
         <v>-304</v>
@@ -6134,7 +6134,7 @@
         <v>172</v>
       </c>
       <c r="I38" s="4">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="J38" s="4"/>
       <c r="K38" s="4">
@@ -6170,7 +6170,7 @@
         <v>172</v>
       </c>
       <c r="I39" s="4">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="J39" s="4"/>
       <c r="K39" s="4">
@@ -6194,7 +6194,7 @@
         <v>178</v>
       </c>
       <c r="E40" s="3">
-        <v>97091.921400000007</v>
+        <v>97091.921399999992</v>
       </c>
       <c r="F40" s="3">
         <v>-304</v>
@@ -6206,7 +6206,7 @@
         <v>172</v>
       </c>
       <c r="I40" s="4">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="J40" s="4"/>
       <c r="K40" s="4">
@@ -6242,7 +6242,7 @@
         <v>172</v>
       </c>
       <c r="I41" s="4">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="J41" s="4"/>
       <c r="K41" s="4">
@@ -6278,7 +6278,7 @@
         <v>172</v>
       </c>
       <c r="I42" s="4">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="J42" s="4"/>
       <c r="K42" s="4">
@@ -6314,7 +6314,7 @@
         <v>172</v>
       </c>
       <c r="I43" s="4">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="J43" s="4"/>
       <c r="K43" s="4">
@@ -6350,7 +6350,7 @@
         <v>172</v>
       </c>
       <c r="I44" s="4">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="J44" s="4"/>
       <c r="K44" s="4">
@@ -6386,7 +6386,7 @@
         <v>172</v>
       </c>
       <c r="I45" s="4">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="J45" s="4"/>
       <c r="K45" s="4">
@@ -6410,7 +6410,7 @@
         <v>196</v>
       </c>
       <c r="E46" s="3">
-        <v>97473.0484</v>
+        <v>97473.048400000014</v>
       </c>
       <c r="F46" s="3">
         <v>-304</v>
@@ -6422,7 +6422,7 @@
         <v>172</v>
       </c>
       <c r="I46" s="4">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="J46" s="4"/>
       <c r="K46" s="4">
@@ -6458,7 +6458,7 @@
         <v>172</v>
       </c>
       <c r="I47" s="4">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="J47" s="4"/>
       <c r="K47" s="4">
@@ -6494,7 +6494,7 @@
         <v>172</v>
       </c>
       <c r="I48" s="4">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="J48" s="4"/>
       <c r="K48" s="4">
@@ -6518,7 +6518,7 @@
         <v>205</v>
       </c>
       <c r="E49" s="3">
-        <v>96846.414399999994</v>
+        <v>96846.414400000009</v>
       </c>
       <c r="F49" s="3">
         <v>-304</v>
@@ -6530,7 +6530,7 @@
         <v>172</v>
       </c>
       <c r="I49" s="4">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="J49" s="4"/>
       <c r="K49" s="4">
@@ -6566,7 +6566,7 @@
         <v>172</v>
       </c>
       <c r="I50" s="4">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="J50" s="4"/>
       <c r="K50" s="4">
@@ -6602,7 +6602,7 @@
         <v>172</v>
       </c>
       <c r="I51" s="4">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="J51" s="4"/>
       <c r="K51" s="4">
@@ -6638,7 +6638,7 @@
         <v>172</v>
       </c>
       <c r="I52" s="4">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="J52" s="4"/>
       <c r="K52" s="4">
@@ -6674,7 +6674,7 @@
         <v>172</v>
       </c>
       <c r="I53" s="4">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="J53" s="4"/>
       <c r="K53" s="4">
@@ -6710,7 +6710,7 @@
         <v>172</v>
       </c>
       <c r="I54" s="4">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="J54" s="4"/>
       <c r="K54" s="4">
@@ -6734,7 +6734,7 @@
         <v>223</v>
       </c>
       <c r="E55" s="3">
-        <v>97588.606400000004</v>
+        <v>97588.60639999999</v>
       </c>
       <c r="F55" s="3">
         <v>-304</v>
@@ -6746,7 +6746,7 @@
         <v>172</v>
       </c>
       <c r="I55" s="4">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="J55" s="4"/>
       <c r="K55" s="4">
@@ -6782,7 +6782,7 @@
         <v>172</v>
       </c>
       <c r="I56" s="4">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="J56" s="4"/>
       <c r="K56" s="4">
@@ -6818,7 +6818,7 @@
         <v>172</v>
       </c>
       <c r="I57" s="4">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="J57" s="4"/>
       <c r="K57" s="4">
@@ -6854,7 +6854,7 @@
         <v>172</v>
       </c>
       <c r="I58" s="4">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="J58" s="4"/>
       <c r="K58" s="4">
@@ -6878,7 +6878,7 @@
         <v>235</v>
       </c>
       <c r="E59" s="3">
-        <v>97302.183399999994</v>
+        <v>97302.183400000009</v>
       </c>
       <c r="F59" s="3">
         <v>-304</v>
@@ -6890,7 +6890,7 @@
         <v>172</v>
       </c>
       <c r="I59" s="4">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="J59" s="4"/>
       <c r="K59" s="4">
@@ -6926,7 +6926,7 @@
         <v>172</v>
       </c>
       <c r="I60" s="4">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="J60" s="4"/>
       <c r="K60" s="4">
@@ -6962,7 +6962,7 @@
         <v>172</v>
       </c>
       <c r="I61" s="4">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="J61" s="4"/>
       <c r="K61" s="4">
@@ -6998,7 +6998,7 @@
         <v>172</v>
       </c>
       <c r="I62" s="4">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="J62" s="4"/>
       <c r="K62" s="4">
@@ -7034,7 +7034,7 @@
         <v>172</v>
       </c>
       <c r="I63" s="4">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="J63" s="4"/>
       <c r="K63" s="4">
@@ -7070,7 +7070,7 @@
         <v>172</v>
       </c>
       <c r="I64" s="4">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="J64" s="4"/>
       <c r="K64" s="4">
@@ -7103,11 +7103,11 @@
         <v>256</v>
       </c>
       <c r="I65" s="4">
-        <v>3.62571589760398E-5</v>
+        <v>3.6257158976039822E-6</v>
       </c>
       <c r="J65" s="4"/>
       <c r="K65" s="4">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="M65" s="3" t="s">
         <v>257</v>
@@ -7136,11 +7136,11 @@
         <v>256</v>
       </c>
       <c r="I66" s="4">
-        <v>3.62571589760398E-5</v>
+        <v>3.6257158976039822E-6</v>
       </c>
       <c r="J66" s="4"/>
       <c r="K66" s="4">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="M66" s="3" t="s">
         <v>257</v>
@@ -7169,11 +7169,11 @@
         <v>256</v>
       </c>
       <c r="I67" s="4">
-        <v>3.62571589760398E-5</v>
+        <v>3.6257158976039822E-6</v>
       </c>
       <c r="J67" s="4"/>
       <c r="K67" s="4">
-        <v>1000</v>
+        <v>100</v>
       </c>
     </row>
     <row r="68" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7199,11 +7199,11 @@
         <v>172</v>
       </c>
       <c r="I68" s="4">
-        <v>3.62571589760398E-5</v>
+        <v>3.6257158976039822E-6</v>
       </c>
       <c r="J68" s="4"/>
       <c r="K68" s="4">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="M68" s="3" t="s">
         <v>257</v>
@@ -7235,11 +7235,11 @@
         <v>172</v>
       </c>
       <c r="I69" s="4">
-        <v>3.62571589760398E-5</v>
+        <v>3.6257158976039822E-6</v>
       </c>
       <c r="J69" s="4"/>
       <c r="K69" s="4">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="M69" s="3" t="s">
         <v>257</v>
@@ -7271,11 +7271,11 @@
         <v>172</v>
       </c>
       <c r="I70" s="4">
-        <v>3.62571589760398E-5</v>
+        <v>3.6257158976039822E-6</v>
       </c>
       <c r="J70" s="4"/>
       <c r="K70" s="4">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="M70" s="3" t="s">
         <v>257</v>
@@ -7307,11 +7307,11 @@
         <v>172</v>
       </c>
       <c r="I71" s="4">
-        <v>3.62571589760398E-5</v>
+        <v>3.6257158976039822E-6</v>
       </c>
       <c r="J71" s="4"/>
       <c r="K71" s="4">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="M71" s="3" t="s">
         <v>257</v>
@@ -7343,11 +7343,11 @@
         <v>172</v>
       </c>
       <c r="I72" s="4">
-        <v>3.62571589760398E-5</v>
+        <v>3.6257158976039822E-6</v>
       </c>
       <c r="J72" s="4"/>
       <c r="K72" s="4">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="M72" s="3" t="s">
         <v>257</v>
@@ -7379,11 +7379,11 @@
         <v>172</v>
       </c>
       <c r="I73" s="4">
-        <v>3.62571589760398E-5</v>
+        <v>3.6257158976039822E-6</v>
       </c>
       <c r="J73" s="4"/>
       <c r="K73" s="4">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="M73" s="3" t="s">
         <v>257</v>
@@ -7415,11 +7415,11 @@
         <v>172</v>
       </c>
       <c r="I74" s="4">
-        <v>3.62571589760398E-5</v>
+        <v>3.6257158976039822E-6</v>
       </c>
       <c r="J74" s="4"/>
       <c r="K74" s="4">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="M74" s="3" t="s">
         <v>257</v>
@@ -7451,11 +7451,11 @@
         <v>172</v>
       </c>
       <c r="I75" s="4">
-        <v>3.62571589760398E-5</v>
+        <v>3.6257158976039822E-6</v>
       </c>
       <c r="J75" s="4"/>
       <c r="K75" s="4">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="M75" s="3" t="s">
         <v>257</v>
@@ -7487,11 +7487,11 @@
         <v>172</v>
       </c>
       <c r="I76" s="4">
-        <v>3.62571589760398E-5</v>
+        <v>3.6257158976039822E-6</v>
       </c>
       <c r="J76" s="4"/>
       <c r="K76" s="4">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="M76" s="3" t="s">
         <v>257</v>
@@ -7523,11 +7523,11 @@
         <v>172</v>
       </c>
       <c r="I77" s="4">
-        <v>3.62571589760398E-5</v>
+        <v>3.6257158976039822E-6</v>
       </c>
       <c r="J77" s="4"/>
       <c r="K77" s="4">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="M77" s="3" t="s">
         <v>257</v>
@@ -7559,11 +7559,11 @@
         <v>172</v>
       </c>
       <c r="I78" s="4">
-        <v>3.62571589760398E-5</v>
+        <v>3.6257158976039822E-6</v>
       </c>
       <c r="J78" s="4"/>
       <c r="K78" s="4">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="M78" s="3" t="s">
         <v>257</v>
@@ -7595,11 +7595,11 @@
         <v>172</v>
       </c>
       <c r="I79" s="4">
-        <v>3.62571589760398E-5</v>
+        <v>3.6257158976039822E-6</v>
       </c>
       <c r="J79" s="4"/>
       <c r="K79" s="4">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="M79" s="3" t="s">
         <v>257</v>
@@ -7631,11 +7631,11 @@
         <v>172</v>
       </c>
       <c r="I80" s="4">
-        <v>3.62571589760398E-5</v>
+        <v>3.6257158976039822E-6</v>
       </c>
       <c r="J80" s="4"/>
       <c r="K80" s="4">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="M80" s="3" t="s">
         <v>257</v>
@@ -7667,11 +7667,11 @@
         <v>172</v>
       </c>
       <c r="I81" s="4">
-        <v>3.62571589760398E-5</v>
+        <v>3.6257158976039822E-6</v>
       </c>
       <c r="J81" s="4"/>
       <c r="K81" s="4">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="M81" s="3" t="s">
         <v>257</v>
@@ -7703,11 +7703,11 @@
         <v>172</v>
       </c>
       <c r="I82" s="4">
-        <v>3.62571589760398E-5</v>
+        <v>3.6257158976039822E-6</v>
       </c>
       <c r="J82" s="4"/>
       <c r="K82" s="4">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="M82" s="3" t="s">
         <v>257</v>
@@ -7739,11 +7739,11 @@
         <v>172</v>
       </c>
       <c r="I83" s="4">
-        <v>3.62571589760398E-5</v>
+        <v>3.6257158976039822E-6</v>
       </c>
       <c r="J83" s="4"/>
       <c r="K83" s="4">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="M83" s="3" t="s">
         <v>257</v>
@@ -7775,11 +7775,11 @@
         <v>172</v>
       </c>
       <c r="I84" s="4">
-        <v>3.62571589760398E-5</v>
+        <v>3.6257158976039822E-6</v>
       </c>
       <c r="J84" s="4"/>
       <c r="K84" s="4">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="M84" s="3" t="s">
         <v>257</v>
@@ -7811,11 +7811,11 @@
         <v>172</v>
       </c>
       <c r="I85" s="4">
-        <v>3.62571589760398E-5</v>
+        <v>3.6257158976039822E-6</v>
       </c>
       <c r="J85" s="4"/>
       <c r="K85" s="4">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="M85" s="3" t="s">
         <v>257</v>
@@ -7847,11 +7847,11 @@
         <v>172</v>
       </c>
       <c r="I86" s="4">
-        <v>3.62571589760398E-5</v>
+        <v>3.6257158976039822E-6</v>
       </c>
       <c r="J86" s="4"/>
       <c r="K86" s="4">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="M86" s="3" t="s">
         <v>257</v>
@@ -7883,11 +7883,11 @@
         <v>172</v>
       </c>
       <c r="I87" s="4">
-        <v>3.62571589760398E-5</v>
+        <v>3.6257158976039822E-6</v>
       </c>
       <c r="J87" s="4"/>
       <c r="K87" s="4">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="M87" s="3" t="s">
         <v>257</v>
@@ -7919,11 +7919,11 @@
         <v>172</v>
       </c>
       <c r="I88" s="4">
-        <v>3.62571589760398E-5</v>
+        <v>3.6257158976039822E-6</v>
       </c>
       <c r="J88" s="4"/>
       <c r="K88" s="4">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="M88" s="3" t="s">
         <v>257</v>
@@ -7955,11 +7955,11 @@
         <v>172</v>
       </c>
       <c r="I89" s="4">
-        <v>3.62571589760398E-5</v>
+        <v>3.6257158976039822E-6</v>
       </c>
       <c r="J89" s="4"/>
       <c r="K89" s="4">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="M89" s="3" t="s">
         <v>257</v>
@@ -7991,11 +7991,11 @@
         <v>172</v>
       </c>
       <c r="I90" s="4">
-        <v>3.62571589760398E-5</v>
+        <v>3.6257158976039822E-6</v>
       </c>
       <c r="J90" s="4"/>
       <c r="K90" s="4">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="M90" s="3" t="s">
         <v>257</v>
@@ -8027,11 +8027,11 @@
         <v>172</v>
       </c>
       <c r="I91" s="4">
-        <v>3.62571589760398E-5</v>
+        <v>3.6257158976039822E-6</v>
       </c>
       <c r="J91" s="4"/>
       <c r="K91" s="4">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="M91" s="3" t="s">
         <v>257</v>
@@ -8063,11 +8063,11 @@
         <v>172</v>
       </c>
       <c r="I92" s="4">
-        <v>3.62571589760398E-5</v>
+        <v>3.6257158976039822E-6</v>
       </c>
       <c r="J92" s="4"/>
       <c r="K92" s="4">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="M92" s="3" t="s">
         <v>257</v>
@@ -8099,11 +8099,11 @@
         <v>172</v>
       </c>
       <c r="I93" s="4">
-        <v>3.62571589760398E-5</v>
+        <v>3.6257158976039822E-6</v>
       </c>
       <c r="J93" s="4"/>
       <c r="K93" s="4">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="M93" s="3" t="s">
         <v>257</v>
@@ -8135,11 +8135,11 @@
         <v>172</v>
       </c>
       <c r="I94" s="4">
-        <v>3.62571589760398E-5</v>
+        <v>3.6257158976039822E-6</v>
       </c>
       <c r="J94" s="4"/>
       <c r="K94" s="4">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="M94" s="3" t="s">
         <v>257</v>
@@ -9983,11 +9983,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K177"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" sqref="A1:XFD1"/>
+      <selection pane="bottomRight" activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -10698,7 +10698,7 @@
         <v>689</v>
       </c>
       <c r="G30" s="7">
-        <v>2.76E-2</v>
+        <v>0.27600000000000002</v>
       </c>
       <c r="I30" s="3" t="s">
         <v>583</v>
@@ -12096,7 +12096,7 @@
         <v>913</v>
       </c>
       <c r="G87" s="7">
-        <v>2.3297446902153699E-4</v>
+        <v>2.3345582123025931E-4</v>
       </c>
       <c r="H87" s="7">
         <v>1E-3</v>
@@ -12131,7 +12131,7 @@
         <v>913</v>
       </c>
       <c r="G88" s="7">
-        <v>2.3297446902153699E-4</v>
+        <v>2.3345582123025931E-4</v>
       </c>
       <c r="H88" s="7">
         <v>1E-3</v>
@@ -12166,7 +12166,7 @@
         <v>913</v>
       </c>
       <c r="G89" s="7">
-        <v>2.3297446902153699E-4</v>
+        <v>2.3345582123025931E-4</v>
       </c>
       <c r="H89" s="7">
         <v>1E-3</v>
@@ -12201,7 +12201,7 @@
         <v>913</v>
       </c>
       <c r="G90" s="7">
-        <v>2.3297446902153699E-4</v>
+        <v>2.3345582123025931E-4</v>
       </c>
       <c r="H90" s="7">
         <v>1E-3</v>
@@ -12236,7 +12236,7 @@
         <v>913</v>
       </c>
       <c r="G91" s="7">
-        <v>2.3297446902153699E-4</v>
+        <v>2.3345582123025931E-4</v>
       </c>
       <c r="H91" s="7">
         <v>1E-3</v>
@@ -12271,7 +12271,7 @@
         <v>913</v>
       </c>
       <c r="G92" s="7">
-        <v>2.3297446902153699E-4</v>
+        <v>2.3345582123025931E-4</v>
       </c>
       <c r="H92" s="7">
         <v>1E-3</v>
@@ -12306,7 +12306,7 @@
         <v>913</v>
       </c>
       <c r="G93" s="7">
-        <v>2.3297446902153699E-4</v>
+        <v>2.3345582123025931E-4</v>
       </c>
       <c r="H93" s="7">
         <v>1E-3</v>
@@ -12341,7 +12341,7 @@
         <v>913</v>
       </c>
       <c r="G94" s="7">
-        <v>2.3297446902153699E-4</v>
+        <v>2.3345582123025931E-4</v>
       </c>
       <c r="H94" s="7">
         <v>1E-3</v>
@@ -12376,7 +12376,7 @@
         <v>913</v>
       </c>
       <c r="G95" s="7">
-        <v>2.3297446902153699E-4</v>
+        <v>2.3345582123025931E-4</v>
       </c>
       <c r="H95" s="7">
         <v>1E-3</v>
@@ -12411,7 +12411,7 @@
         <v>913</v>
       </c>
       <c r="G96" s="7">
-        <v>2.3297446902153699E-4</v>
+        <v>2.3345582123025931E-4</v>
       </c>
       <c r="H96" s="7">
         <v>1E-3</v>
@@ -12446,7 +12446,7 @@
         <v>913</v>
       </c>
       <c r="G97" s="7">
-        <v>2.3297446902153699E-4</v>
+        <v>2.3345582123025931E-4</v>
       </c>
       <c r="H97" s="7">
         <v>1E-3</v>
@@ -12481,7 +12481,7 @@
         <v>913</v>
       </c>
       <c r="G98" s="7">
-        <v>2.3297446902153699E-4</v>
+        <v>2.3345582123025931E-4</v>
       </c>
       <c r="H98" s="7">
         <v>1E-3</v>
@@ -12516,7 +12516,7 @@
         <v>913</v>
       </c>
       <c r="G99" s="7">
-        <v>2.3297446902153699E-4</v>
+        <v>2.3345582123025931E-4</v>
       </c>
       <c r="H99" s="7">
         <v>1E-3</v>
@@ -12551,7 +12551,7 @@
         <v>913</v>
       </c>
       <c r="G100" s="7">
-        <v>2.3297446902153699E-4</v>
+        <v>2.3345582123025931E-4</v>
       </c>
       <c r="H100" s="7">
         <v>1E-3</v>
@@ -12586,7 +12586,7 @@
         <v>913</v>
       </c>
       <c r="G101" s="7">
-        <v>2.3297446902153699E-4</v>
+        <v>2.3345582123025931E-4</v>
       </c>
       <c r="H101" s="7">
         <v>1E-3</v>
@@ -12621,7 +12621,7 @@
         <v>913</v>
       </c>
       <c r="G102" s="7">
-        <v>2.3297446902153699E-4</v>
+        <v>2.3345582123025931E-4</v>
       </c>
       <c r="H102" s="7">
         <v>1E-3</v>
@@ -12656,7 +12656,7 @@
         <v>913</v>
       </c>
       <c r="G103" s="7">
-        <v>2.3297446902153699E-4</v>
+        <v>2.3345582123025931E-4</v>
       </c>
       <c r="H103" s="7">
         <v>1E-3</v>
@@ -12691,7 +12691,7 @@
         <v>913</v>
       </c>
       <c r="G104" s="7">
-        <v>2.3297446902153699E-4</v>
+        <v>2.3345582123025931E-4</v>
       </c>
       <c r="H104" s="7">
         <v>1E-3</v>
@@ -12726,7 +12726,7 @@
         <v>913</v>
       </c>
       <c r="G105" s="7">
-        <v>2.3297446902153699E-4</v>
+        <v>2.3345582123025931E-4</v>
       </c>
       <c r="H105" s="7">
         <v>1E-3</v>
@@ -12761,7 +12761,7 @@
         <v>913</v>
       </c>
       <c r="G106" s="7">
-        <v>2.3297446902153699E-4</v>
+        <v>2.3345582123025931E-4</v>
       </c>
       <c r="H106" s="7">
         <v>1E-3</v>
@@ -12796,7 +12796,7 @@
         <v>913</v>
       </c>
       <c r="G107" s="7">
-        <v>2.3297446902153699E-4</v>
+        <v>2.3345582123025931E-4</v>
       </c>
       <c r="H107" s="7">
         <v>1E-3</v>
@@ -12831,7 +12831,7 @@
         <v>913</v>
       </c>
       <c r="G108" s="7">
-        <v>2.3297446902153699E-4</v>
+        <v>2.3345582123025931E-4</v>
       </c>
       <c r="H108" s="7">
         <v>1E-3</v>
@@ -12866,7 +12866,7 @@
         <v>913</v>
       </c>
       <c r="G109" s="7">
-        <v>2.3297446902153699E-4</v>
+        <v>2.3345582123025931E-4</v>
       </c>
       <c r="H109" s="7">
         <v>1E-3</v>
@@ -12901,7 +12901,7 @@
         <v>913</v>
       </c>
       <c r="G110" s="7">
-        <v>2.3297446902153699E-4</v>
+        <v>2.3345582123025931E-4</v>
       </c>
       <c r="H110" s="7">
         <v>1E-3</v>
@@ -12936,7 +12936,7 @@
         <v>913</v>
       </c>
       <c r="G111" s="7">
-        <v>2.3297446902153699E-4</v>
+        <v>2.3345582123025931E-4</v>
       </c>
       <c r="H111" s="7">
         <v>1E-3</v>
@@ -12971,7 +12971,7 @@
         <v>913</v>
       </c>
       <c r="G112" s="7">
-        <v>2.3297446902153699E-4</v>
+        <v>2.3345582123025931E-4</v>
       </c>
       <c r="H112" s="7">
         <v>1E-3</v>
@@ -13006,7 +13006,7 @@
         <v>913</v>
       </c>
       <c r="G113" s="7">
-        <v>2.3297446902153699E-4</v>
+        <v>2.3345582123025931E-4</v>
       </c>
       <c r="H113" s="7">
         <v>1E-3</v>
@@ -13041,7 +13041,7 @@
         <v>913</v>
       </c>
       <c r="G114" s="7">
-        <v>2.3297446902153699E-4</v>
+        <v>2.3345582123025931E-4</v>
       </c>
       <c r="H114" s="7">
         <v>1E-3</v>
@@ -13076,7 +13076,7 @@
         <v>913</v>
       </c>
       <c r="G115" s="7">
-        <v>2.3297446902153699E-4</v>
+        <v>2.3345582123025931E-4</v>
       </c>
       <c r="H115" s="7">
         <v>1E-3</v>
@@ -13111,7 +13111,7 @@
         <v>913</v>
       </c>
       <c r="G116" s="7">
-        <v>2.3297446902153699E-4</v>
+        <v>2.3345582123025931E-4</v>
       </c>
       <c r="H116" s="7">
         <v>1E-3</v>
@@ -13146,7 +13146,7 @@
         <v>1006</v>
       </c>
       <c r="G117" s="7">
-        <v>7.7016353395549494E-6</v>
+        <v>9.6270441744436842E-6</v>
       </c>
       <c r="H117" s="7">
         <v>5.0000000000000001E-4</v>
@@ -13181,7 +13181,7 @@
         <v>1011</v>
       </c>
       <c r="G118" s="7">
-        <v>7.7016353395549494E-6</v>
+        <v>9.6270441744436842E-6</v>
       </c>
       <c r="H118" s="7">
         <v>5.0000000000000001E-4</v>
@@ -13216,7 +13216,7 @@
         <v>1015</v>
       </c>
       <c r="G119" s="7">
-        <v>7.7016353395549494E-6</v>
+        <v>9.6270441744436842E-6</v>
       </c>
       <c r="H119" s="7">
         <v>5.0000000000000001E-4</v>
@@ -13251,7 +13251,7 @@
         <v>1019</v>
       </c>
       <c r="G120" s="7">
-        <v>7.7016353395549494E-6</v>
+        <v>9.6270441744436842E-6</v>
       </c>
       <c r="H120" s="7">
         <v>5.0000000000000001E-4</v>
@@ -13286,7 +13286,7 @@
         <v>1023</v>
       </c>
       <c r="G121" s="7">
-        <v>7.7016353395549494E-6</v>
+        <v>9.6270441744436842E-6</v>
       </c>
       <c r="H121" s="7">
         <v>5.0000000000000001E-4</v>
@@ -13321,7 +13321,7 @@
         <v>1027</v>
       </c>
       <c r="G122" s="7">
-        <v>7.7016353395549494E-6</v>
+        <v>9.6270441744436842E-6</v>
       </c>
       <c r="H122" s="7">
         <v>5.0000000000000001E-4</v>
@@ -13356,7 +13356,7 @@
         <v>1031</v>
       </c>
       <c r="G123" s="7">
-        <v>7.7016353395549494E-6</v>
+        <v>9.6270441744436842E-6</v>
       </c>
       <c r="H123" s="7">
         <v>5.0000000000000001E-4</v>
@@ -13391,7 +13391,7 @@
         <v>1035</v>
       </c>
       <c r="G124" s="7">
-        <v>7.7016353395549494E-6</v>
+        <v>9.6270441744436842E-6</v>
       </c>
       <c r="H124" s="7">
         <v>5.0000000000000001E-4</v>
@@ -13426,7 +13426,7 @@
         <v>1039</v>
       </c>
       <c r="G125" s="7">
-        <v>7.7016353395549494E-6</v>
+        <v>9.6270441744436842E-6</v>
       </c>
       <c r="H125" s="7">
         <v>5.0000000000000001E-4</v>
@@ -13461,7 +13461,7 @@
         <v>1043</v>
       </c>
       <c r="G126" s="7">
-        <v>7.7016353395549494E-6</v>
+        <v>9.6270441744436842E-6</v>
       </c>
       <c r="H126" s="7">
         <v>5.0000000000000001E-4</v>
@@ -13496,7 +13496,7 @@
         <v>1047</v>
       </c>
       <c r="G127" s="7">
-        <v>7.7016353395549494E-6</v>
+        <v>9.6270441744436842E-6</v>
       </c>
       <c r="H127" s="7">
         <v>5.0000000000000001E-4</v>
@@ -13531,7 +13531,7 @@
         <v>1051</v>
       </c>
       <c r="G128" s="7">
-        <v>7.7016353395549494E-6</v>
+        <v>9.6270441744436842E-6</v>
       </c>
       <c r="H128" s="7">
         <v>5.0000000000000001E-4</v>
@@ -13566,7 +13566,7 @@
         <v>1055</v>
       </c>
       <c r="G129" s="7">
-        <v>7.7016353395549494E-6</v>
+        <v>9.6270441744436842E-6</v>
       </c>
       <c r="H129" s="7">
         <v>5.0000000000000001E-4</v>
@@ -13601,7 +13601,7 @@
         <v>1059</v>
       </c>
       <c r="G130" s="7">
-        <v>7.7016353395549494E-6</v>
+        <v>9.6270441744436842E-6</v>
       </c>
       <c r="H130" s="7">
         <v>5.0000000000000001E-4</v>
@@ -13636,7 +13636,7 @@
         <v>1063</v>
       </c>
       <c r="G131" s="7">
-        <v>7.7016353395549494E-6</v>
+        <v>9.6270441744436842E-6</v>
       </c>
       <c r="H131" s="7">
         <v>5.0000000000000001E-4</v>
@@ -13671,7 +13671,7 @@
         <v>1067</v>
       </c>
       <c r="G132" s="7">
-        <v>7.7016353395549494E-6</v>
+        <v>9.6270441744436842E-6</v>
       </c>
       <c r="H132" s="7">
         <v>5.0000000000000001E-4</v>
@@ -13706,7 +13706,7 @@
         <v>1071</v>
       </c>
       <c r="G133" s="7">
-        <v>7.7016353395549494E-6</v>
+        <v>9.6270441744436842E-6</v>
       </c>
       <c r="H133" s="7">
         <v>5.0000000000000001E-4</v>
@@ -13741,7 +13741,7 @@
         <v>1075</v>
       </c>
       <c r="G134" s="7">
-        <v>7.7016353395549494E-6</v>
+        <v>9.6270441744436842E-6</v>
       </c>
       <c r="H134" s="7">
         <v>5.0000000000000001E-4</v>
@@ -13776,7 +13776,7 @@
         <v>1079</v>
       </c>
       <c r="G135" s="7">
-        <v>7.7016353395549494E-6</v>
+        <v>9.6270441744436842E-6</v>
       </c>
       <c r="H135" s="7">
         <v>5.0000000000000001E-4</v>
@@ -13811,7 +13811,7 @@
         <v>1083</v>
       </c>
       <c r="G136" s="7">
-        <v>7.7016353395549494E-6</v>
+        <v>9.6270441744436842E-6</v>
       </c>
       <c r="H136" s="7">
         <v>5.0000000000000001E-4</v>
@@ -13846,7 +13846,7 @@
         <v>1087</v>
       </c>
       <c r="G137" s="7">
-        <v>7.7016353395549494E-6</v>
+        <v>9.6270441744436842E-6</v>
       </c>
       <c r="H137" s="7">
         <v>5.0000000000000001E-4</v>
@@ -13881,7 +13881,7 @@
         <v>1091</v>
       </c>
       <c r="G138" s="7">
-        <v>7.7016353395549494E-6</v>
+        <v>9.6270441744436842E-6</v>
       </c>
       <c r="H138" s="7">
         <v>5.0000000000000001E-4</v>
@@ -13916,7 +13916,7 @@
         <v>1095</v>
       </c>
       <c r="G139" s="7">
-        <v>7.7016353395549494E-6</v>
+        <v>9.6270441744436842E-6</v>
       </c>
       <c r="H139" s="7">
         <v>5.0000000000000001E-4</v>
@@ -13951,7 +13951,7 @@
         <v>1099</v>
       </c>
       <c r="G140" s="7">
-        <v>7.7016353395549494E-6</v>
+        <v>9.6270441744436842E-6</v>
       </c>
       <c r="H140" s="7">
         <v>5.0000000000000001E-4</v>
@@ -13986,7 +13986,7 @@
         <v>1103</v>
       </c>
       <c r="G141" s="7">
-        <v>7.7016353395549494E-6</v>
+        <v>9.6270441744436842E-6</v>
       </c>
       <c r="H141" s="7">
         <v>5.0000000000000001E-4</v>
@@ -14021,7 +14021,7 @@
         <v>1107</v>
       </c>
       <c r="G142" s="7">
-        <v>7.7016353395549494E-6</v>
+        <v>9.6270441744436842E-6</v>
       </c>
       <c r="H142" s="7">
         <v>5.0000000000000001E-4</v>
@@ -14056,7 +14056,7 @@
         <v>1111</v>
       </c>
       <c r="G143" s="7">
-        <v>7.7016353395549494E-6</v>
+        <v>9.6270441744436842E-6</v>
       </c>
       <c r="H143" s="7">
         <v>5.0000000000000001E-4</v>
@@ -14091,7 +14091,7 @@
         <v>1115</v>
       </c>
       <c r="G144" s="7">
-        <v>7.7016353395549494E-6</v>
+        <v>9.6270441744436842E-6</v>
       </c>
       <c r="H144" s="7">
         <v>5.0000000000000001E-4</v>
@@ -14126,7 +14126,7 @@
         <v>1119</v>
       </c>
       <c r="G145" s="7">
-        <v>7.7016353395549494E-6</v>
+        <v>9.6270441744436842E-6</v>
       </c>
       <c r="H145" s="7">
         <v>5.0000000000000001E-4</v>
@@ -14161,7 +14161,7 @@
         <v>1123</v>
       </c>
       <c r="G146" s="7">
-        <v>7.7016353395549494E-6</v>
+        <v>9.6270441744436842E-6</v>
       </c>
       <c r="H146" s="7">
         <v>5.0000000000000001E-4</v>
@@ -14196,10 +14196,10 @@
         <v>1127</v>
       </c>
       <c r="G147" s="7">
-        <v>2.31049060186648E-4</v>
+        <v>2.3104906018664841E-4</v>
       </c>
       <c r="H147" s="7">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="I147" s="3" t="s">
         <v>583</v>
@@ -14231,10 +14231,10 @@
         <v>1133</v>
       </c>
       <c r="G148" s="7">
-        <v>2.31049060186648E-4</v>
+        <v>2.3104906018664841E-4</v>
       </c>
       <c r="H148" s="7">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="I148" s="3" t="s">
         <v>583</v>
@@ -14266,10 +14266,10 @@
         <v>1137</v>
       </c>
       <c r="G149" s="7">
-        <v>2.31049060186648E-4</v>
+        <v>2.3104906018664841E-4</v>
       </c>
       <c r="H149" s="7">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="I149" s="3" t="s">
         <v>583</v>
@@ -14301,10 +14301,10 @@
         <v>1141</v>
       </c>
       <c r="G150" s="7">
-        <v>2.31049060186648E-4</v>
+        <v>2.3104906018664841E-4</v>
       </c>
       <c r="H150" s="7">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="I150" s="3" t="s">
         <v>583</v>
@@ -14336,10 +14336,10 @@
         <v>1145</v>
       </c>
       <c r="G151" s="7">
-        <v>2.31049060186648E-4</v>
+        <v>2.3104906018664841E-4</v>
       </c>
       <c r="H151" s="7">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="I151" s="3" t="s">
         <v>583</v>
@@ -14371,10 +14371,10 @@
         <v>1149</v>
       </c>
       <c r="G152" s="7">
-        <v>2.31049060186648E-4</v>
+        <v>2.3104906018664841E-4</v>
       </c>
       <c r="H152" s="7">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="I152" s="3" t="s">
         <v>583</v>
@@ -14406,10 +14406,10 @@
         <v>1153</v>
       </c>
       <c r="G153" s="7">
-        <v>2.31049060186648E-4</v>
+        <v>2.3104906018664841E-4</v>
       </c>
       <c r="H153" s="7">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="I153" s="3" t="s">
         <v>583</v>
@@ -14441,10 +14441,10 @@
         <v>1157</v>
       </c>
       <c r="G154" s="7">
-        <v>2.31049060186648E-4</v>
+        <v>2.3104906018664841E-4</v>
       </c>
       <c r="H154" s="7">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="I154" s="3" t="s">
         <v>583</v>
@@ -14476,10 +14476,10 @@
         <v>1161</v>
       </c>
       <c r="G155" s="7">
-        <v>2.31049060186648E-4</v>
+        <v>2.3104906018664841E-4</v>
       </c>
       <c r="H155" s="7">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="I155" s="3" t="s">
         <v>583</v>
@@ -14511,10 +14511,10 @@
         <v>1165</v>
       </c>
       <c r="G156" s="7">
-        <v>2.31049060186648E-4</v>
+        <v>2.3104906018664841E-4</v>
       </c>
       <c r="H156" s="7">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="I156" s="3" t="s">
         <v>583</v>
@@ -14546,10 +14546,10 @@
         <v>1169</v>
       </c>
       <c r="G157" s="7">
-        <v>2.31049060186648E-4</v>
+        <v>2.3104906018664841E-4</v>
       </c>
       <c r="H157" s="7">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="I157" s="3" t="s">
         <v>583</v>
@@ -14581,10 +14581,10 @@
         <v>1173</v>
       </c>
       <c r="G158" s="7">
-        <v>2.31049060186648E-4</v>
+        <v>2.3104906018664841E-4</v>
       </c>
       <c r="H158" s="7">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="I158" s="3" t="s">
         <v>583</v>
@@ -14616,10 +14616,10 @@
         <v>1177</v>
       </c>
       <c r="G159" s="7">
-        <v>2.31049060186648E-4</v>
+        <v>2.3104906018664841E-4</v>
       </c>
       <c r="H159" s="7">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="I159" s="3" t="s">
         <v>583</v>
@@ -14651,10 +14651,10 @@
         <v>1181</v>
       </c>
       <c r="G160" s="7">
-        <v>2.31049060186648E-4</v>
+        <v>2.3104906018664841E-4</v>
       </c>
       <c r="H160" s="7">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="I160" s="3" t="s">
         <v>583</v>
@@ -14686,10 +14686,10 @@
         <v>1185</v>
       </c>
       <c r="G161" s="7">
-        <v>2.31049060186648E-4</v>
+        <v>2.3104906018664841E-4</v>
       </c>
       <c r="H161" s="7">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="I161" s="3" t="s">
         <v>583</v>
@@ -14721,10 +14721,10 @@
         <v>1189</v>
       </c>
       <c r="G162" s="7">
-        <v>2.31049060186648E-4</v>
+        <v>2.3104906018664841E-4</v>
       </c>
       <c r="H162" s="7">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="I162" s="3" t="s">
         <v>583</v>
@@ -14756,10 +14756,10 @@
         <v>1193</v>
       </c>
       <c r="G163" s="7">
-        <v>2.31049060186648E-4</v>
+        <v>2.3104906018664841E-4</v>
       </c>
       <c r="H163" s="7">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="I163" s="3" t="s">
         <v>583</v>
@@ -14791,10 +14791,10 @@
         <v>1197</v>
       </c>
       <c r="G164" s="7">
-        <v>2.31049060186648E-4</v>
+        <v>2.3104906018664841E-4</v>
       </c>
       <c r="H164" s="7">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="I164" s="3" t="s">
         <v>583</v>
@@ -14826,10 +14826,10 @@
         <v>1201</v>
       </c>
       <c r="G165" s="7">
-        <v>2.31049060186648E-4</v>
+        <v>2.3104906018664841E-4</v>
       </c>
       <c r="H165" s="7">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="I165" s="3" t="s">
         <v>583</v>
@@ -14861,10 +14861,10 @@
         <v>1205</v>
       </c>
       <c r="G166" s="7">
-        <v>2.31049060186648E-4</v>
+        <v>2.3104906018664841E-4</v>
       </c>
       <c r="H166" s="7">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="I166" s="3" t="s">
         <v>583</v>
@@ -14896,10 +14896,10 @@
         <v>1209</v>
       </c>
       <c r="G167" s="7">
-        <v>2.31049060186648E-4</v>
+        <v>2.3104906018664841E-4</v>
       </c>
       <c r="H167" s="7">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="I167" s="3" t="s">
         <v>583</v>
@@ -14931,10 +14931,10 @@
         <v>1213</v>
       </c>
       <c r="G168" s="7">
-        <v>2.31049060186648E-4</v>
+        <v>2.3104906018664841E-4</v>
       </c>
       <c r="H168" s="7">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="I168" s="3" t="s">
         <v>583</v>
@@ -14966,10 +14966,10 @@
         <v>1217</v>
       </c>
       <c r="G169" s="7">
-        <v>2.31049060186648E-4</v>
+        <v>2.3104906018664841E-4</v>
       </c>
       <c r="H169" s="7">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="I169" s="3" t="s">
         <v>583</v>
@@ -15001,10 +15001,10 @@
         <v>1221</v>
       </c>
       <c r="G170" s="7">
-        <v>2.31049060186648E-4</v>
+        <v>2.3104906018664841E-4</v>
       </c>
       <c r="H170" s="7">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="I170" s="3" t="s">
         <v>583</v>
@@ -15036,10 +15036,10 @@
         <v>1225</v>
       </c>
       <c r="G171" s="7">
-        <v>2.31049060186648E-4</v>
+        <v>2.3104906018664841E-4</v>
       </c>
       <c r="H171" s="7">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="I171" s="3" t="s">
         <v>583</v>
@@ -15071,10 +15071,10 @@
         <v>1229</v>
       </c>
       <c r="G172" s="7">
-        <v>2.31049060186648E-4</v>
+        <v>2.3104906018664841E-4</v>
       </c>
       <c r="H172" s="7">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="I172" s="3" t="s">
         <v>583</v>
@@ -15106,10 +15106,10 @@
         <v>1233</v>
       </c>
       <c r="G173" s="7">
-        <v>2.31049060186648E-4</v>
+        <v>2.3104906018664841E-4</v>
       </c>
       <c r="H173" s="7">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="I173" s="3" t="s">
         <v>583</v>
@@ -15141,10 +15141,10 @@
         <v>1237</v>
       </c>
       <c r="G174" s="7">
-        <v>2.31049060186648E-4</v>
+        <v>2.3104906018664841E-4</v>
       </c>
       <c r="H174" s="7">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="I174" s="3" t="s">
         <v>583</v>
@@ -15176,10 +15176,10 @@
         <v>1241</v>
       </c>
       <c r="G175" s="7">
-        <v>2.31049060186648E-4</v>
+        <v>2.3104906018664841E-4</v>
       </c>
       <c r="H175" s="7">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="I175" s="3" t="s">
         <v>583</v>
@@ -15211,10 +15211,10 @@
         <v>1245</v>
       </c>
       <c r="G176" s="7">
-        <v>2.31049060186648E-4</v>
+        <v>2.3104906018664841E-4</v>
       </c>
       <c r="H176" s="7">
-        <v>1.8128579488019899E-7</v>
+        <v>1.812857948801991E-7</v>
       </c>
       <c r="I176" s="3" t="s">
         <v>583</v>
@@ -15237,7 +15237,7 @@
         <v>3</v>
       </c>
       <c r="D177" s="3" t="s">
-        <v>1248</v>
+        <v>1327</v>
       </c>
     </row>
   </sheetData>
@@ -15280,10 +15280,10 @@
         <v>573</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>1248</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>1249</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>1250</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>11</v>
@@ -15291,38 +15291,38 @@
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>1250</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>1251</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>1252</v>
       </c>
       <c r="D2" s="3">
         <v>28800</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>1253</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>1254</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>1255</v>
       </c>
       <c r="D3" s="3">
         <v>300</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>1256</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>1257</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>3</v>
@@ -15331,18 +15331,18 @@
         <v>12</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>1257</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>1258</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>1259</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>1259</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>1260</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>1261</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>3</v>
@@ -15351,27 +15351,27 @@
         <v>20</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>1262</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>1263</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>1264</v>
       </c>
       <c r="D6" s="3">
         <v>0.3</v>
       </c>
       <c r="E6" s="3" t="s">
+        <v>1264</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>1265</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>1266</v>
       </c>
     </row>
   </sheetData>
@@ -15419,86 +15419,86 @@
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>1266</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>1267</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>1268</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>1269</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>1270</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>1270</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>1271</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
+        <v>1268</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>1272</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>1269</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>1273</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>1273</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>1274</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
+        <v>1268</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>1275</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>1269</v>
-      </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>1276</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>1277</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>1277</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>1278</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
+        <v>1268</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>1279</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>1269</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>1280</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>1280</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>1281</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="3" t="s">
+        <v>1268</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>1282</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>1269</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>1283</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>1283</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>1284</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>1285</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>1286</v>
       </c>
       <c r="D7" s="3">
         <v>815332823</v>
@@ -15506,83 +15506,83 @@
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>1286</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>1287</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="C8" s="3" t="s">
+        <v>1268</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>1288</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>1269</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>1289</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
+        <v>1289</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>1290</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="3" t="s">
+        <v>1268</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>1291</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>1269</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>1292</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>1293</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C10" s="3" t="s">
+        <v>1268</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>1294</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>1269</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>1295</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
+        <v>1295</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>1296</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="C11" s="3" t="s">
+        <v>1268</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>1297</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>1269</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>1298</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>1299</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="C12" s="3" t="s">
+        <v>1268</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>1300</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>1269</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>1301</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
+        <v>1301</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>1302</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>1303</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>1304</v>
       </c>
       <c r="D13" s="3">
         <v>33184</v>
@@ -15590,100 +15590,100 @@
     </row>
     <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>1317</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>1268</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>1318</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>1269</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>1319</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="C16" s="3" t="s">
+        <v>1311</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>1312</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>1313</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
+        <v>1310</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>1323</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>1311</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>1324</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>1312</v>
-      </c>
       <c r="D20" s="3" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
     </row>
   </sheetData>

</xml_diff>